<commit_message>
add Crous 2017 to meta analysis sheet
</commit_message>
<xml_diff>
--- a/lit_search_np_fert_exps.xlsx
+++ b/lit_search_np_fert_exps.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eaperkowski/git/p_meta/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E1A2823-23C5-A140-964F-08F53865BF34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E318BB6-92B6-D947-BBB5-CDA4FB54BDCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2040" yWindow="3480" windowWidth="49580" windowHeight="28300" xr2:uid="{50492CE8-F5C0-524A-968F-FD9EC2022F6C}"/>
+    <workbookView xWindow="1660" yWindow="500" windowWidth="44880" windowHeight="28300" xr2:uid="{50492CE8-F5C0-524A-968F-FD9EC2022F6C}"/>
   </bookViews>
   <sheets>
     <sheet name="all_papers" sheetId="1" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="802" uniqueCount="372">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="798" uniqueCount="370">
   <si>
     <t>category (drop down, auto colors row)</t>
   </si>
@@ -802,9 +802,6 @@
     <t>Crous et al.</t>
   </si>
   <si>
-    <t>Nitorgen and phosphorus availabilityies interact to modulate leaf trait scaling relationships across six plant functional types in a controlled-environment study</t>
-  </si>
-  <si>
     <t>https://doi.org/10.1111/nph.14591</t>
   </si>
   <si>
@@ -1210,17 +1207,14 @@
     <t>Data will be made available on request; leaf nutrient data are extractable from Table 2</t>
   </si>
   <si>
-    <t>added_to_datasheet_yn</t>
-  </si>
-  <si>
-    <t>y (50%)</t>
+    <t>Nitrogen and phosphorus availabilities interact to modulate leaf trait scaling relationships across six plant functional types in a controlled-environment study</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1274,13 +1268,6 @@
     </font>
     <font>
       <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
       <color rgb="FF0070C0"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
@@ -1314,11 +1301,47 @@
       <name val="Aptos Narrow"/>
     </font>
     <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <u/>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
-      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1388,7 +1411,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1424,39 +1447,48 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1464,16 +1496,7 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="29">
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
+  <dxfs count="28">
     <dxf>
       <fill>
         <patternFill>
@@ -1718,27 +1741,26 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8093FBDE-B7CD-8C4A-9997-94ED3A5AF75C}" name="Table1" displayName="Table1" ref="A1:R57" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27">
-  <autoFilter ref="A1:R57" xr:uid="{8093FBDE-B7CD-8C4A-9997-94ED3A5AF75C}"/>
-  <tableColumns count="18">
-    <tableColumn id="1" xr3:uid="{E15574CC-1F76-B945-BDBD-AD4BA8C8C3B7}" name="category (drop down, auto colors row)" dataDxfId="26"/>
-    <tableColumn id="19" xr3:uid="{6AFE88A9-1A96-4113-AD81-F820945F5841}" name="notes_by(your name)" dataDxfId="25"/>
-    <tableColumn id="14" xr3:uid="{CAFD1825-FCB5-4229-8252-87372B4269FB}" name="authors" dataDxfId="24"/>
-    <tableColumn id="2" xr3:uid="{3CEA2BFA-BD8F-594C-BAA2-8C8B6F8C553C}" name="year" dataDxfId="23"/>
-    <tableColumn id="3" xr3:uid="{C9E5E426-1492-8748-A2E5-D10DF0CB21E7}" name="title" dataDxfId="22"/>
-    <tableColumn id="4" xr3:uid="{CE25BE8F-B854-264F-BDDD-2F8207E04481}" name="journal" dataDxfId="21"/>
-    <tableColumn id="5" xr3:uid="{47E94D51-0CD6-234D-BFD6-C597383AF0F8}" name="doi" dataDxfId="20" dataCellStyle="Hyperlink"/>
-    <tableColumn id="6" xr3:uid="{1A230D2C-4AF7-8240-8A8A-813805B9F442}" name="traits_measured" dataDxfId="19"/>
-    <tableColumn id="7" xr3:uid="{EAB07DEB-B8D2-7F4D-87F0-F44EA418AE96}" name="n_fert_yn" dataDxfId="18"/>
-    <tableColumn id="8" xr3:uid="{28747112-425A-EF46-BC2E-352E96918620}" name="p_fert_yn" dataDxfId="17"/>
-    <tableColumn id="9" xr3:uid="{B2C892FE-5FF1-7B4A-BA0A-E82FA960CA3D}" name="np_fert_method" dataDxfId="16"/>
-    <tableColumn id="10" xr3:uid="{DB1AB260-DCF4-3049-8F11-4321A3205248}" name="n_avail_yn" dataDxfId="15"/>
-    <tableColumn id="11" xr3:uid="{C4BE562A-BE9F-AF49-A89E-2A47F832C256}" name="p_avail_yn" dataDxfId="14"/>
-    <tableColumn id="12" xr3:uid="{70CD1115-165E-D34F-84D2-2E2BC95B0A35}" name="np_method" dataDxfId="13"/>
-    <tableColumn id="15" xr3:uid="{45D59765-0EA3-F44D-A74A-98D0D16C0FF1}" name="experiment_type" dataDxfId="12"/>
-    <tableColumn id="16" xr3:uid="{FF08C533-3661-42BC-95A5-7AD222A24ACE}" name="data_available_yn" dataDxfId="11"/>
-    <tableColumn id="13" xr3:uid="{A95F19E6-DD0D-574F-B162-EA325C31A05F}" name="notes" dataDxfId="10"/>
-    <tableColumn id="17" xr3:uid="{9042AC09-0FD2-5A4D-84F5-927474DC88F2}" name="added_to_datasheet_yn" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8093FBDE-B7CD-8C4A-9997-94ED3A5AF75C}" name="Table1" displayName="Table1" ref="A1:Q60" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26">
+  <autoFilter ref="A1:Q60" xr:uid="{8093FBDE-B7CD-8C4A-9997-94ED3A5AF75C}"/>
+  <tableColumns count="17">
+    <tableColumn id="1" xr3:uid="{E15574CC-1F76-B945-BDBD-AD4BA8C8C3B7}" name="category (drop down, auto colors row)" dataDxfId="25"/>
+    <tableColumn id="19" xr3:uid="{6AFE88A9-1A96-4113-AD81-F820945F5841}" name="notes_by(your name)" dataDxfId="24"/>
+    <tableColumn id="14" xr3:uid="{CAFD1825-FCB5-4229-8252-87372B4269FB}" name="authors" dataDxfId="23"/>
+    <tableColumn id="2" xr3:uid="{3CEA2BFA-BD8F-594C-BAA2-8C8B6F8C553C}" name="year" dataDxfId="22"/>
+    <tableColumn id="3" xr3:uid="{C9E5E426-1492-8748-A2E5-D10DF0CB21E7}" name="title" dataDxfId="21"/>
+    <tableColumn id="4" xr3:uid="{CE25BE8F-B854-264F-BDDD-2F8207E04481}" name="journal" dataDxfId="20"/>
+    <tableColumn id="5" xr3:uid="{47E94D51-0CD6-234D-BFD6-C597383AF0F8}" name="doi" dataDxfId="19" dataCellStyle="Hyperlink"/>
+    <tableColumn id="6" xr3:uid="{1A230D2C-4AF7-8240-8A8A-813805B9F442}" name="traits_measured" dataDxfId="18"/>
+    <tableColumn id="7" xr3:uid="{EAB07DEB-B8D2-7F4D-87F0-F44EA418AE96}" name="n_fert_yn" dataDxfId="17"/>
+    <tableColumn id="8" xr3:uid="{28747112-425A-EF46-BC2E-352E96918620}" name="p_fert_yn" dataDxfId="16"/>
+    <tableColumn id="9" xr3:uid="{B2C892FE-5FF1-7B4A-BA0A-E82FA960CA3D}" name="np_fert_method" dataDxfId="15"/>
+    <tableColumn id="10" xr3:uid="{DB1AB260-DCF4-3049-8F11-4321A3205248}" name="n_avail_yn" dataDxfId="14"/>
+    <tableColumn id="11" xr3:uid="{C4BE562A-BE9F-AF49-A89E-2A47F832C256}" name="p_avail_yn" dataDxfId="13"/>
+    <tableColumn id="12" xr3:uid="{70CD1115-165E-D34F-84D2-2E2BC95B0A35}" name="np_method" dataDxfId="12"/>
+    <tableColumn id="15" xr3:uid="{45D59765-0EA3-F44D-A74A-98D0D16C0FF1}" name="experiment_type" dataDxfId="11"/>
+    <tableColumn id="16" xr3:uid="{FF08C533-3661-42BC-95A5-7AD222A24ACE}" name="data_available_yn" dataDxfId="10"/>
+    <tableColumn id="13" xr3:uid="{A95F19E6-DD0D-574F-B162-EA325C31A05F}" name="notes" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2061,13 +2083,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72E471E8-ACD0-FD4B-A457-BF8C11A8C657}">
-  <dimension ref="A1:T57"/>
+  <dimension ref="A1:S60"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B37" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B36" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G40" sqref="G40"/>
+      <selection pane="bottomRight" activeCell="K41" sqref="K41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2087,13 +2109,13 @@
     <col min="14" max="14" width="22.33203125" style="2" customWidth="1"/>
     <col min="15" max="15" width="18.5" style="2" customWidth="1"/>
     <col min="16" max="16" width="19.5" style="2" customWidth="1"/>
-    <col min="17" max="18" width="24.6640625" style="2" customWidth="1"/>
-    <col min="19" max="19" width="11" style="2"/>
-    <col min="20" max="20" width="19.1640625" style="2" customWidth="1"/>
-    <col min="21" max="16384" width="11" style="2"/>
+    <col min="17" max="17" width="24.6640625" style="2" customWidth="1"/>
+    <col min="18" max="18" width="11" style="2"/>
+    <col min="19" max="19" width="19.1640625" style="2" customWidth="1"/>
+    <col min="20" max="16384" width="11" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="1" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" s="1" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2145,14 +2167,11 @@
       <c r="Q1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
-        <v>370</v>
-      </c>
-      <c r="T1" s="8" t="s">
+      <c r="S1" s="8" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="119" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19" ht="119" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>18</v>
       </c>
@@ -2197,12 +2216,11 @@
       </c>
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
-      <c r="R2" s="21"/>
-      <c r="T2" s="4" t="s">
+      <c r="S2" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="85" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:19" ht="85" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>27</v>
       </c>
@@ -2247,12 +2265,11 @@
       </c>
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
-      <c r="R3" s="21"/>
-      <c r="T3" s="5" t="s">
+      <c r="S3" s="5" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:20" ht="68" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:19" ht="68" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>35</v>
       </c>
@@ -2297,12 +2314,11 @@
       </c>
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
-      <c r="R4" s="21"/>
-      <c r="T4" s="6" t="s">
+      <c r="S4" s="6" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:20" ht="136" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:19" ht="136" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>18</v>
       </c>
@@ -2347,12 +2363,11 @@
       </c>
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
-      <c r="R5" s="21"/>
-      <c r="T5" s="7" t="s">
+      <c r="S5" s="7" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:20" ht="68" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:19" ht="68" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>18</v>
       </c>
@@ -2400,9 +2415,8 @@
       <c r="Q6" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="R6" s="21"/>
-    </row>
-    <row r="7" spans="1:20" ht="85" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:19" ht="85" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>18</v>
       </c>
@@ -2447,9 +2461,8 @@
       </c>
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
-      <c r="R7" s="21"/>
-    </row>
-    <row r="8" spans="1:20" ht="102" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:19" ht="102" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>27</v>
       </c>
@@ -2494,61 +2507,59 @@
       </c>
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
-      <c r="R8" s="21"/>
-    </row>
-    <row r="9" spans="1:20" ht="136" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
+    </row>
+    <row r="9" spans="1:19" ht="136" x14ac:dyDescent="0.2">
+      <c r="A9" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="24" t="s">
         <v>61</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D9" s="24">
         <v>2022</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="F9" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="G9" s="3" t="s">
+      <c r="G9" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="H9" s="24" t="s">
         <v>65</v>
       </c>
-      <c r="I9" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="K9" s="1" t="s">
+      <c r="I9" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="J9" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="K9" s="24" t="s">
         <v>66</v>
       </c>
-      <c r="L9" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="M9" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="N9" s="1" t="s">
+      <c r="L9" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="M9" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="N9" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="O9" s="1" t="s">
+      <c r="O9" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="P9" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q9" s="1"/>
-      <c r="R9" s="21"/>
-    </row>
-    <row r="10" spans="1:20" ht="119" x14ac:dyDescent="0.2">
+      <c r="P9" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q9" s="24"/>
+    </row>
+    <row r="10" spans="1:19" ht="119" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>27</v>
       </c>
@@ -2593,9 +2604,8 @@
       </c>
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
-      <c r="R10" s="21"/>
-    </row>
-    <row r="11" spans="1:20" ht="85" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:19" ht="85" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>27</v>
       </c>
@@ -2640,9 +2650,8 @@
       </c>
       <c r="O11" s="1"/>
       <c r="P11" s="1"/>
-      <c r="R11" s="21"/>
-    </row>
-    <row r="12" spans="1:20" ht="136" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:19" ht="136" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>18</v>
       </c>
@@ -2687,9 +2696,8 @@
       </c>
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
-      <c r="R12" s="21"/>
-    </row>
-    <row r="13" spans="1:20" ht="102" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:19" ht="102" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>27</v>
       </c>
@@ -2734,9 +2742,8 @@
       </c>
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
-      <c r="R13" s="21"/>
-    </row>
-    <row r="14" spans="1:20" ht="136" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:19" ht="136" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>27</v>
       </c>
@@ -2784,9 +2791,8 @@
       <c r="Q14" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="R14" s="21"/>
-    </row>
-    <row r="15" spans="1:20" ht="85" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:19" ht="85" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>18</v>
       </c>
@@ -2834,9 +2840,8 @@
       <c r="Q15" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="R15" s="21"/>
-    </row>
-    <row r="16" spans="1:20" ht="68" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:19" ht="68" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>27</v>
       </c>
@@ -2881,9 +2886,8 @@
       </c>
       <c r="O16" s="1"/>
       <c r="P16" s="1"/>
-      <c r="R16" s="21"/>
-    </row>
-    <row r="17" spans="1:18" ht="85" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:17" ht="85" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>18</v>
       </c>
@@ -2928,9 +2932,8 @@
       </c>
       <c r="O17" s="1"/>
       <c r="P17" s="1"/>
-      <c r="R17" s="21"/>
-    </row>
-    <row r="18" spans="1:18" ht="119" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:17" ht="119" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>41</v>
       </c>
@@ -2977,9 +2980,8 @@
       <c r="P18" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="R18" s="21"/>
-    </row>
-    <row r="19" spans="1:18" ht="68" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:17" ht="68" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>18</v>
       </c>
@@ -3024,9 +3026,8 @@
       </c>
       <c r="O19" s="1"/>
       <c r="P19" s="1"/>
-      <c r="R19" s="21"/>
-    </row>
-    <row r="20" spans="1:18" ht="85" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:17" ht="85" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>18</v>
       </c>
@@ -3074,9 +3075,8 @@
       <c r="Q20" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="R20" s="21"/>
-    </row>
-    <row r="21" spans="1:18" ht="102" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:17" ht="102" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>41</v>
       </c>
@@ -3121,9 +3121,8 @@
       <c r="P21" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="R21" s="21"/>
-    </row>
-    <row r="22" spans="1:18" ht="153" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:17" ht="153" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>41</v>
       </c>
@@ -3170,9 +3169,8 @@
       <c r="P22" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="R22" s="21"/>
-    </row>
-    <row r="23" spans="1:18" ht="119" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="1:17" ht="119" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>35</v>
       </c>
@@ -3212,9 +3210,8 @@
       <c r="M23" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="R23" s="21"/>
-    </row>
-    <row r="24" spans="1:18" ht="119" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="1:17" ht="119" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>41</v>
       </c>
@@ -3262,9 +3259,8 @@
         <v>25</v>
       </c>
       <c r="Q24" s="1"/>
-      <c r="R24" s="21"/>
-    </row>
-    <row r="25" spans="1:18" ht="102" x14ac:dyDescent="0.2">
+    </row>
+    <row r="25" spans="1:17" ht="102" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>41</v>
       </c>
@@ -3314,9 +3310,8 @@
       <c r="Q25" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="R25" s="21"/>
-    </row>
-    <row r="26" spans="1:18" ht="119" x14ac:dyDescent="0.2">
+    </row>
+    <row r="26" spans="1:17" ht="119" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>41</v>
       </c>
@@ -3364,9 +3359,8 @@
         <v>155</v>
       </c>
       <c r="Q26" s="1"/>
-      <c r="R26" s="21"/>
-    </row>
-    <row r="27" spans="1:18" ht="136" x14ac:dyDescent="0.2">
+    </row>
+    <row r="27" spans="1:17" ht="136" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>41</v>
       </c>
@@ -3414,9 +3408,8 @@
         <v>155</v>
       </c>
       <c r="Q27" s="1"/>
-      <c r="R27" s="21"/>
-    </row>
-    <row r="28" spans="1:18" ht="68" x14ac:dyDescent="0.2">
+    </row>
+    <row r="28" spans="1:17" ht="68" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>27</v>
       </c>
@@ -3464,9 +3457,8 @@
       <c r="Q28" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="R28" s="21"/>
-    </row>
-    <row r="29" spans="1:18" ht="102" x14ac:dyDescent="0.2">
+    </row>
+    <row r="29" spans="1:17" ht="102" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>41</v>
       </c>
@@ -3514,61 +3506,59 @@
         <v>25</v>
       </c>
       <c r="Q29" s="1"/>
-      <c r="R29" s="21"/>
-    </row>
-    <row r="30" spans="1:18" ht="119" x14ac:dyDescent="0.2">
-      <c r="A30" s="1" t="s">
+    </row>
+    <row r="30" spans="1:17" ht="119" x14ac:dyDescent="0.2">
+      <c r="A30" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B30" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="C30" s="24" t="s">
         <v>184</v>
       </c>
-      <c r="D30" s="1">
+      <c r="D30" s="24">
         <v>2021</v>
       </c>
-      <c r="E30" s="1" t="s">
+      <c r="E30" s="24" t="s">
         <v>185</v>
       </c>
-      <c r="F30" s="1" t="s">
+      <c r="F30" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="G30" s="3" t="s">
+      <c r="G30" s="25" t="s">
         <v>186</v>
       </c>
-      <c r="H30" s="1" t="s">
+      <c r="H30" s="24" t="s">
         <v>187</v>
       </c>
-      <c r="I30" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="J30" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="K30" s="1" t="s">
+      <c r="I30" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="J30" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="K30" s="24" t="s">
         <v>188</v>
       </c>
-      <c r="L30" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="M30" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="N30" s="1" t="s">
+      <c r="L30" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="M30" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="N30" s="24" t="s">
         <v>189</v>
       </c>
-      <c r="O30" s="1"/>
-      <c r="P30" s="1" t="s">
+      <c r="O30" s="24"/>
+      <c r="P30" s="24" t="s">
         <v>190</v>
       </c>
-      <c r="Q30" s="1" t="s">
+      <c r="Q30" s="24" t="s">
         <v>191</v>
       </c>
-      <c r="R30" s="21"/>
-    </row>
-    <row r="31" spans="1:18" ht="68" x14ac:dyDescent="0.2">
+    </row>
+    <row r="31" spans="1:17" ht="68" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>41</v>
       </c>
@@ -3614,9 +3604,8 @@
       <c r="Q31" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="R31" s="21"/>
-    </row>
-    <row r="32" spans="1:18" ht="170" x14ac:dyDescent="0.2">
+    </row>
+    <row r="32" spans="1:17" ht="170" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>27</v>
       </c>
@@ -3662,9 +3651,8 @@
       <c r="O32" s="1"/>
       <c r="P32" s="1"/>
       <c r="Q32" s="1"/>
-      <c r="R32" s="21"/>
-    </row>
-    <row r="33" spans="1:18" ht="85" x14ac:dyDescent="0.2">
+    </row>
+    <row r="33" spans="1:17" ht="85" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>27</v>
       </c>
@@ -3710,9 +3698,8 @@
       <c r="O33" s="1"/>
       <c r="P33" s="1"/>
       <c r="Q33" s="1"/>
-      <c r="R33" s="21"/>
-    </row>
-    <row r="34" spans="1:18" ht="119" x14ac:dyDescent="0.2">
+    </row>
+    <row r="34" spans="1:17" ht="119" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>27</v>
       </c>
@@ -3758,9 +3745,8 @@
       <c r="O34" s="1"/>
       <c r="P34" s="1"/>
       <c r="Q34" s="1"/>
-      <c r="R34" s="21"/>
-    </row>
-    <row r="35" spans="1:18" ht="153" x14ac:dyDescent="0.2">
+    </row>
+    <row r="35" spans="1:17" ht="153" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>41</v>
       </c>
@@ -3771,7 +3757,7 @@
         <v>216</v>
       </c>
       <c r="D35" s="1">
-        <v>1999</v>
+        <v>2014</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>217</v>
@@ -3808,9 +3794,8 @@
         <v>222</v>
       </c>
       <c r="Q35" s="1"/>
-      <c r="R35" s="21"/>
-    </row>
-    <row r="36" spans="1:18" ht="187" x14ac:dyDescent="0.2">
+    </row>
+    <row r="36" spans="1:17" ht="187" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>41</v>
       </c>
@@ -3858,9 +3843,8 @@
         <v>25</v>
       </c>
       <c r="Q36" s="1"/>
-      <c r="R36" s="21"/>
-    </row>
-    <row r="37" spans="1:18" ht="85" x14ac:dyDescent="0.2">
+    </row>
+    <row r="37" spans="1:17" ht="85" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>27</v>
       </c>
@@ -3908,59 +3892,57 @@
       <c r="Q37" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="R37" s="21"/>
-    </row>
-    <row r="38" spans="1:18" ht="119" x14ac:dyDescent="0.2">
-      <c r="A38" s="1" t="s">
+    </row>
+    <row r="38" spans="1:17" ht="119" x14ac:dyDescent="0.2">
+      <c r="A38" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="B38" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="C38" s="1" t="s">
+      <c r="C38" s="24" t="s">
         <v>238</v>
       </c>
-      <c r="D38" s="1">
+      <c r="D38" s="24">
         <v>2017</v>
       </c>
-      <c r="E38" s="1" t="s">
+      <c r="E38" s="24" t="s">
+        <v>369</v>
+      </c>
+      <c r="F38" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="G38" s="25" t="s">
         <v>239</v>
       </c>
-      <c r="F38" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="G38" s="3" t="s">
+      <c r="H38" s="24" t="s">
         <v>240</v>
       </c>
-      <c r="H38" s="1" t="s">
+      <c r="I38" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="J38" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="K38" s="24" t="s">
         <v>241</v>
       </c>
-      <c r="I38" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="J38" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="K38" s="1" t="s">
+      <c r="L38" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="M38" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="N38" s="24" t="s">
         <v>242</v>
       </c>
-      <c r="L38" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="M38" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="N38" s="1" t="s">
+      <c r="O38" s="24"/>
+      <c r="P38" s="24" t="s">
         <v>243</v>
       </c>
-      <c r="O38" s="1"/>
-      <c r="P38" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="Q38" s="1"/>
-      <c r="R38" s="21"/>
-    </row>
-    <row r="39" spans="1:18" ht="102" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Q38" s="24"/>
+    </row>
+    <row r="39" spans="1:17" ht="102" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>27</v>
       </c>
@@ -3968,19 +3950,19 @@
         <v>19</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D39" s="1">
         <v>2014</v>
       </c>
       <c r="E39" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="F39" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="F39" s="1" t="s">
+      <c r="G39" s="3" t="s">
         <v>247</v>
-      </c>
-      <c r="G39" s="3" t="s">
-        <v>248</v>
       </c>
       <c r="H39" s="1"/>
       <c r="I39" s="1" t="s">
@@ -4000,9 +3982,8 @@
       <c r="O39" s="1"/>
       <c r="P39" s="1"/>
       <c r="Q39" s="1"/>
-      <c r="R39" s="21"/>
-    </row>
-    <row r="40" spans="1:18" ht="136" x14ac:dyDescent="0.2">
+    </row>
+    <row r="40" spans="1:17" ht="136" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>41</v>
       </c>
@@ -4010,49 +3991,48 @@
         <v>19</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D40" s="1">
         <v>2014</v>
       </c>
       <c r="E40" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="F40" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="F40" s="1" t="s">
+      <c r="G40" s="3" t="s">
         <v>251</v>
       </c>
-      <c r="G40" s="3" t="s">
+      <c r="H40" s="1" t="s">
         <v>252</v>
       </c>
-      <c r="H40" s="1" t="s">
+      <c r="I40" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J40" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K40" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="I40" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="J40" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="K40" s="1" t="s">
+      <c r="L40" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="M40" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="N40" s="1" t="s">
         <v>254</v>
-      </c>
-      <c r="L40" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="M40" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="N40" s="1" t="s">
-        <v>255</v>
       </c>
       <c r="O40" s="1"/>
       <c r="P40" s="1" t="s">
         <v>25</v>
       </c>
       <c r="Q40" s="1"/>
-      <c r="R40" s="21"/>
-    </row>
-    <row r="41" spans="1:18" ht="102" x14ac:dyDescent="0.2">
+    </row>
+    <row r="41" spans="1:17" ht="102" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>41</v>
       </c>
@@ -4060,31 +4040,31 @@
         <v>19</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D41" s="1">
         <v>2007</v>
       </c>
       <c r="E41" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="F41" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="F41" s="1" t="s">
+      <c r="G41" s="3" t="s">
         <v>258</v>
       </c>
-      <c r="G41" s="3" t="s">
+      <c r="H41" s="1" t="s">
         <v>259</v>
       </c>
-      <c r="H41" s="1" t="s">
+      <c r="I41" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J41" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K41" s="1" t="s">
         <v>260</v>
-      </c>
-      <c r="I41" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="J41" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="K41" s="1" t="s">
-        <v>261</v>
       </c>
       <c r="L41" s="1" t="s">
         <v>25</v>
@@ -4097,14 +4077,13 @@
       </c>
       <c r="O41" s="1"/>
       <c r="P41" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="Q41" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="Q41" s="1" t="s">
-        <v>263</v>
-      </c>
-      <c r="R41" s="21"/>
-    </row>
-    <row r="42" spans="1:18" ht="119" x14ac:dyDescent="0.2">
+    </row>
+    <row r="42" spans="1:17" ht="119" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>41</v>
       </c>
@@ -4112,31 +4091,31 @@
         <v>19</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D42" s="1">
         <v>2005</v>
       </c>
       <c r="E42" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="F42" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="F42" s="1" t="s">
+      <c r="G42" s="3" t="s">
         <v>266</v>
       </c>
-      <c r="G42" s="3" t="s">
+      <c r="H42" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="H42" s="1" t="s">
+      <c r="I42" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J42" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K42" s="1" t="s">
         <v>268</v>
-      </c>
-      <c r="I42" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="J42" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="K42" s="1" t="s">
-        <v>269</v>
       </c>
       <c r="L42" s="1" t="s">
         <v>25</v>
@@ -4149,14 +4128,13 @@
       </c>
       <c r="O42" s="1"/>
       <c r="P42" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="Q42" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="Q42" s="1" t="s">
-        <v>263</v>
-      </c>
-      <c r="R42" s="21"/>
-    </row>
-    <row r="43" spans="1:18" ht="102" x14ac:dyDescent="0.2">
+    </row>
+    <row r="43" spans="1:17" ht="102" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>41</v>
       </c>
@@ -4164,31 +4142,31 @@
         <v>19</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D43" s="1">
         <v>2002</v>
       </c>
       <c r="E43" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="G43" s="3" t="s">
         <v>271</v>
       </c>
-      <c r="F43" s="1" t="s">
-        <v>258</v>
-      </c>
-      <c r="G43" s="3" t="s">
+      <c r="H43" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="H43" s="1" t="s">
+      <c r="I43" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J43" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K43" s="1" t="s">
         <v>273</v>
-      </c>
-      <c r="I43" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="J43" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="K43" s="1" t="s">
-        <v>274</v>
       </c>
       <c r="L43" s="1" t="s">
         <v>25</v>
@@ -4202,117 +4180,112 @@
       <c r="O43" s="1"/>
       <c r="P43" s="1"/>
       <c r="Q43" s="1" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17" s="17" customFormat="1" ht="102" x14ac:dyDescent="0.2">
+      <c r="A44" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="B44" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C44" s="14" t="s">
+        <v>269</v>
+      </c>
+      <c r="D44" s="14">
+        <v>2002</v>
+      </c>
+      <c r="E44" s="14" t="s">
+        <v>270</v>
+      </c>
+      <c r="F44" s="14" t="s">
+        <v>257</v>
+      </c>
+      <c r="G44" s="16" t="s">
+        <v>271</v>
+      </c>
+      <c r="H44" s="14" t="s">
+        <v>272</v>
+      </c>
+      <c r="I44" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="J44" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="K44" s="14" t="s">
         <v>275</v>
       </c>
-      <c r="R43" s="21"/>
-    </row>
-    <row r="44" spans="1:18" s="18" customFormat="1" ht="102" x14ac:dyDescent="0.2">
-      <c r="A44" s="15" t="s">
+      <c r="L44" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="M44" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="N44" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="O44" s="14"/>
+      <c r="P44" s="14" t="s">
+        <v>276</v>
+      </c>
+      <c r="Q44" s="14" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17" s="12" customFormat="1" ht="119" x14ac:dyDescent="0.2">
+      <c r="A45" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="B44" s="15" t="s">
+      <c r="B45" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="C44" s="15" t="s">
-        <v>270</v>
-      </c>
-      <c r="D44" s="15">
-        <v>2002</v>
-      </c>
-      <c r="E44" s="15" t="s">
-        <v>271</v>
-      </c>
-      <c r="F44" s="15" t="s">
-        <v>258</v>
-      </c>
-      <c r="G44" s="17" t="s">
-        <v>272</v>
-      </c>
-      <c r="H44" s="15" t="s">
-        <v>273</v>
-      </c>
-      <c r="I44" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="J44" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="K44" s="15" t="s">
-        <v>276</v>
-      </c>
-      <c r="L44" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="M44" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="N44" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="O44" s="15"/>
-      <c r="P44" s="15" t="s">
-        <v>277</v>
-      </c>
-      <c r="Q44" s="15" t="s">
+      <c r="C45" s="22" t="s">
+        <v>184</v>
+      </c>
+      <c r="D45" s="22">
+        <v>2019</v>
+      </c>
+      <c r="E45" s="22" t="s">
         <v>278</v>
       </c>
-      <c r="R44" s="22"/>
-    </row>
-    <row r="45" spans="1:18" s="13" customFormat="1" ht="119" x14ac:dyDescent="0.2">
-      <c r="A45" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="B45" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="C45" s="12" t="s">
-        <v>184</v>
-      </c>
-      <c r="D45" s="12">
-        <v>2019</v>
-      </c>
-      <c r="E45" s="12" t="s">
+      <c r="F45" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="G45" s="23" t="s">
         <v>279</v>
       </c>
-      <c r="F45" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="G45" s="19" t="s">
+      <c r="H45" s="22" t="s">
         <v>280</v>
       </c>
-      <c r="H45" s="12" t="s">
+      <c r="I45" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="J45" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="K45" s="22" t="s">
         <v>281</v>
       </c>
-      <c r="I45" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="J45" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="K45" s="12" t="s">
+      <c r="L45" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="M45" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="N45" s="22" t="s">
         <v>282</v>
       </c>
-      <c r="L45" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="M45" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="N45" s="12" t="s">
+      <c r="O45" s="22"/>
+      <c r="P45" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q45" s="22" t="s">
         <v>283</v>
       </c>
-      <c r="O45" s="12"/>
-      <c r="P45" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q45" s="12" t="s">
-        <v>284</v>
-      </c>
-      <c r="R45" s="23" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="46" spans="1:18" ht="102" x14ac:dyDescent="0.2">
+    </row>
+    <row r="46" spans="1:17" ht="102" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>27</v>
       </c>
@@ -4320,22 +4293,22 @@
         <v>19</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D46" s="1">
         <v>2009</v>
       </c>
       <c r="E46" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="F46" s="1" t="s">
         <v>286</v>
       </c>
-      <c r="F46" s="1" t="s">
+      <c r="G46" s="3" t="s">
         <v>287</v>
       </c>
-      <c r="G46" s="3" t="s">
+      <c r="H46" s="1" t="s">
         <v>288</v>
-      </c>
-      <c r="H46" s="1" t="s">
-        <v>289</v>
       </c>
       <c r="I46" s="1" t="s">
         <v>25</v>
@@ -4353,116 +4326,113 @@
         <v>33</v>
       </c>
       <c r="N46" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="O46" s="1"/>
       <c r="P46" s="1"/>
       <c r="Q46" s="1" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17" ht="119" x14ac:dyDescent="0.2">
+      <c r="A47" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="B47" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C47" s="14" t="s">
         <v>291</v>
       </c>
-      <c r="R46" s="21"/>
-    </row>
-    <row r="47" spans="1:18" ht="119" x14ac:dyDescent="0.2">
-      <c r="A47" s="15" t="s">
+      <c r="D47" s="14">
+        <v>1989</v>
+      </c>
+      <c r="E47" s="14" t="s">
+        <v>292</v>
+      </c>
+      <c r="F47" s="14" t="s">
+        <v>225</v>
+      </c>
+      <c r="G47" s="16" t="s">
+        <v>293</v>
+      </c>
+      <c r="H47" s="14" t="s">
+        <v>294</v>
+      </c>
+      <c r="I47" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="J47" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="K47" s="14" t="s">
+        <v>295</v>
+      </c>
+      <c r="L47" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="M47" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="N47" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="O47" s="1"/>
+      <c r="P47" s="14" t="s">
+        <v>222</v>
+      </c>
+      <c r="Q47" s="1"/>
+    </row>
+    <row r="48" spans="1:17" s="17" customFormat="1" ht="153" x14ac:dyDescent="0.2">
+      <c r="A48" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="B47" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="C47" s="15" t="s">
-        <v>292</v>
-      </c>
-      <c r="D47" s="15">
-        <v>1989</v>
-      </c>
-      <c r="E47" s="15" t="s">
-        <v>293</v>
-      </c>
-      <c r="F47" s="15" t="s">
-        <v>225</v>
-      </c>
-      <c r="G47" s="17" t="s">
-        <v>294</v>
-      </c>
-      <c r="H47" s="15" t="s">
-        <v>295</v>
-      </c>
-      <c r="I47" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="J47" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="K47" s="15" t="s">
+      <c r="B48" s="14" t="s">
         <v>296</v>
       </c>
-      <c r="L47" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="M47" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="N47" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="O47" s="1"/>
-      <c r="P47" s="15" t="s">
-        <v>222</v>
-      </c>
-      <c r="Q47" s="1"/>
-      <c r="R47" s="21"/>
-    </row>
-    <row r="48" spans="1:18" s="18" customFormat="1" ht="153" x14ac:dyDescent="0.2">
-      <c r="A48" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="B48" s="15" t="s">
+      <c r="C48" s="14" t="s">
         <v>297</v>
       </c>
-      <c r="C48" s="15" t="s">
+      <c r="D48" s="14">
+        <v>1995</v>
+      </c>
+      <c r="E48" s="14" t="s">
         <v>298</v>
       </c>
-      <c r="D48" s="15">
-        <v>1995</v>
-      </c>
-      <c r="E48" s="15" t="s">
+      <c r="F48" s="14" t="s">
         <v>299</v>
       </c>
-      <c r="F48" s="15" t="s">
+      <c r="G48" s="16" t="s">
         <v>300</v>
       </c>
-      <c r="G48" s="17" t="s">
+      <c r="H48" s="14" t="s">
         <v>301</v>
       </c>
-      <c r="H48" s="15" t="s">
+      <c r="I48" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="J48" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="K48" s="14" t="s">
         <v>302</v>
       </c>
-      <c r="I48" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="J48" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="K48" s="15" t="s">
+      <c r="L48" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="M48" s="14"/>
+      <c r="N48" s="14"/>
+      <c r="O48" s="14" t="s">
         <v>303</v>
       </c>
-      <c r="L48" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="M48" s="15"/>
-      <c r="N48" s="15"/>
-      <c r="O48" s="15" t="s">
+      <c r="P48" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q48" s="14" t="s">
         <v>304</v>
       </c>
-      <c r="P48" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q48" s="15" t="s">
-        <v>305</v>
-      </c>
-      <c r="R48" s="22"/>
-    </row>
-    <row r="49" spans="1:18" ht="119" x14ac:dyDescent="0.2">
+    </row>
+    <row r="49" spans="1:17" ht="119" x14ac:dyDescent="0.2">
       <c r="A49" s="1"/>
       <c r="B49" s="1" t="s">
         <v>19</v>
@@ -4474,13 +4444,13 @@
         <v>2019</v>
       </c>
       <c r="E49" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="F49" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="F49" s="1" t="s">
+      <c r="G49" s="3" t="s">
         <v>307</v>
-      </c>
-      <c r="G49" s="3" t="s">
-        <v>308</v>
       </c>
       <c r="H49" s="1"/>
       <c r="I49" s="1"/>
@@ -4492,27 +4462,26 @@
       <c r="O49" s="1"/>
       <c r="P49" s="1"/>
       <c r="Q49" s="1"/>
-      <c r="R49" s="21"/>
-    </row>
-    <row r="50" spans="1:18" ht="68" x14ac:dyDescent="0.2">
+    </row>
+    <row r="50" spans="1:17" ht="68" x14ac:dyDescent="0.2">
       <c r="A50" s="1"/>
       <c r="B50" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D50" s="1">
         <v>2011</v>
       </c>
       <c r="E50" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="G50" s="3" t="s">
         <v>309</v>
-      </c>
-      <c r="F50" s="1" t="s">
-        <v>258</v>
-      </c>
-      <c r="G50" s="3" t="s">
-        <v>310</v>
       </c>
       <c r="H50" s="1"/>
       <c r="I50" s="1"/>
@@ -4524,414 +4493,459 @@
       <c r="O50" s="1"/>
       <c r="P50" s="1"/>
       <c r="Q50" s="1"/>
-      <c r="R50" s="21"/>
-    </row>
-    <row r="51" spans="1:18" s="18" customFormat="1" ht="153" x14ac:dyDescent="0.2">
-      <c r="A51" s="15" t="s">
+    </row>
+    <row r="51" spans="1:17" s="17" customFormat="1" ht="153" x14ac:dyDescent="0.2">
+      <c r="A51" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="B51" s="15" t="s">
+      <c r="B51" s="19" t="s">
+        <v>310</v>
+      </c>
+      <c r="C51" s="19" t="s">
         <v>311</v>
       </c>
-      <c r="C51" s="15" t="s">
+      <c r="D51" s="19">
+        <v>2022</v>
+      </c>
+      <c r="E51" s="19" t="s">
         <v>312</v>
       </c>
-      <c r="D51" s="15">
+      <c r="F51" s="19" t="s">
+        <v>313</v>
+      </c>
+      <c r="G51" s="26" t="s">
+        <v>314</v>
+      </c>
+      <c r="H51" s="19" t="s">
+        <v>315</v>
+      </c>
+      <c r="I51" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="J51" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="K51" s="19" t="s">
+        <v>316</v>
+      </c>
+      <c r="L51" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="M51" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="N51" s="19"/>
+      <c r="O51" s="19"/>
+      <c r="P51" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q51" s="19" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="52" spans="1:17" ht="102" x14ac:dyDescent="0.2">
+      <c r="A52" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="B52" s="14" t="s">
+        <v>296</v>
+      </c>
+      <c r="C52" s="14" t="s">
+        <v>317</v>
+      </c>
+      <c r="D52" s="14">
+        <v>2014</v>
+      </c>
+      <c r="E52" s="14" t="s">
+        <v>318</v>
+      </c>
+      <c r="F52" s="14" t="s">
+        <v>165</v>
+      </c>
+      <c r="G52" s="15" t="s">
+        <v>319</v>
+      </c>
+      <c r="H52" s="14" t="s">
+        <v>320</v>
+      </c>
+      <c r="I52" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="J52" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="K52" s="14" t="s">
+        <v>321</v>
+      </c>
+      <c r="L52" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="M52" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="N52" s="14" t="s">
+        <v>322</v>
+      </c>
+      <c r="O52" s="14" t="s">
+        <v>303</v>
+      </c>
+      <c r="P52" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q52" s="13"/>
+    </row>
+    <row r="53" spans="1:17" s="17" customFormat="1" ht="187" x14ac:dyDescent="0.2">
+      <c r="A53" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="B53" s="14" t="s">
+        <v>296</v>
+      </c>
+      <c r="C53" s="14" t="s">
+        <v>323</v>
+      </c>
+      <c r="D53" s="14">
         <v>2022</v>
       </c>
-      <c r="E51" s="15" t="s">
-        <v>313</v>
-      </c>
-      <c r="F51" s="15" t="s">
-        <v>314</v>
-      </c>
-      <c r="G51" s="17" t="s">
-        <v>315</v>
-      </c>
-      <c r="H51" s="15" t="s">
-        <v>316</v>
-      </c>
-      <c r="I51" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="J51" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="K51" s="15" t="s">
-        <v>317</v>
-      </c>
-      <c r="L51" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="M51" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="N51" s="15"/>
-      <c r="O51" s="15"/>
-      <c r="P51" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q51" s="15" t="s">
-        <v>369</v>
-      </c>
-      <c r="R51" s="22" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="52" spans="1:18" ht="102" x14ac:dyDescent="0.2">
-      <c r="A52" s="15" t="s">
+      <c r="E53" s="14" t="s">
+        <v>324</v>
+      </c>
+      <c r="F53" s="14" t="s">
+        <v>306</v>
+      </c>
+      <c r="G53" s="15" t="s">
+        <v>325</v>
+      </c>
+      <c r="H53" s="14" t="s">
+        <v>326</v>
+      </c>
+      <c r="I53" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="J53" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="K53" s="14" t="s">
+        <v>327</v>
+      </c>
+      <c r="L53" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="M53" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="N53" s="14" t="s">
+        <v>328</v>
+      </c>
+      <c r="O53" s="14" t="s">
+        <v>329</v>
+      </c>
+      <c r="P53" s="14" t="s">
+        <v>330</v>
+      </c>
+      <c r="Q53" s="14" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="54" spans="1:17" s="17" customFormat="1" ht="306" x14ac:dyDescent="0.2">
+      <c r="A54" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="B52" s="15" t="s">
-        <v>297</v>
-      </c>
-      <c r="C52" s="15" t="s">
-        <v>318</v>
-      </c>
-      <c r="D52" s="15">
-        <v>2014</v>
-      </c>
-      <c r="E52" s="15" t="s">
-        <v>319</v>
-      </c>
-      <c r="F52" s="15" t="s">
-        <v>165</v>
-      </c>
-      <c r="G52" s="16" t="s">
-        <v>320</v>
-      </c>
-      <c r="H52" s="15" t="s">
-        <v>321</v>
-      </c>
-      <c r="I52" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="J52" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="K52" s="15" t="s">
-        <v>322</v>
-      </c>
-      <c r="L52" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="M52" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="N52" s="15" t="s">
-        <v>323</v>
-      </c>
-      <c r="O52" s="15" t="s">
-        <v>304</v>
-      </c>
-      <c r="P52" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q52" s="14"/>
-      <c r="R52" s="21"/>
-    </row>
-    <row r="53" spans="1:18" s="18" customFormat="1" ht="187" x14ac:dyDescent="0.2">
-      <c r="A53" s="15" t="s">
+      <c r="B54" s="14" t="s">
+        <v>310</v>
+      </c>
+      <c r="C54" s="14" t="s">
+        <v>332</v>
+      </c>
+      <c r="D54" s="14">
+        <v>2024</v>
+      </c>
+      <c r="E54" s="14" t="s">
+        <v>333</v>
+      </c>
+      <c r="F54" s="14" t="s">
+        <v>334</v>
+      </c>
+      <c r="G54" s="15" t="s">
+        <v>335</v>
+      </c>
+      <c r="H54" s="14" t="s">
+        <v>336</v>
+      </c>
+      <c r="I54" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="J54" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="K54" s="14" t="s">
+        <v>337</v>
+      </c>
+      <c r="L54" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="M54" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="N54" s="18" t="s">
+        <v>338</v>
+      </c>
+      <c r="O54" s="14" t="s">
+        <v>329</v>
+      </c>
+      <c r="P54" s="14" t="s">
+        <v>339</v>
+      </c>
+      <c r="Q54" s="14" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="55" spans="1:17" s="17" customFormat="1" ht="113.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="B53" s="15" t="s">
-        <v>297</v>
-      </c>
-      <c r="C53" s="15" t="s">
-        <v>324</v>
-      </c>
-      <c r="D53" s="15">
-        <v>2022</v>
-      </c>
-      <c r="E53" s="15" t="s">
-        <v>325</v>
-      </c>
-      <c r="F53" s="15" t="s">
-        <v>307</v>
-      </c>
-      <c r="G53" s="16" t="s">
-        <v>326</v>
-      </c>
-      <c r="H53" s="15" t="s">
-        <v>327</v>
-      </c>
-      <c r="I53" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="J53" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="K53" s="15" t="s">
-        <v>328</v>
-      </c>
-      <c r="L53" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="M53" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="N53" s="15" t="s">
+      <c r="B55" s="19" t="s">
+        <v>310</v>
+      </c>
+      <c r="C55" s="19" t="s">
+        <v>341</v>
+      </c>
+      <c r="D55" s="19">
+        <v>2023</v>
+      </c>
+      <c r="E55" s="19" t="s">
+        <v>342</v>
+      </c>
+      <c r="F55" s="19" t="s">
+        <v>343</v>
+      </c>
+      <c r="G55" s="20" t="s">
+        <v>344</v>
+      </c>
+      <c r="H55" s="21" t="s">
+        <v>345</v>
+      </c>
+      <c r="I55" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="J55" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="K55" s="19"/>
+      <c r="L55" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="M55" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="N55" s="19" t="s">
+        <v>346</v>
+      </c>
+      <c r="O55" s="19" t="s">
         <v>329</v>
       </c>
-      <c r="O53" s="15" t="s">
-        <v>330</v>
-      </c>
-      <c r="P53" s="15" t="s">
-        <v>331</v>
-      </c>
-      <c r="Q53" s="15" t="s">
-        <v>332</v>
-      </c>
-      <c r="R53" s="22"/>
-    </row>
-    <row r="54" spans="1:18" s="18" customFormat="1" ht="306" x14ac:dyDescent="0.2">
-      <c r="A54" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="B54" s="15" t="s">
-        <v>311</v>
-      </c>
-      <c r="C54" s="15" t="s">
-        <v>333</v>
-      </c>
-      <c r="D54" s="15">
-        <v>2024</v>
-      </c>
-      <c r="E54" s="15" t="s">
-        <v>334</v>
-      </c>
-      <c r="F54" s="15" t="s">
-        <v>335</v>
-      </c>
-      <c r="G54" s="16" t="s">
-        <v>336</v>
-      </c>
-      <c r="H54" s="15" t="s">
-        <v>337</v>
-      </c>
-      <c r="I54" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="J54" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="K54" s="15" t="s">
-        <v>338</v>
-      </c>
-      <c r="L54" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="M54" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="N54" s="20" t="s">
-        <v>339</v>
-      </c>
-      <c r="O54" s="15" t="s">
-        <v>330</v>
-      </c>
-      <c r="P54" s="15" t="s">
-        <v>340</v>
-      </c>
-      <c r="Q54" s="15" t="s">
-        <v>341</v>
-      </c>
-      <c r="R54" s="22"/>
-    </row>
-    <row r="55" spans="1:18" s="18" customFormat="1" ht="113.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="B55" s="15" t="s">
-        <v>311</v>
-      </c>
-      <c r="C55" s="15" t="s">
-        <v>342</v>
-      </c>
-      <c r="D55" s="15">
-        <v>2023</v>
-      </c>
-      <c r="E55" s="15" t="s">
-        <v>343</v>
-      </c>
-      <c r="F55" s="15" t="s">
-        <v>344</v>
-      </c>
-      <c r="G55" s="16" t="s">
-        <v>345</v>
-      </c>
-      <c r="H55" s="20" t="s">
-        <v>346</v>
-      </c>
-      <c r="I55" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="J55" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="K55" s="15"/>
-      <c r="L55" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="M55" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="N55" s="15" t="s">
+      <c r="P55" s="19" t="s">
         <v>347</v>
       </c>
-      <c r="O55" s="15" t="s">
-        <v>330</v>
-      </c>
-      <c r="P55" s="15" t="s">
+      <c r="Q55" s="19" t="s">
         <v>348</v>
       </c>
-      <c r="Q55" s="15" t="s">
-        <v>349</v>
-      </c>
-      <c r="R55" s="22" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="56" spans="1:18" ht="85" x14ac:dyDescent="0.2">
+    </row>
+    <row r="56" spans="1:17" ht="85" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>41</v>
       </c>
       <c r="B56" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="C56" s="1" t="s">
         <v>350</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>351</v>
       </c>
       <c r="D56" s="1">
         <v>2020</v>
       </c>
       <c r="E56" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="G56" s="9" t="s">
         <v>352</v>
       </c>
-      <c r="F56" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="G56" s="9" t="s">
+      <c r="H56" s="1" t="s">
         <v>353</v>
       </c>
-      <c r="H56" s="1" t="s">
+      <c r="I56" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J56" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K56" s="1" t="s">
         <v>354</v>
       </c>
-      <c r="I56" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="J56" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="K56" s="1" t="s">
+      <c r="L56" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M56" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N56" s="1" t="s">
         <v>355</v>
       </c>
-      <c r="L56" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="M56" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="N56" s="1" t="s">
+      <c r="O56" s="1" t="s">
         <v>356</v>
       </c>
-      <c r="O56" s="1" t="s">
+      <c r="P56" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q56" s="1" t="s">
         <v>357</v>
       </c>
-      <c r="P56" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q56" s="1" t="s">
-        <v>358</v>
-      </c>
-      <c r="R56" s="21"/>
-    </row>
-    <row r="57" spans="1:18" ht="85" x14ac:dyDescent="0.2">
+    </row>
+    <row r="57" spans="1:17" ht="85" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>41</v>
       </c>
       <c r="B57" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="C57" s="1" t="s">
         <v>359</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>360</v>
       </c>
       <c r="D57" s="1">
         <v>2024</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="F57" s="1" t="s">
         <v>76</v>
       </c>
       <c r="G57" s="9" t="s">
+        <v>361</v>
+      </c>
+      <c r="H57" s="1" t="s">
         <v>362</v>
       </c>
-      <c r="H57" s="1" t="s">
+      <c r="I57" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J57" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K57" s="1" t="s">
         <v>363</v>
       </c>
-      <c r="I57" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="J57" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="K57" s="1" t="s">
+      <c r="L57" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="M57" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="N57" s="1" t="s">
         <v>364</v>
       </c>
-      <c r="L57" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="M57" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="N57" s="1" t="s">
+      <c r="O57" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="P57" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q57" s="1" t="s">
         <v>365</v>
       </c>
-      <c r="O57" s="1" t="s">
-        <v>330</v>
-      </c>
-      <c r="P57" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q57" s="1" t="s">
-        <v>366</v>
-      </c>
-      <c r="R57" s="21"/>
+    </row>
+    <row r="58" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A58" s="1"/>
+      <c r="B58" s="1"/>
+      <c r="C58" s="1"/>
+      <c r="D58" s="1"/>
+      <c r="E58" s="1"/>
+      <c r="F58" s="1"/>
+      <c r="G58" s="9"/>
+      <c r="H58" s="1"/>
+      <c r="I58" s="1"/>
+      <c r="J58" s="1"/>
+      <c r="K58" s="1"/>
+      <c r="L58" s="1"/>
+      <c r="M58" s="1"/>
+      <c r="N58" s="1"/>
+      <c r="O58" s="1"/>
+      <c r="P58" s="1"/>
+      <c r="Q58" s="1"/>
+    </row>
+    <row r="59" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A59" s="1"/>
+      <c r="B59" s="1"/>
+      <c r="C59" s="1"/>
+      <c r="D59" s="1"/>
+      <c r="E59" s="1"/>
+      <c r="F59" s="1"/>
+      <c r="G59" s="9"/>
+      <c r="H59" s="1"/>
+      <c r="I59" s="1"/>
+      <c r="J59" s="1"/>
+      <c r="K59" s="1"/>
+      <c r="L59" s="1"/>
+      <c r="M59" s="1"/>
+      <c r="N59" s="1"/>
+      <c r="O59" s="1"/>
+      <c r="P59" s="1"/>
+      <c r="Q59" s="1"/>
+    </row>
+    <row r="60" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A60" s="1"/>
+      <c r="B60" s="1"/>
+      <c r="C60" s="1"/>
+      <c r="D60" s="1"/>
+      <c r="E60" s="1"/>
+      <c r="F60" s="1"/>
+      <c r="G60" s="9"/>
+      <c r="H60" s="1"/>
+      <c r="I60" s="1"/>
+      <c r="J60" s="1"/>
+      <c r="K60" s="1"/>
+      <c r="L60" s="1"/>
+      <c r="M60" s="1"/>
+      <c r="N60" s="1"/>
+      <c r="O60" s="1"/>
+      <c r="P60" s="1"/>
+      <c r="Q60" s="1"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:Q53 A54:M54 O54:Q54 F55:G55 I55:Q55 A55:D56 F56:Q56 A57:Q1048576">
-    <cfRule type="expression" dxfId="9" priority="5">
+    <cfRule type="expression" dxfId="8" priority="5">
       <formula>$A1="Does not quantify P availability and/or does not manipulate P fertilization"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="6">
+    <cfRule type="expression" dxfId="7" priority="6">
       <formula>$A1="P fertilization experiment that measures photosynthetic traits"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="7">
+    <cfRule type="expression" dxfId="6" priority="7">
       <formula>$A1="P fertilization experiment but does not measure photosynthetic traits"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="8">
+    <cfRule type="expression" dxfId="5" priority="8">
       <formula>$A1="Quantifies P availability"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E55:E56">
-    <cfRule type="expression" dxfId="5" priority="1">
+    <cfRule type="expression" dxfId="4" priority="1">
       <formula>$A55="Does not quantify P availability and/or does not manipulate P fertilization"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="2">
+    <cfRule type="expression" dxfId="3" priority="2">
       <formula>$A55="P fertilization experiment that measures photosynthetic traits"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="3">
+    <cfRule type="expression" dxfId="2" priority="3">
       <formula>$A55="P fertilization experiment but does not measure photosynthetic traits"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="4">
+    <cfRule type="expression" dxfId="1" priority="4">
       <formula>$A55="Quantifies P availability"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Category colors" error="Use the drop down to select one of the 4 potentail color coding categories. Once you select one the row will automatically become colored to fit the &quot;color key&quot;. Thank you! " promptTitle="category" sqref="A1:A1048576" xr:uid="{66CEC525-B843-465C-88B1-968B1C3B8D2D}">
-      <formula1>$T$2:$T$5</formula1>
+      <formula1>$S$2:$S$5</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
@@ -5027,10 +5041,10 @@
   <sheetData>
     <row r="1" spans="1:17" s="10" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
+        <v>366</v>
+      </c>
+      <c r="B1" s="11" t="s">
         <v>367</v>
-      </c>
-      <c r="B1" s="11" t="s">
-        <v>368</v>
       </c>
       <c r="C1" s="11" t="s">
         <v>2</v>
@@ -5673,7 +5687,7 @@
         <v>Singh et al.</v>
       </c>
       <c r="D13" s="2">
-        <v>1999</v>
+        <v>2014</v>
       </c>
       <c r="E13" s="1" t="str">
         <v>Growth, nutrient dynamics, and efficiency responses to carbon dioxide and phosphorus nutrition in soybean</v>
@@ -5782,7 +5796,7 @@
         <v>2017</v>
       </c>
       <c r="E15" s="1" t="str">
-        <v>Nitorgen and phosphorus availabilityies interact to modulate leaf trait scaling relationships across six plant functional types in a controlled-environment study</v>
+        <v>Nitrogen and phosphorus availabilities interact to modulate leaf trait scaling relationships across six plant functional types in a controlled-environment study</v>
       </c>
       <c r="F15" s="2" t="str">
         <v>New Phytologist</v>
@@ -6192,7 +6206,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:17" ht="238" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:17" ht="119" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="str">
         <v>P fertilization experiment that measures photosynthetic traits</v>
       </c>
@@ -6631,7 +6645,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:Q1048576">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>$A1="P fertilization experiment that measures photosynthetic traits"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
add updates from 1/5
</commit_message>
<xml_diff>
--- a/lit_search_np_fert_exps.xlsx
+++ b/lit_search_np_fert_exps.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eaperkowski/git/p_meta/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E318BB6-92B6-D947-BBB5-CDA4FB54BDCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6DF8CBB-95F4-6C4F-B76C-F524445257B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1660" yWindow="500" windowWidth="44880" windowHeight="28300" xr2:uid="{50492CE8-F5C0-524A-968F-FD9EC2022F6C}"/>
+    <workbookView xWindow="6320" yWindow="500" windowWidth="44880" windowHeight="28300" xr2:uid="{50492CE8-F5C0-524A-968F-FD9EC2022F6C}"/>
   </bookViews>
   <sheets>
     <sheet name="all_papers" sheetId="1" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="798" uniqueCount="370">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="809" uniqueCount="373">
   <si>
     <t>category (drop down, auto colors row)</t>
   </si>
@@ -997,10 +997,6 @@
     <t>growth chambers</t>
   </si>
   <si>
-    <t>Three CO2 concentrations (376, 652 and 935 μmol mol-1), and varying pot volumes. 
-old data set unlikely to be avaialbel (paper and website mention nothing about data availablity)</t>
-  </si>
-  <si>
     <t>Interactive effects of temperature and phosphorus nutrition on soybean: leaf photosynthesis, chlorophyll fluorescence, and nutrient efficiency</t>
   </si>
   <si>
@@ -1208,13 +1204,26 @@
   </si>
   <si>
     <t>Nitrogen and phosphorus availabilities interact to modulate leaf trait scaling relationships across six plant functional types in a controlled-environment study</t>
+  </si>
+  <si>
+    <t>Three CO2 concentrations (376, 652 and 935 μmol mol-1), and varying pot volumes. 
+old data set unlikely to be available (paper and website mention nothing about data availablity)</t>
+  </si>
+  <si>
+    <t>Narea, Parea, leaf N:P, Amax, gsw, Vcmax, J, TPU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P added at four concentrations as equimolar K2HPO4 and KH2PO4: 0, 0.005, 0.02, 0.1 mM P) </t>
+  </si>
+  <si>
+    <t>n; treatment mean and standard errors in text</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1275,13 +1284,6 @@
     </font>
     <font>
       <sz val="12"/>
-      <color rgb="FFFFC000"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
       <color rgb="FFFF0000"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
@@ -1294,32 +1296,6 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Aptos Narrow"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color rgb="FFFF0000"/>
-      <name val="Aptos Narrow"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <u/>
-      <sz val="12"/>
-      <color rgb="FFFF0000"/>
-      <name val="Aptos Narrow"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Aptos Narrow"/>
     </font>
     <font>
       <b/>
@@ -1343,6 +1319,43 @@
       <color theme="10"/>
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow (Body)"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow (Body)"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow (Body)"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
     </font>
   </fonts>
   <fills count="7">
@@ -1411,7 +1424,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1452,43 +1465,49 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2086,10 +2105,10 @@
   <dimension ref="A1:S60"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B36" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B38" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K41" sqref="K41"/>
+      <selection pane="bottomRight" activeCell="G42" sqref="G42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2509,55 +2528,55 @@
       <c r="P8" s="1"/>
     </row>
     <row r="9" spans="1:19" ht="136" x14ac:dyDescent="0.2">
-      <c r="A9" s="24" t="s">
+      <c r="A9" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="B9" s="24" t="s">
+      <c r="B9" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="24" t="s">
+      <c r="C9" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="D9" s="24">
+      <c r="D9" s="18">
         <v>2022</v>
       </c>
-      <c r="E9" s="24" t="s">
+      <c r="E9" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="F9" s="24" t="s">
+      <c r="F9" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="G9" s="25" t="s">
+      <c r="G9" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="H9" s="24" t="s">
+      <c r="H9" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="I9" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="J9" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="K9" s="24" t="s">
+      <c r="I9" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="J9" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="K9" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="L9" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="M9" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="N9" s="24" t="s">
+      <c r="L9" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="M9" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="N9" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="O9" s="24" t="s">
+      <c r="O9" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="P9" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q9" s="24"/>
+      <c r="P9" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q9" s="18"/>
     </row>
     <row r="10" spans="1:19" ht="119" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
@@ -3508,53 +3527,53 @@
       <c r="Q29" s="1"/>
     </row>
     <row r="30" spans="1:17" ht="119" x14ac:dyDescent="0.2">
-      <c r="A30" s="24" t="s">
+      <c r="A30" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="B30" s="24" t="s">
+      <c r="B30" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="C30" s="24" t="s">
+      <c r="C30" s="18" t="s">
         <v>184</v>
       </c>
-      <c r="D30" s="24">
+      <c r="D30" s="18">
         <v>2021</v>
       </c>
-      <c r="E30" s="24" t="s">
+      <c r="E30" s="18" t="s">
         <v>185</v>
       </c>
-      <c r="F30" s="24" t="s">
+      <c r="F30" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="G30" s="25" t="s">
+      <c r="G30" s="19" t="s">
         <v>186</v>
       </c>
-      <c r="H30" s="24" t="s">
+      <c r="H30" s="18" t="s">
         <v>187</v>
       </c>
-      <c r="I30" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="J30" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="K30" s="24" t="s">
+      <c r="I30" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="J30" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="K30" s="18" t="s">
         <v>188</v>
       </c>
-      <c r="L30" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="M30" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="N30" s="24" t="s">
+      <c r="L30" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="M30" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="N30" s="18" t="s">
         <v>189</v>
       </c>
-      <c r="O30" s="24"/>
-      <c r="P30" s="24" t="s">
+      <c r="O30" s="18"/>
+      <c r="P30" s="18" t="s">
         <v>190</v>
       </c>
-      <c r="Q30" s="24" t="s">
+      <c r="Q30" s="18" t="s">
         <v>191</v>
       </c>
     </row>
@@ -3894,53 +3913,53 @@
       </c>
     </row>
     <row r="38" spans="1:17" ht="119" x14ac:dyDescent="0.2">
-      <c r="A38" s="24" t="s">
+      <c r="A38" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="B38" s="24" t="s">
+      <c r="B38" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="C38" s="24" t="s">
+      <c r="C38" s="18" t="s">
         <v>238</v>
       </c>
-      <c r="D38" s="24">
+      <c r="D38" s="18">
         <v>2017</v>
       </c>
-      <c r="E38" s="24" t="s">
-        <v>369</v>
-      </c>
-      <c r="F38" s="24" t="s">
+      <c r="E38" s="18" t="s">
+        <v>368</v>
+      </c>
+      <c r="F38" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="G38" s="25" t="s">
+      <c r="G38" s="19" t="s">
         <v>239</v>
       </c>
-      <c r="H38" s="24" t="s">
+      <c r="H38" s="18" t="s">
         <v>240</v>
       </c>
-      <c r="I38" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="J38" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="K38" s="24" t="s">
+      <c r="I38" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="J38" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="K38" s="18" t="s">
         <v>241</v>
       </c>
-      <c r="L38" s="24" t="s">
-        <v>25</v>
-      </c>
-      <c r="M38" s="24" t="s">
-        <v>25</v>
-      </c>
-      <c r="N38" s="24" t="s">
+      <c r="L38" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="M38" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="N38" s="18" t="s">
         <v>242</v>
       </c>
-      <c r="O38" s="24"/>
-      <c r="P38" s="24" t="s">
+      <c r="O38" s="18"/>
+      <c r="P38" s="18" t="s">
         <v>243</v>
       </c>
-      <c r="Q38" s="24"/>
+      <c r="Q38" s="18"/>
     </row>
     <row r="39" spans="1:17" ht="102" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
@@ -4033,104 +4052,104 @@
       <c r="Q40" s="1"/>
     </row>
     <row r="41" spans="1:17" ht="102" x14ac:dyDescent="0.2">
-      <c r="A41" s="1" t="s">
+      <c r="A41" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="B41" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="C41" s="1" t="s">
+      <c r="C41" s="18" t="s">
         <v>255</v>
       </c>
-      <c r="D41" s="1">
+      <c r="D41" s="18">
         <v>2007</v>
       </c>
-      <c r="E41" s="1" t="s">
+      <c r="E41" s="18" t="s">
         <v>256</v>
       </c>
-      <c r="F41" s="1" t="s">
+      <c r="F41" s="18" t="s">
         <v>257</v>
       </c>
-      <c r="G41" s="3" t="s">
+      <c r="G41" s="19" t="s">
         <v>258</v>
       </c>
-      <c r="H41" s="1" t="s">
+      <c r="H41" s="18" t="s">
         <v>259</v>
       </c>
-      <c r="I41" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="J41" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="K41" s="1" t="s">
+      <c r="I41" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="J41" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="K41" s="18" t="s">
         <v>260</v>
       </c>
-      <c r="L41" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="M41" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="N41" s="1" t="s">
+      <c r="L41" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="M41" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="N41" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="O41" s="1"/>
-      <c r="P41" s="1" t="s">
+      <c r="O41" s="18"/>
+      <c r="P41" s="18" t="s">
         <v>261</v>
       </c>
-      <c r="Q41" s="1" t="s">
+      <c r="Q41" s="18" t="s">
         <v>262</v>
       </c>
     </row>
     <row r="42" spans="1:17" ht="119" x14ac:dyDescent="0.2">
-      <c r="A42" s="1" t="s">
+      <c r="A42" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="B42" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="C42" s="1" t="s">
+      <c r="C42" s="18" t="s">
         <v>263</v>
       </c>
-      <c r="D42" s="1">
+      <c r="D42" s="18">
         <v>2005</v>
       </c>
-      <c r="E42" s="1" t="s">
+      <c r="E42" s="18" t="s">
         <v>264</v>
       </c>
-      <c r="F42" s="1" t="s">
+      <c r="F42" s="18" t="s">
         <v>265</v>
       </c>
-      <c r="G42" s="3" t="s">
+      <c r="G42" s="19" t="s">
         <v>266</v>
       </c>
-      <c r="H42" s="1" t="s">
+      <c r="H42" s="18" t="s">
         <v>267</v>
       </c>
-      <c r="I42" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="J42" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="K42" s="1" t="s">
+      <c r="I42" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="J42" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="K42" s="18" t="s">
         <v>268</v>
       </c>
-      <c r="L42" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="M42" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="N42" s="1" t="s">
+      <c r="L42" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="M42" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="N42" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="O42" s="1"/>
-      <c r="P42" s="1" t="s">
+      <c r="O42" s="18"/>
+      <c r="P42" s="18" t="s">
         <v>261</v>
       </c>
-      <c r="Q42" s="1" t="s">
+      <c r="Q42" s="18" t="s">
         <v>262</v>
       </c>
     </row>
@@ -4183,105 +4202,105 @@
         <v>274</v>
       </c>
     </row>
-    <row r="44" spans="1:17" s="17" customFormat="1" ht="102" x14ac:dyDescent="0.2">
-      <c r="A44" s="14" t="s">
+    <row r="44" spans="1:17" s="15" customFormat="1" ht="102" x14ac:dyDescent="0.2">
+      <c r="A44" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="B44" s="14" t="s">
+      <c r="B44" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="C44" s="14" t="s">
+      <c r="C44" s="18" t="s">
         <v>269</v>
       </c>
-      <c r="D44" s="14">
+      <c r="D44" s="18">
         <v>2002</v>
       </c>
-      <c r="E44" s="14" t="s">
+      <c r="E44" s="18" t="s">
         <v>270</v>
       </c>
-      <c r="F44" s="14" t="s">
+      <c r="F44" s="18" t="s">
         <v>257</v>
       </c>
-      <c r="G44" s="16" t="s">
+      <c r="G44" s="20" t="s">
         <v>271</v>
       </c>
-      <c r="H44" s="14" t="s">
+      <c r="H44" s="18" t="s">
         <v>272</v>
       </c>
-      <c r="I44" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="J44" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="K44" s="14" t="s">
+      <c r="I44" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="J44" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="K44" s="18" t="s">
         <v>275</v>
       </c>
-      <c r="L44" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="M44" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="N44" s="14" t="s">
+      <c r="L44" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="M44" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="N44" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="O44" s="14"/>
-      <c r="P44" s="14" t="s">
+      <c r="O44" s="18"/>
+      <c r="P44" s="18" t="s">
         <v>276</v>
       </c>
-      <c r="Q44" s="14" t="s">
+      <c r="Q44" s="18" t="s">
         <v>277</v>
       </c>
     </row>
     <row r="45" spans="1:17" s="12" customFormat="1" ht="119" x14ac:dyDescent="0.2">
-      <c r="A45" s="22" t="s">
+      <c r="A45" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="B45" s="22" t="s">
+      <c r="B45" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="C45" s="22" t="s">
+      <c r="C45" s="16" t="s">
         <v>184</v>
       </c>
-      <c r="D45" s="22">
+      <c r="D45" s="16">
         <v>2019</v>
       </c>
-      <c r="E45" s="22" t="s">
+      <c r="E45" s="16" t="s">
         <v>278</v>
       </c>
-      <c r="F45" s="22" t="s">
+      <c r="F45" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="G45" s="23" t="s">
+      <c r="G45" s="17" t="s">
         <v>279</v>
       </c>
-      <c r="H45" s="22" t="s">
+      <c r="H45" s="16" t="s">
         <v>280</v>
       </c>
-      <c r="I45" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="J45" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="K45" s="22" t="s">
+      <c r="I45" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="J45" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="K45" s="16" t="s">
         <v>281</v>
       </c>
-      <c r="L45" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="M45" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="N45" s="22" t="s">
+      <c r="L45" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="M45" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="N45" s="16" t="s">
         <v>282</v>
       </c>
-      <c r="O45" s="22"/>
-      <c r="P45" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q45" s="22" t="s">
+      <c r="O45" s="16"/>
+      <c r="P45" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q45" s="16" t="s">
         <v>283</v>
       </c>
     </row>
@@ -4335,105 +4354,107 @@
       </c>
     </row>
     <row r="47" spans="1:17" ht="119" x14ac:dyDescent="0.2">
-      <c r="A47" s="14" t="s">
+      <c r="A47" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="B47" s="14" t="s">
+      <c r="B47" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="C47" s="14" t="s">
+      <c r="C47" s="13" t="s">
         <v>291</v>
       </c>
-      <c r="D47" s="14">
+      <c r="D47" s="13">
         <v>1989</v>
       </c>
-      <c r="E47" s="14" t="s">
+      <c r="E47" s="13" t="s">
         <v>292</v>
       </c>
-      <c r="F47" s="14" t="s">
+      <c r="F47" s="13" t="s">
         <v>225</v>
       </c>
-      <c r="G47" s="16" t="s">
+      <c r="G47" s="14" t="s">
         <v>293</v>
       </c>
-      <c r="H47" s="14" t="s">
+      <c r="H47" s="13" t="s">
         <v>294</v>
       </c>
-      <c r="I47" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="J47" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="K47" s="14" t="s">
+      <c r="I47" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="J47" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="K47" s="13" t="s">
         <v>295</v>
       </c>
-      <c r="L47" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="M47" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="N47" s="14" t="s">
+      <c r="L47" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="M47" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="N47" s="13" t="s">
         <v>26</v>
       </c>
       <c r="O47" s="1"/>
-      <c r="P47" s="14" t="s">
+      <c r="P47" s="13" t="s">
         <v>222</v>
       </c>
       <c r="Q47" s="1"/>
     </row>
-    <row r="48" spans="1:17" s="17" customFormat="1" ht="153" x14ac:dyDescent="0.2">
-      <c r="A48" s="14" t="s">
+    <row r="48" spans="1:17" s="15" customFormat="1" ht="153" x14ac:dyDescent="0.2">
+      <c r="A48" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="B48" s="14" t="s">
+      <c r="B48" s="13" t="s">
         <v>296</v>
       </c>
-      <c r="C48" s="14" t="s">
+      <c r="C48" s="13" t="s">
         <v>297</v>
       </c>
-      <c r="D48" s="14">
+      <c r="D48" s="13">
         <v>1995</v>
       </c>
-      <c r="E48" s="14" t="s">
+      <c r="E48" s="13" t="s">
         <v>298</v>
       </c>
-      <c r="F48" s="14" t="s">
+      <c r="F48" s="13" t="s">
         <v>299</v>
       </c>
-      <c r="G48" s="16" t="s">
+      <c r="G48" s="14" t="s">
         <v>300</v>
       </c>
-      <c r="H48" s="14" t="s">
+      <c r="H48" s="13" t="s">
         <v>301</v>
       </c>
-      <c r="I48" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="J48" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="K48" s="14" t="s">
+      <c r="I48" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="J48" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="K48" s="13" t="s">
         <v>302</v>
       </c>
-      <c r="L48" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="M48" s="14"/>
-      <c r="N48" s="14"/>
-      <c r="O48" s="14" t="s">
+      <c r="L48" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="M48" s="13"/>
+      <c r="N48" s="13"/>
+      <c r="O48" s="13" t="s">
         <v>303</v>
       </c>
-      <c r="P48" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q48" s="14" t="s">
-        <v>304</v>
+      <c r="P48" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q48" s="13" t="s">
+        <v>369</v>
       </c>
     </row>
     <row r="49" spans="1:17" ht="119" x14ac:dyDescent="0.2">
-      <c r="A49" s="1"/>
+      <c r="A49" s="1" t="s">
+        <v>41</v>
+      </c>
       <c r="B49" s="1" t="s">
         <v>19</v>
       </c>
@@ -4444,13 +4465,13 @@
         <v>2019</v>
       </c>
       <c r="E49" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="F49" s="1" t="s">
         <v>305</v>
       </c>
-      <c r="F49" s="1" t="s">
+      <c r="G49" s="3" t="s">
         <v>306</v>
-      </c>
-      <c r="G49" s="3" t="s">
-        <v>307</v>
       </c>
       <c r="H49" s="1"/>
       <c r="I49" s="1"/>
@@ -4463,398 +4484,418 @@
       <c r="P49" s="1"/>
       <c r="Q49" s="1"/>
     </row>
-    <row r="50" spans="1:17" ht="68" x14ac:dyDescent="0.2">
-      <c r="A50" s="1"/>
-      <c r="B50" s="1" t="s">
+    <row r="50" spans="1:17" ht="85" x14ac:dyDescent="0.2">
+      <c r="A50" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="B50" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="C50" s="1" t="s">
+      <c r="C50" s="18" t="s">
         <v>269</v>
       </c>
-      <c r="D50" s="1">
+      <c r="D50" s="18">
         <v>2011</v>
       </c>
-      <c r="E50" s="1" t="s">
+      <c r="E50" s="18" t="s">
+        <v>307</v>
+      </c>
+      <c r="F50" s="18" t="s">
+        <v>257</v>
+      </c>
+      <c r="G50" s="19" t="s">
         <v>308</v>
       </c>
-      <c r="F50" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="G50" s="3" t="s">
+      <c r="H50" s="21" t="s">
+        <v>370</v>
+      </c>
+      <c r="I50" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="J50" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="K50" s="21" t="s">
+        <v>371</v>
+      </c>
+      <c r="L50" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="M50" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="N50" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="O50" s="10" t="s">
+        <v>355</v>
+      </c>
+      <c r="P50" s="10" t="s">
+        <v>372</v>
+      </c>
+      <c r="Q50" s="18"/>
+    </row>
+    <row r="51" spans="1:17" s="15" customFormat="1" ht="153" x14ac:dyDescent="0.2">
+      <c r="A51" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="B51" s="18" t="s">
         <v>309</v>
       </c>
-      <c r="H50" s="1"/>
-      <c r="I50" s="1"/>
-      <c r="J50" s="1"/>
-      <c r="K50" s="1"/>
-      <c r="L50" s="1"/>
-      <c r="M50" s="1"/>
-      <c r="N50" s="1"/>
-      <c r="O50" s="1"/>
-      <c r="P50" s="1"/>
-      <c r="Q50" s="1"/>
-    </row>
-    <row r="51" spans="1:17" s="17" customFormat="1" ht="153" x14ac:dyDescent="0.2">
-      <c r="A51" s="19" t="s">
+      <c r="C51" s="18" t="s">
+        <v>310</v>
+      </c>
+      <c r="D51" s="18">
+        <v>2022</v>
+      </c>
+      <c r="E51" s="18" t="s">
+        <v>311</v>
+      </c>
+      <c r="F51" s="18" t="s">
+        <v>312</v>
+      </c>
+      <c r="G51" s="20" t="s">
+        <v>313</v>
+      </c>
+      <c r="H51" s="18" t="s">
+        <v>314</v>
+      </c>
+      <c r="I51" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="J51" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="K51" s="18" t="s">
+        <v>315</v>
+      </c>
+      <c r="L51" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="M51" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="N51" s="18"/>
+      <c r="O51" s="18"/>
+      <c r="P51" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q51" s="18" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="52" spans="1:17" ht="102" x14ac:dyDescent="0.2">
+      <c r="A52" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="B51" s="19" t="s">
-        <v>310</v>
-      </c>
-      <c r="C51" s="19" t="s">
-        <v>311</v>
-      </c>
-      <c r="D51" s="19">
+      <c r="B52" s="25" t="s">
+        <v>296</v>
+      </c>
+      <c r="C52" s="25" t="s">
+        <v>316</v>
+      </c>
+      <c r="D52" s="25">
+        <v>2014</v>
+      </c>
+      <c r="E52" s="25" t="s">
+        <v>317</v>
+      </c>
+      <c r="F52" s="25" t="s">
+        <v>165</v>
+      </c>
+      <c r="G52" s="26" t="s">
+        <v>318</v>
+      </c>
+      <c r="H52" s="25" t="s">
+        <v>319</v>
+      </c>
+      <c r="I52" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="J52" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="K52" s="25" t="s">
+        <v>320</v>
+      </c>
+      <c r="L52" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="M52" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="N52" s="25" t="s">
+        <v>321</v>
+      </c>
+      <c r="O52" s="25" t="s">
+        <v>303</v>
+      </c>
+      <c r="P52" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q52" s="25"/>
+    </row>
+    <row r="53" spans="1:17" s="15" customFormat="1" ht="187" x14ac:dyDescent="0.2">
+      <c r="A53" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="B53" s="25" t="s">
+        <v>296</v>
+      </c>
+      <c r="C53" s="25" t="s">
+        <v>322</v>
+      </c>
+      <c r="D53" s="25">
         <v>2022</v>
       </c>
-      <c r="E51" s="19" t="s">
-        <v>312</v>
-      </c>
-      <c r="F51" s="19" t="s">
-        <v>313</v>
-      </c>
-      <c r="G51" s="26" t="s">
-        <v>314</v>
-      </c>
-      <c r="H51" s="19" t="s">
-        <v>315</v>
-      </c>
-      <c r="I51" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="J51" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="K51" s="19" t="s">
-        <v>316</v>
-      </c>
-      <c r="L51" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="M51" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="N51" s="19"/>
-      <c r="O51" s="19"/>
-      <c r="P51" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q51" s="19" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="52" spans="1:17" ht="102" x14ac:dyDescent="0.2">
-      <c r="A52" s="14" t="s">
+      <c r="E53" s="25" t="s">
+        <v>323</v>
+      </c>
+      <c r="F53" s="25" t="s">
+        <v>305</v>
+      </c>
+      <c r="G53" s="26" t="s">
+        <v>324</v>
+      </c>
+      <c r="H53" s="25" t="s">
+        <v>325</v>
+      </c>
+      <c r="I53" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="J53" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="K53" s="25" t="s">
+        <v>326</v>
+      </c>
+      <c r="L53" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="M53" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="N53" s="25" t="s">
+        <v>327</v>
+      </c>
+      <c r="O53" s="25" t="s">
+        <v>328</v>
+      </c>
+      <c r="P53" s="25" t="s">
+        <v>329</v>
+      </c>
+      <c r="Q53" s="25" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="54" spans="1:17" s="15" customFormat="1" ht="306" x14ac:dyDescent="0.2">
+      <c r="A54" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="B52" s="14" t="s">
-        <v>296</v>
-      </c>
-      <c r="C52" s="14" t="s">
-        <v>317</v>
-      </c>
-      <c r="D52" s="14">
-        <v>2014</v>
-      </c>
-      <c r="E52" s="14" t="s">
-        <v>318</v>
-      </c>
-      <c r="F52" s="14" t="s">
-        <v>165</v>
-      </c>
-      <c r="G52" s="15" t="s">
-        <v>319</v>
-      </c>
-      <c r="H52" s="14" t="s">
-        <v>320</v>
-      </c>
-      <c r="I52" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="J52" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="K52" s="14" t="s">
-        <v>321</v>
-      </c>
-      <c r="L52" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="M52" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="N52" s="14" t="s">
-        <v>322</v>
-      </c>
-      <c r="O52" s="14" t="s">
-        <v>303</v>
-      </c>
-      <c r="P52" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q52" s="13"/>
-    </row>
-    <row r="53" spans="1:17" s="17" customFormat="1" ht="187" x14ac:dyDescent="0.2">
-      <c r="A53" s="14" t="s">
+      <c r="B54" s="25" t="s">
+        <v>309</v>
+      </c>
+      <c r="C54" s="25" t="s">
+        <v>331</v>
+      </c>
+      <c r="D54" s="25">
+        <v>2024</v>
+      </c>
+      <c r="E54" s="25" t="s">
+        <v>332</v>
+      </c>
+      <c r="F54" s="25" t="s">
+        <v>333</v>
+      </c>
+      <c r="G54" s="26" t="s">
+        <v>334</v>
+      </c>
+      <c r="H54" s="25" t="s">
+        <v>335</v>
+      </c>
+      <c r="I54" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="J54" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="K54" s="25" t="s">
+        <v>336</v>
+      </c>
+      <c r="L54" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="M54" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="N54" s="27" t="s">
+        <v>337</v>
+      </c>
+      <c r="O54" s="25" t="s">
+        <v>328</v>
+      </c>
+      <c r="P54" s="25" t="s">
+        <v>338</v>
+      </c>
+      <c r="Q54" s="25" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="55" spans="1:17" s="15" customFormat="1" ht="113.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="B53" s="14" t="s">
-        <v>296</v>
-      </c>
-      <c r="C53" s="14" t="s">
-        <v>323</v>
-      </c>
-      <c r="D53" s="14">
-        <v>2022</v>
-      </c>
-      <c r="E53" s="14" t="s">
-        <v>324</v>
-      </c>
-      <c r="F53" s="14" t="s">
-        <v>306</v>
-      </c>
-      <c r="G53" s="15" t="s">
-        <v>325</v>
-      </c>
-      <c r="H53" s="14" t="s">
-        <v>326</v>
-      </c>
-      <c r="I53" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="J53" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="K53" s="14" t="s">
-        <v>327</v>
-      </c>
-      <c r="L53" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="M53" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="N53" s="14" t="s">
+      <c r="B55" s="22" t="s">
+        <v>309</v>
+      </c>
+      <c r="C55" s="22" t="s">
+        <v>340</v>
+      </c>
+      <c r="D55" s="22">
+        <v>2023</v>
+      </c>
+      <c r="E55" s="22" t="s">
+        <v>341</v>
+      </c>
+      <c r="F55" s="22" t="s">
+        <v>342</v>
+      </c>
+      <c r="G55" s="23" t="s">
+        <v>343</v>
+      </c>
+      <c r="H55" s="24" t="s">
+        <v>344</v>
+      </c>
+      <c r="I55" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="J55" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="K55" s="22"/>
+      <c r="L55" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="M55" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="N55" s="22" t="s">
+        <v>345</v>
+      </c>
+      <c r="O55" s="22" t="s">
         <v>328</v>
       </c>
-      <c r="O53" s="14" t="s">
-        <v>329</v>
-      </c>
-      <c r="P53" s="14" t="s">
-        <v>330</v>
-      </c>
-      <c r="Q53" s="14" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="54" spans="1:17" s="17" customFormat="1" ht="306" x14ac:dyDescent="0.2">
-      <c r="A54" s="14" t="s">
+      <c r="P55" s="22" t="s">
+        <v>346</v>
+      </c>
+      <c r="Q55" s="22" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="56" spans="1:17" ht="85" x14ac:dyDescent="0.2">
+      <c r="A56" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="B54" s="14" t="s">
-        <v>310</v>
-      </c>
-      <c r="C54" s="14" t="s">
-        <v>332</v>
-      </c>
-      <c r="D54" s="14">
+      <c r="B56" s="25" t="s">
+        <v>348</v>
+      </c>
+      <c r="C56" s="25" t="s">
+        <v>349</v>
+      </c>
+      <c r="D56" s="25">
+        <v>2020</v>
+      </c>
+      <c r="E56" s="25" t="s">
+        <v>350</v>
+      </c>
+      <c r="F56" s="25" t="s">
+        <v>250</v>
+      </c>
+      <c r="G56" s="26" t="s">
+        <v>351</v>
+      </c>
+      <c r="H56" s="25" t="s">
+        <v>352</v>
+      </c>
+      <c r="I56" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="J56" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="K56" s="25" t="s">
+        <v>353</v>
+      </c>
+      <c r="L56" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="M56" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="N56" s="25" t="s">
+        <v>354</v>
+      </c>
+      <c r="O56" s="25" t="s">
+        <v>355</v>
+      </c>
+      <c r="P56" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q56" s="25" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="57" spans="1:17" ht="102" x14ac:dyDescent="0.2">
+      <c r="A57" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="B57" s="18" t="s">
+        <v>357</v>
+      </c>
+      <c r="C57" s="18" t="s">
+        <v>358</v>
+      </c>
+      <c r="D57" s="18">
         <v>2024</v>
       </c>
-      <c r="E54" s="14" t="s">
-        <v>333</v>
-      </c>
-      <c r="F54" s="14" t="s">
-        <v>334</v>
-      </c>
-      <c r="G54" s="15" t="s">
-        <v>335</v>
-      </c>
-      <c r="H54" s="14" t="s">
-        <v>336</v>
-      </c>
-      <c r="I54" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="J54" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="K54" s="14" t="s">
-        <v>337</v>
-      </c>
-      <c r="L54" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="M54" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="N54" s="18" t="s">
-        <v>338</v>
-      </c>
-      <c r="O54" s="14" t="s">
-        <v>329</v>
-      </c>
-      <c r="P54" s="14" t="s">
-        <v>339</v>
-      </c>
-      <c r="Q54" s="14" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="55" spans="1:17" s="17" customFormat="1" ht="113.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="19" t="s">
-        <v>41</v>
-      </c>
-      <c r="B55" s="19" t="s">
-        <v>310</v>
-      </c>
-      <c r="C55" s="19" t="s">
-        <v>341</v>
-      </c>
-      <c r="D55" s="19">
-        <v>2023</v>
-      </c>
-      <c r="E55" s="19" t="s">
-        <v>342</v>
-      </c>
-      <c r="F55" s="19" t="s">
-        <v>343</v>
-      </c>
-      <c r="G55" s="20" t="s">
-        <v>344</v>
-      </c>
-      <c r="H55" s="21" t="s">
-        <v>345</v>
-      </c>
-      <c r="I55" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="J55" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="K55" s="19"/>
-      <c r="L55" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="M55" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="N55" s="19" t="s">
-        <v>346</v>
-      </c>
-      <c r="O55" s="19" t="s">
-        <v>329</v>
-      </c>
-      <c r="P55" s="19" t="s">
-        <v>347</v>
-      </c>
-      <c r="Q55" s="19" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="56" spans="1:17" ht="85" x14ac:dyDescent="0.2">
-      <c r="A56" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>349</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>350</v>
-      </c>
-      <c r="D56" s="1">
-        <v>2020</v>
-      </c>
-      <c r="E56" s="1" t="s">
-        <v>351</v>
-      </c>
-      <c r="F56" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="G56" s="9" t="s">
-        <v>352</v>
-      </c>
-      <c r="H56" s="1" t="s">
-        <v>353</v>
-      </c>
-      <c r="I56" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="J56" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="K56" s="1" t="s">
-        <v>354</v>
-      </c>
-      <c r="L56" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="M56" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="N56" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="O56" s="1" t="s">
-        <v>356</v>
-      </c>
-      <c r="P56" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q56" s="1" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="57" spans="1:17" ht="85" x14ac:dyDescent="0.2">
-      <c r="A57" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B57" s="1" t="s">
-        <v>358</v>
-      </c>
-      <c r="C57" s="1" t="s">
+      <c r="E57" s="18" t="s">
         <v>359</v>
       </c>
-      <c r="D57" s="1">
-        <v>2024</v>
-      </c>
-      <c r="E57" s="1" t="s">
+      <c r="F57" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="G57" s="28" t="s">
         <v>360</v>
       </c>
-      <c r="F57" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="G57" s="9" t="s">
+      <c r="H57" s="18" t="s">
         <v>361</v>
       </c>
-      <c r="H57" s="1" t="s">
+      <c r="I57" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="J57" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="K57" s="18" t="s">
         <v>362</v>
       </c>
-      <c r="I57" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="J57" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="K57" s="1" t="s">
+      <c r="L57" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="M57" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="N57" s="18" t="s">
         <v>363</v>
       </c>
-      <c r="L57" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="M57" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="N57" s="1" t="s">
+      <c r="O57" s="18" t="s">
+        <v>328</v>
+      </c>
+      <c r="P57" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q57" s="18" t="s">
         <v>364</v>
-      </c>
-      <c r="O57" s="1" t="s">
-        <v>329</v>
-      </c>
-      <c r="P57" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q57" s="1" t="s">
-        <v>365</v>
       </c>
     </row>
     <row r="58" spans="1:17" x14ac:dyDescent="0.2">
@@ -4915,7 +4956,7 @@
       <c r="Q60" s="1"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:Q53 A54:M54 O54:Q54 F55:G55 I55:Q55 A55:D56 F56:Q56 A57:Q1048576">
+  <conditionalFormatting sqref="A1:Q49 A50:G50 J50 L50:Q50 A51:Q53 A54:M54 O54:Q54 F55:G55 I55:Q55 A55:D56 F56:Q56 A57:Q1048576">
     <cfRule type="expression" dxfId="8" priority="5">
       <formula>$A1="Does not quantify P availability and/or does not manipulate P fertilization"</formula>
     </cfRule>
@@ -5014,7 +5055,7 @@
   <sheetPr>
     <tabColor theme="9" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:Q30"/>
+  <dimension ref="A1:Q32"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -5041,10 +5082,10 @@
   <sheetData>
     <row r="1" spans="1:17" s="10" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
+        <v>365</v>
+      </c>
+      <c r="B1" s="11" t="s">
         <v>366</v>
-      </c>
-      <c r="B1" s="11" t="s">
-        <v>367</v>
       </c>
       <c r="C1" s="11" t="s">
         <v>2</v>
@@ -5094,7 +5135,7 @@
     </row>
     <row r="2" spans="1:17" ht="85" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="str" cm="1">
-        <f t="array" ref="A2:Q30">_xlfn._xlws.FILTER(all_papers!A:Q, all_papers!A:A = "P fertilization experiment that measures photosynthetic traits")</f>
+        <f t="array" ref="A2:Q32">_xlfn._xlws.FILTER(all_papers!A:Q, all_papers!A:A = "P fertilization experiment that measures photosynthetic traits")</f>
         <v>P fertilization experiment that measures photosynthetic traits</v>
       </c>
       <c r="B2" s="2" t="str">
@@ -6257,48 +6298,48 @@
       </c>
       <c r="Q23" s="1" t="str">
         <v>Three CO2 concentrations (376, 652 and 935 μmol mol-1), and varying pot volumes. 
-old data set unlikely to be avaialbel (paper and website mention nothing about data availablity)</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17" ht="153" x14ac:dyDescent="0.2">
+old data set unlikely to be available (paper and website mention nothing about data availablity)</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" ht="85" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="str">
         <v>P fertilization experiment that measures photosynthetic traits</v>
       </c>
       <c r="B24" s="1" t="str">
-        <v>Huiying</v>
+        <v>evan</v>
       </c>
       <c r="C24" s="1" t="str">
-        <v>Yu et al.</v>
+        <v>Singh et al.</v>
       </c>
       <c r="D24" s="1">
-        <v>2022</v>
+        <v>2019</v>
       </c>
       <c r="E24" s="1" t="str">
-        <v>Foliar phosphorus allocation and photosynthesis reveal plants' adaptative strategies to phosphorus limitation in tropical forests at different successional stages</v>
+        <v>Interactive effects of temperature and phosphorus nutrition on soybean: leaf photosynthesis, chlorophyll fluorescence, and nutrient efficiency</v>
       </c>
       <c r="F24" s="1" t="str">
-        <v>Science of Total Environment</v>
+        <v>Photosynthetica</v>
       </c>
       <c r="G24" s="1" t="str">
-        <v>https://doi.org/10.1016/j.scitotenv.2022.157456</v>
-      </c>
-      <c r="H24" s="1" t="str">
-        <v>Amax, gsw, chlorophyll content, LA, LT, LDMC, SLA, PNUE, PPUE, leaf C, N &amp; P, leaf P allocated to four parts</v>
-      </c>
-      <c r="I24" s="1" t="str">
-        <v>y</v>
-      </c>
-      <c r="J24" s="1" t="str">
-        <v>y</v>
-      </c>
-      <c r="K24" s="1" t="str">
-        <v>N addition (N50, 50 kg N ha−1 yr−1), P addition (P50, 50 kg P ha−1 yr−1), and NP addition (N50P50, 50 kg N ha−1 yr−1 + 50 kg P ha−1 yr−1). N and P were added in the forms of NH4NO3 and Ca(H2PO4)2 dissolved in 30 L of water</v>
-      </c>
-      <c r="L24" s="1" t="str">
-        <v>y</v>
-      </c>
-      <c r="M24" s="1" t="str">
-        <v>y</v>
+        <v>10.32615/ps.2019.036</v>
+      </c>
+      <c r="H24" s="1">
+        <v>0</v>
+      </c>
+      <c r="I24" s="1">
+        <v>0</v>
+      </c>
+      <c r="J24" s="1">
+        <v>0</v>
+      </c>
+      <c r="K24" s="1">
+        <v>0</v>
+      </c>
+      <c r="L24" s="1">
+        <v>0</v>
+      </c>
+      <c r="M24" s="1">
+        <v>0</v>
       </c>
       <c r="N24" s="1">
         <v>0</v>
@@ -6306,37 +6347,37 @@
       <c r="O24" s="1">
         <v>0</v>
       </c>
-      <c r="P24" s="1" t="str">
-        <v>y</v>
-      </c>
-      <c r="Q24" s="1" t="str">
-        <v>Data will be made available on request; leaf nutrient data are extractable from Table 2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17" ht="85" x14ac:dyDescent="0.2">
+      <c r="P24" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q24" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" ht="119" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="str">
         <v>P fertilization experiment that measures photosynthetic traits</v>
       </c>
       <c r="B25" s="1" t="str">
-        <v>monika</v>
+        <v>evan</v>
       </c>
       <c r="C25" s="1" t="str">
-        <v>Cheng et al.</v>
+        <v>Warren &amp; Adams</v>
       </c>
       <c r="D25" s="1">
-        <v>2014</v>
+        <v>2011</v>
       </c>
       <c r="E25" s="1" t="str">
-        <v>Interactions between light intensity and phosphorus nutrition affect the phosphate-mining capacity of white lupin (Lupinus albus L.)</v>
+        <v>How does P affect photosynthesis and metabolite profiles of Eucalyptus globulus?</v>
       </c>
       <c r="F25" s="1" t="str">
-        <v>Journal of Experimental Botany</v>
+        <v>Tree Physiology</v>
       </c>
       <c r="G25" s="1" t="str">
-        <v>https://doi.org/10.1093/jxb/eru135</v>
+        <v>https://doi.org/10.1093/treephys/tpr064</v>
       </c>
       <c r="H25" s="1" t="str">
-        <v>Cluster roots, root length &amp; surface area, Net photosynthetic rate (Pn), P concentraiton of roots and shoots, root exudates, RNA</v>
+        <v>Narea, Parea, leaf N:P, Amax, gsw, Vcmax, J, TPU</v>
       </c>
       <c r="I25" s="1" t="str">
         <v>n</v>
@@ -6345,301 +6386,407 @@
         <v>y</v>
       </c>
       <c r="K25" s="1" t="str">
+        <v xml:space="preserve">P added at four concentrations as equimolar K2HPO4 and KH2PO4: 0, 0.005, 0.02, 0.1 mM P) </v>
+      </c>
+      <c r="L25" s="1" t="str">
+        <v>n</v>
+      </c>
+      <c r="M25" s="1" t="str">
+        <v>n</v>
+      </c>
+      <c r="N25" s="1" t="str">
+        <v>n/a</v>
+      </c>
+      <c r="O25" s="1" t="str">
+        <v>greenhouse</v>
+      </c>
+      <c r="P25" s="1" t="str">
+        <v>n; treatment mean and standard errors in text</v>
+      </c>
+      <c r="Q25" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" ht="153" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="str">
+        <v>P fertilization experiment that measures photosynthetic traits</v>
+      </c>
+      <c r="B26" s="1" t="str">
+        <v>Huiying</v>
+      </c>
+      <c r="C26" s="1" t="str">
+        <v>Yu et al.</v>
+      </c>
+      <c r="D26" s="1">
+        <v>2022</v>
+      </c>
+      <c r="E26" s="1" t="str">
+        <v>Foliar phosphorus allocation and photosynthesis reveal plants' adaptative strategies to phosphorus limitation in tropical forests at different successional stages</v>
+      </c>
+      <c r="F26" s="1" t="str">
+        <v>Science of Total Environment</v>
+      </c>
+      <c r="G26" s="1" t="str">
+        <v>https://doi.org/10.1016/j.scitotenv.2022.157456</v>
+      </c>
+      <c r="H26" s="1" t="str">
+        <v>Amax, gsw, chlorophyll content, LA, LT, LDMC, SLA, PNUE, PPUE, leaf C, N &amp; P, leaf P allocated to four parts</v>
+      </c>
+      <c r="I26" s="1" t="str">
+        <v>y</v>
+      </c>
+      <c r="J26" s="1" t="str">
+        <v>y</v>
+      </c>
+      <c r="K26" s="1" t="str">
+        <v>N addition (N50, 50 kg N ha−1 yr−1), P addition (P50, 50 kg P ha−1 yr−1), and NP addition (N50P50, 50 kg N ha−1 yr−1 + 50 kg P ha−1 yr−1). N and P were added in the forms of NH4NO3 and Ca(H2PO4)2 dissolved in 30 L of water</v>
+      </c>
+      <c r="L26" s="1" t="str">
+        <v>y</v>
+      </c>
+      <c r="M26" s="1" t="str">
+        <v>y</v>
+      </c>
+      <c r="N26" s="1">
+        <v>0</v>
+      </c>
+      <c r="O26" s="1">
+        <v>0</v>
+      </c>
+      <c r="P26" s="1" t="str">
+        <v>y</v>
+      </c>
+      <c r="Q26" s="1" t="str">
+        <v>Data will be made available on request; leaf nutrient data are extractable from Table 2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" ht="85" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="str">
+        <v>P fertilization experiment that measures photosynthetic traits</v>
+      </c>
+      <c r="B27" s="1" t="str">
+        <v>monika</v>
+      </c>
+      <c r="C27" s="1" t="str">
+        <v>Cheng et al.</v>
+      </c>
+      <c r="D27" s="1">
+        <v>2014</v>
+      </c>
+      <c r="E27" s="1" t="str">
+        <v>Interactions between light intensity and phosphorus nutrition affect the phosphate-mining capacity of white lupin (Lupinus albus L.)</v>
+      </c>
+      <c r="F27" s="1" t="str">
+        <v>Journal of Experimental Botany</v>
+      </c>
+      <c r="G27" s="1" t="str">
+        <v>https://doi.org/10.1093/jxb/eru135</v>
+      </c>
+      <c r="H27" s="1" t="str">
+        <v>Cluster roots, root length &amp; surface area, Net photosynthetic rate (Pn), P concentraiton of roots and shoots, root exudates, RNA</v>
+      </c>
+      <c r="I27" s="1" t="str">
+        <v>n</v>
+      </c>
+      <c r="J27" s="1" t="str">
+        <v>y</v>
+      </c>
+      <c r="K27" s="1" t="str">
         <v>P supplied at 1  µM (P deficiency) or 50  µM (P sufficienct). P supplied at KH2PO4</v>
       </c>
-      <c r="L25" s="1" t="str">
-        <v>y</v>
-      </c>
-      <c r="M25" s="1" t="str">
-        <v>y</v>
-      </c>
-      <c r="N25" s="1" t="str">
+      <c r="L27" s="1" t="str">
+        <v>y</v>
+      </c>
+      <c r="M27" s="1" t="str">
+        <v>y</v>
+      </c>
+      <c r="N27" s="1" t="str">
         <v>N: 2000 µM Ca(NO3), 0.01 µM (NH4)6Mo7O24 . 
 P: 50 µM and 1 µM as KH2PO4</v>
       </c>
-      <c r="O25" s="1" t="str">
+      <c r="O27" s="1" t="str">
         <v>growth chambers</v>
       </c>
-      <c r="P25" s="1" t="str">
+      <c r="P27" s="1" t="str">
         <v>n</v>
       </c>
-      <c r="Q25" s="1">
+      <c r="Q27" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:17" ht="136" x14ac:dyDescent="0.2">
-      <c r="A26" s="1" t="str">
+    <row r="28" spans="1:17" ht="136" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="str">
         <v>P fertilization experiment that measures photosynthetic traits</v>
       </c>
-      <c r="B26" s="1" t="str">
+      <c r="B28" s="1" t="str">
         <v>monika</v>
       </c>
-      <c r="C26" s="1" t="str">
+      <c r="C28" s="1" t="str">
         <v>Zhao et al.</v>
       </c>
-      <c r="D26" s="1">
+      <c r="D28" s="1">
         <v>2022</v>
       </c>
-      <c r="E26" s="1" t="str">
+      <c r="E28" s="1" t="str">
         <v>Phosphate fertilizers increase CO2 assimilation and yield of soybean in a shaded environment</v>
       </c>
-      <c r="F26" s="1" t="str">
+      <c r="F28" s="1" t="str">
         <v>Photosynthetica</v>
       </c>
-      <c r="G26" s="1" t="str">
+      <c r="G28" s="1" t="str">
         <v>https://ps.ueb.cas.cz/pdfs/phs/2022/02/01.pdf</v>
       </c>
-      <c r="H26" s="1" t="str">
+      <c r="H28" s="1" t="str">
         <v>Net photosynthetic rate  - light intensity curves, chlorophyll fluorescence</v>
       </c>
-      <c r="I26" s="1" t="str">
+      <c r="I28" s="1" t="str">
         <v>n</v>
       </c>
-      <c r="J26" s="1" t="str">
-        <v>y</v>
-      </c>
-      <c r="K26" s="1" t="str">
+      <c r="J28" s="1" t="str">
+        <v>y</v>
+      </c>
+      <c r="K28" s="1" t="str">
         <v>two P concentrations: 
 P1, 0 kg(P2O5) ha-1; 
 P2, 180 kg(P2O5) ha-1</v>
       </c>
-      <c r="L26" s="1" t="str">
-        <v>y</v>
-      </c>
-      <c r="M26" s="1" t="str">
-        <v>y</v>
-      </c>
-      <c r="N26" s="1" t="str">
+      <c r="L28" s="1" t="str">
+        <v>y</v>
+      </c>
+      <c r="M28" s="1" t="str">
+        <v>y</v>
+      </c>
+      <c r="N28" s="1" t="str">
         <v>within the 0–20 cm soil depth were: 12.53 g(soil organic
 carbon) kg−1, 1.15 g(soil total nitrogen) kg−1, 11.27
 mg(available phosphorus) kg−1, 0.68 g(total phosphorus)
 kg–1, 80.9 mg(available potassium) kg–1, and pH of 6.8</v>
       </c>
-      <c r="O26" s="1" t="str">
+      <c r="O28" s="1" t="str">
         <v>field</v>
       </c>
-      <c r="P26" s="1" t="str">
+      <c r="P28" s="1" t="str">
         <v>unsure
 Might have to reach out to authors for data</v>
       </c>
-      <c r="Q26" s="1" t="str">
+      <c r="Q28" s="1" t="str">
         <v xml:space="preserve">two light treatments, ambient sunlight, and 40% shade.
 </v>
       </c>
     </row>
-    <row r="27" spans="1:17" ht="289" x14ac:dyDescent="0.2">
-      <c r="A27" s="1" t="str">
+    <row r="29" spans="1:17" ht="85" x14ac:dyDescent="0.2">
+      <c r="A29" s="2" t="str">
         <v>P fertilization experiment that measures photosynthetic traits</v>
       </c>
-      <c r="B27" s="1" t="str">
+      <c r="B29" s="2" t="str">
         <v>Huiying</v>
       </c>
-      <c r="C27" s="1" t="str">
+      <c r="C29" s="2" t="str">
         <v xml:space="preserve">Xiaodong Wang </v>
       </c>
-      <c r="D27" s="1">
+      <c r="D29" s="2">
         <v>2024</v>
       </c>
-      <c r="E27" s="1" t="str">
+      <c r="E29" s="1" t="str">
         <v>The effect of phosphorus addition on the rhizosphere process and root and leaf traits for dominant tree species of Schima superba and Castanopsis fargesii in an evergreen broad-leaved forest</v>
       </c>
-      <c r="F27" s="1" t="str">
+      <c r="F29" s="2" t="str">
         <v>PhD thesis</v>
       </c>
-      <c r="G27" s="1" t="str">
+      <c r="G29" s="2" t="str">
         <v>https://tlink.lib.tsinghua.edu.cn/https/443/net/cnki/kns/yitlink/kcms2/article/abstract?v=UjEBX92ALNEtsjI9aefwRwj3YlLSAn5S1mkrShM31qMg1m9eqwXAOt7cj_iUZx_i4zJvZMveBPwSdwZThRTNbN-OM_WtlD3iOxh54hvZMuiAhMSnnlr2H12FVws-ptRip7CsrKCIUCpQ-Yh0hHsWj1qltYOtjS0xfYmDH2eWfH8BqqmAUV_yT4kOe2swxvCe&amp;uniplatform=NZKPT&amp;language=CHS</v>
       </c>
-      <c r="H27" s="1" t="str">
+      <c r="H29" s="1" t="str">
         <v>chlorophyll content; PNUE; Vcmax; Jmax; gs; A; iWUE</v>
       </c>
-      <c r="I27" s="1" t="str">
+      <c r="I29" s="2" t="str">
         <v>n</v>
       </c>
-      <c r="J27" s="1" t="str">
-        <v>y</v>
-      </c>
-      <c r="K27" s="1" t="str">
+      <c r="J29" s="2" t="str">
+        <v>y</v>
+      </c>
+      <c r="K29" s="2" t="str">
         <v>50 kg P ha-1 a-1</v>
       </c>
-      <c r="L27" s="1" t="str">
-        <v>y</v>
-      </c>
-      <c r="M27" s="1" t="str">
-        <v>y</v>
-      </c>
-      <c r="N27" s="1" t="str">
+      <c r="L29" s="2" t="str">
+        <v>y</v>
+      </c>
+      <c r="M29" s="2" t="str">
+        <v>y</v>
+      </c>
+      <c r="N29" s="2" t="str">
         <v>NaH2PO4 was applied in March and Sept</v>
       </c>
-      <c r="O27" s="1" t="str">
+      <c r="O29" s="2" t="str">
         <v>field</v>
       </c>
-      <c r="P27" s="1" t="str">
+      <c r="P29" s="2" t="str">
         <v>unsure
 having trouble finding paper, help</v>
       </c>
-      <c r="Q27" s="1" t="str">
+      <c r="Q29" s="2" t="str">
         <v>can be extracted from figure, mean and se. 
 Having trouble finding paper, help! - Monika</v>
       </c>
     </row>
-    <row r="28" spans="1:17" ht="119" x14ac:dyDescent="0.2">
-      <c r="A28" s="1" t="str">
+    <row r="30" spans="1:17" ht="68" x14ac:dyDescent="0.2">
+      <c r="A30" s="2" t="str">
         <v>P fertilization experiment that measures photosynthetic traits</v>
       </c>
-      <c r="B28" s="1" t="str">
+      <c r="B30" s="2" t="str">
         <v>Huiying</v>
       </c>
-      <c r="C28" s="1" t="str">
+      <c r="C30" s="2" t="str">
         <v>Ma et al.</v>
       </c>
-      <c r="D28" s="1">
+      <c r="D30" s="2">
         <v>2023</v>
       </c>
-      <c r="E28" s="1" t="str">
+      <c r="E30" s="1" t="str">
         <v>Effects of Nitrogen and Phosphorus Addition on Photosynthetic Characteristics and Antioxidant System of Suaeda salsa in the Yellow River Delta</v>
       </c>
-      <c r="F28" s="1" t="str">
+      <c r="F30" s="2" t="str">
         <v>Journal of Yunnan Agricultural University</v>
       </c>
-      <c r="G28" s="1" t="str">
+      <c r="G30" s="2" t="str">
         <v>10.12101/j.issn.1004-390X(n).202209020</v>
       </c>
-      <c r="H28" s="1" t="str">
+      <c r="H30" s="1" t="str">
         <v>chlorophyll content; Anet; gs; ci; WUE</v>
       </c>
-      <c r="I28" s="1" t="str">
-        <v>y</v>
-      </c>
-      <c r="J28" s="1" t="str">
-        <v>y</v>
-      </c>
-      <c r="K28" s="1">
+      <c r="I30" s="2" t="str">
+        <v>y</v>
+      </c>
+      <c r="J30" s="2" t="str">
+        <v>y</v>
+      </c>
+      <c r="K30" s="2">
         <v>0</v>
       </c>
-      <c r="L28" s="1" t="str">
-        <v>y</v>
-      </c>
-      <c r="M28" s="1" t="str">
-        <v>y</v>
-      </c>
-      <c r="N28" s="1" t="str">
+      <c r="L30" s="2" t="str">
+        <v>y</v>
+      </c>
+      <c r="M30" s="2" t="str">
+        <v>y</v>
+      </c>
+      <c r="N30" s="2" t="str">
         <v>N0, N5, N15, N45 are  0, 5, 15 and 45 g/m2; P0 and P1 are 0 and 1g/m2; N5P0、N15P0, N45P0, N0P1, N5P1, N15P1, N45P1, N0P0</v>
       </c>
-      <c r="O28" s="1" t="str">
+      <c r="O30" s="2" t="str">
         <v>field</v>
       </c>
-      <c r="P28" s="1" t="str">
+      <c r="P30" s="2" t="str">
         <v>part available
 having trouble finding paper, help</v>
       </c>
-      <c r="Q28" s="1" t="str">
+      <c r="Q30" s="2" t="str">
         <v xml:space="preserve">can be extracted from figure, </v>
       </c>
     </row>
-    <row r="29" spans="1:17" ht="51" x14ac:dyDescent="0.2">
-      <c r="A29" s="2" t="str">
+    <row r="31" spans="1:17" ht="51" x14ac:dyDescent="0.2">
+      <c r="A31" s="2" t="str">
         <v>P fertilization experiment that measures photosynthetic traits</v>
       </c>
-      <c r="B29" s="2" t="str">
+      <c r="B31" s="2" t="str">
         <v>Jan</v>
       </c>
-      <c r="C29" s="2" t="str">
+      <c r="C31" s="2" t="str">
         <v>S. Wang et al</v>
       </c>
-      <c r="D29" s="2">
+      <c r="D31" s="2">
         <v>2020</v>
       </c>
-      <c r="E29" s="1" t="str">
+      <c r="E31" s="1" t="str">
         <v>Source and sink activity of Holcus lanatus in response to absolute and relative supply of nitrogen and phosphorus</v>
       </c>
-      <c r="F29" s="2" t="str">
+      <c r="F31" s="2" t="str">
         <v>Functional Plant Biology</v>
       </c>
-      <c r="G29" s="2" t="str">
+      <c r="G31" s="2" t="str">
         <v>DOI: 10.1071/FP20118</v>
       </c>
-      <c r="H29" s="1" t="str">
+      <c r="H31" s="1" t="str">
         <v xml:space="preserve">Amax, SLA, </v>
       </c>
-      <c r="I29" s="2" t="str">
-        <v>y</v>
-      </c>
-      <c r="J29" s="2" t="str">
-        <v>y</v>
-      </c>
-      <c r="K29" s="2" t="str">
+      <c r="I31" s="2" t="str">
+        <v>y</v>
+      </c>
+      <c r="J31" s="2" t="str">
+        <v>y</v>
+      </c>
+      <c r="K31" s="2" t="str">
         <v xml:space="preserve">three N:P ratio's, two absolute levels. </v>
       </c>
-      <c r="L29" s="2" t="str">
+      <c r="L31" s="2" t="str">
         <v>n</v>
       </c>
-      <c r="M29" s="2" t="str">
+      <c r="M31" s="2" t="str">
         <v>n</v>
       </c>
-      <c r="N29" s="2" t="str">
+      <c r="N31" s="2" t="str">
         <v>N: low:30, 52, 90, 90, 156, 270 (mg)
 P: 6, 3.5, 2, 18, 10.5, 6 (mg)</v>
       </c>
-      <c r="O29" s="2" t="str">
+      <c r="O31" s="2" t="str">
         <v>greenhouse</v>
       </c>
-      <c r="P29" s="2" t="str">
+      <c r="P31" s="2" t="str">
         <v>n</v>
       </c>
-      <c r="Q29" s="2" t="str">
+      <c r="Q31" s="2" t="str">
         <v>Maybe ask Hugo</v>
       </c>
     </row>
-    <row r="30" spans="1:17" ht="51" x14ac:dyDescent="0.2">
-      <c r="A30" s="2" t="str">
+    <row r="32" spans="1:17" ht="51" x14ac:dyDescent="0.2">
+      <c r="A32" s="2" t="str">
         <v>P fertilization experiment that measures photosynthetic traits</v>
       </c>
-      <c r="B30" s="2" t="str">
+      <c r="B32" s="2" t="str">
         <v>Evan</v>
       </c>
-      <c r="C30" s="2" t="str">
+      <c r="C32" s="2" t="str">
         <v>Fan et al.</v>
       </c>
-      <c r="D30" s="2">
+      <c r="D32" s="2">
         <v>2024</v>
       </c>
-      <c r="E30" s="1" t="str">
+      <c r="E32" s="1" t="str">
         <v>Variation in leaf phosphorus fractions reflects plant adaptations and distribution in low-phosphorus tropical forests</v>
       </c>
-      <c r="F30" s="2" t="str">
+      <c r="F32" s="2" t="str">
         <v>Functional Ecology</v>
       </c>
-      <c r="G30" s="2" t="str">
+      <c r="G32" s="2" t="str">
         <v>https://doi.org/10.1111/1365-2435.14721</v>
       </c>
-      <c r="H30" s="1" t="str">
+      <c r="H32" s="1" t="str">
         <v>LMA, Nmass, Pmass, RGR, Amax, Vcmax, Jmax, PPUE, PNUE, leaf phosphorus fractions</v>
       </c>
-      <c r="I30" s="2" t="str">
+      <c r="I32" s="2" t="str">
         <v>n</v>
       </c>
-      <c r="J30" s="2" t="str">
-        <v>y</v>
-      </c>
-      <c r="K30" s="2" t="str">
+      <c r="J32" s="2" t="str">
+        <v>y</v>
+      </c>
+      <c r="K32" s="2" t="str">
         <v>40 mg/kg P as NaH2PO4*H2O and a control (no P addition)</v>
       </c>
-      <c r="L30" s="2" t="str">
-        <v>y</v>
-      </c>
-      <c r="M30" s="2" t="str">
-        <v>y</v>
-      </c>
-      <c r="N30" s="2" t="str">
+      <c r="L32" s="2" t="str">
+        <v>y</v>
+      </c>
+      <c r="M32" s="2" t="str">
+        <v>y</v>
+      </c>
+      <c r="N32" s="2" t="str">
         <v>g/kg</v>
       </c>
-      <c r="O30" s="2" t="str">
+      <c r="O32" s="2" t="str">
         <v>field</v>
       </c>
-      <c r="P30" s="2" t="str">
-        <v>y</v>
-      </c>
-      <c r="Q30" s="2" t="str">
+      <c r="P32" s="2" t="str">
+        <v>y</v>
+      </c>
+      <c r="Q32" s="2" t="str">
         <v>really ideal dataset for this meta analysis!</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add firn et al 2019, zavisic et al 2018, and bloomfield et al 2014 datasets, then plow through first go at meta-analysis
</commit_message>
<xml_diff>
--- a/lit_search_np_fert_exps.xlsx
+++ b/lit_search_np_fert_exps.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eaperkowski/git/p_meta/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6DF8CBB-95F4-6C4F-B76C-F524445257B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7C58801-5A95-0D4C-91CC-C77EB87455DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6320" yWindow="500" windowWidth="44880" windowHeight="28300" xr2:uid="{50492CE8-F5C0-524A-968F-FD9EC2022F6C}"/>
+    <workbookView xWindow="1400" yWindow="500" windowWidth="44880" windowHeight="28300" activeTab="1" xr2:uid="{50492CE8-F5C0-524A-968F-FD9EC2022F6C}"/>
   </bookViews>
   <sheets>
     <sheet name="all_papers" sheetId="1" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="809" uniqueCount="373">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="822" uniqueCount="378">
   <si>
     <t>category (drop down, auto colors row)</t>
   </si>
@@ -1218,12 +1218,27 @@
   <si>
     <t>n; treatment mean and standard errors in text</t>
   </si>
+  <si>
+    <t>Firn et al.</t>
+  </si>
+  <si>
+    <t>Nature Ecology and Evoluation</t>
+  </si>
+  <si>
+    <t>Leaf nutrients, not specific leaf area, are consistent indicators of elevated nutrient inputs</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1038/s41559-018-0790-1</t>
+  </si>
+  <si>
+    <t>LMA (through SLA), Nmass, Pmass. Can use LMA to calculate Narea and Parea</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1357,6 +1372,12 @@
       <color theme="1"/>
       <name val="Aptos Narrow"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -1424,7 +1445,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1498,9 +1519,6 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1509,6 +1527,15 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2104,11 +2131,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72E471E8-ACD0-FD4B-A457-BF8C11A8C657}">
   <dimension ref="A1:S60"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B38" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B54" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G42" sqref="G42"/>
+      <selection pane="bottomRight" activeCell="C58" sqref="C58:H58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3330,54 +3357,54 @@
         <v>156</v>
       </c>
     </row>
-    <row r="26" spans="1:17" ht="119" x14ac:dyDescent="0.2">
-      <c r="A26" s="1" t="s">
+    <row r="26" spans="1:17" s="28" customFormat="1" ht="119" x14ac:dyDescent="0.2">
+      <c r="A26" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B26" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="C26" s="18" t="s">
         <v>157</v>
       </c>
-      <c r="D26" s="1">
+      <c r="D26" s="18">
         <v>2018</v>
       </c>
-      <c r="E26" s="1" t="s">
+      <c r="E26" s="18" t="s">
         <v>158</v>
       </c>
-      <c r="F26" s="1" t="s">
+      <c r="F26" s="18" t="s">
         <v>143</v>
       </c>
-      <c r="G26" s="3" t="s">
+      <c r="G26" s="19" t="s">
         <v>159</v>
       </c>
-      <c r="H26" s="1" t="s">
+      <c r="H26" s="18" t="s">
         <v>160</v>
       </c>
-      <c r="I26" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="J26" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="K26" s="1" t="s">
+      <c r="I26" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="J26" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="K26" s="18" t="s">
         <v>161</v>
       </c>
-      <c r="L26" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="M26" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="N26" s="1" t="s">
+      <c r="L26" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="M26" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="N26" s="18" t="s">
         <v>162</v>
       </c>
-      <c r="O26" s="1"/>
-      <c r="P26" s="1" t="s">
+      <c r="O26" s="18"/>
+      <c r="P26" s="18" t="s">
         <v>155</v>
       </c>
-      <c r="Q26" s="1"/>
+      <c r="Q26" s="18"/>
     </row>
     <row r="27" spans="1:17" ht="136" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
@@ -4002,54 +4029,54 @@
       <c r="P39" s="1"/>
       <c r="Q39" s="1"/>
     </row>
-    <row r="40" spans="1:17" ht="136" x14ac:dyDescent="0.2">
-      <c r="A40" s="1" t="s">
+    <row r="40" spans="1:17" s="28" customFormat="1" ht="136" x14ac:dyDescent="0.2">
+      <c r="A40" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="B40" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="C40" s="1" t="s">
+      <c r="C40" s="18" t="s">
         <v>248</v>
       </c>
-      <c r="D40" s="1">
+      <c r="D40" s="18">
         <v>2014</v>
       </c>
-      <c r="E40" s="1" t="s">
+      <c r="E40" s="18" t="s">
         <v>249</v>
       </c>
-      <c r="F40" s="1" t="s">
+      <c r="F40" s="18" t="s">
         <v>250</v>
       </c>
-      <c r="G40" s="3" t="s">
+      <c r="G40" s="19" t="s">
         <v>251</v>
       </c>
-      <c r="H40" s="1" t="s">
+      <c r="H40" s="18" t="s">
         <v>252</v>
       </c>
-      <c r="I40" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="J40" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="K40" s="1" t="s">
+      <c r="I40" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="J40" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="K40" s="18" t="s">
         <v>253</v>
       </c>
-      <c r="L40" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="M40" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="N40" s="1" t="s">
+      <c r="L40" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="M40" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="N40" s="18" t="s">
         <v>254</v>
       </c>
-      <c r="O40" s="1"/>
-      <c r="P40" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q40" s="1"/>
+      <c r="O40" s="18"/>
+      <c r="P40" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q40" s="18"/>
     </row>
     <row r="41" spans="1:17" ht="102" x14ac:dyDescent="0.2">
       <c r="A41" s="18" t="s">
@@ -4585,159 +4612,159 @@
       </c>
     </row>
     <row r="52" spans="1:17" ht="102" x14ac:dyDescent="0.2">
-      <c r="A52" s="25" t="s">
+      <c r="A52" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B52" s="25" t="s">
+      <c r="B52" s="1" t="s">
         <v>296</v>
       </c>
-      <c r="C52" s="25" t="s">
+      <c r="C52" s="1" t="s">
         <v>316</v>
       </c>
-      <c r="D52" s="25">
+      <c r="D52" s="1">
         <v>2014</v>
       </c>
-      <c r="E52" s="25" t="s">
+      <c r="E52" s="1" t="s">
         <v>317</v>
       </c>
-      <c r="F52" s="25" t="s">
+      <c r="F52" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="G52" s="26" t="s">
+      <c r="G52" s="25" t="s">
         <v>318</v>
       </c>
-      <c r="H52" s="25" t="s">
+      <c r="H52" s="1" t="s">
         <v>319</v>
       </c>
-      <c r="I52" s="25" t="s">
-        <v>25</v>
-      </c>
-      <c r="J52" s="25" t="s">
-        <v>33</v>
-      </c>
-      <c r="K52" s="25" t="s">
+      <c r="I52" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J52" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K52" s="1" t="s">
         <v>320</v>
       </c>
-      <c r="L52" s="25" t="s">
-        <v>33</v>
-      </c>
-      <c r="M52" s="25" t="s">
-        <v>33</v>
-      </c>
-      <c r="N52" s="25" t="s">
+      <c r="L52" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="M52" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="N52" s="1" t="s">
         <v>321</v>
       </c>
-      <c r="O52" s="25" t="s">
+      <c r="O52" s="1" t="s">
         <v>303</v>
       </c>
-      <c r="P52" s="25" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q52" s="25"/>
+      <c r="P52" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q52" s="1"/>
     </row>
     <row r="53" spans="1:17" s="15" customFormat="1" ht="187" x14ac:dyDescent="0.2">
-      <c r="A53" s="25" t="s">
+      <c r="A53" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B53" s="25" t="s">
+      <c r="B53" s="1" t="s">
         <v>296</v>
       </c>
-      <c r="C53" s="25" t="s">
+      <c r="C53" s="1" t="s">
         <v>322</v>
       </c>
-      <c r="D53" s="25">
+      <c r="D53" s="1">
         <v>2022</v>
       </c>
-      <c r="E53" s="25" t="s">
+      <c r="E53" s="1" t="s">
         <v>323</v>
       </c>
-      <c r="F53" s="25" t="s">
+      <c r="F53" s="1" t="s">
         <v>305</v>
       </c>
-      <c r="G53" s="26" t="s">
+      <c r="G53" s="25" t="s">
         <v>324</v>
       </c>
-      <c r="H53" s="25" t="s">
+      <c r="H53" s="1" t="s">
         <v>325</v>
       </c>
-      <c r="I53" s="25" t="s">
-        <v>25</v>
-      </c>
-      <c r="J53" s="25" t="s">
-        <v>33</v>
-      </c>
-      <c r="K53" s="25" t="s">
+      <c r="I53" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J53" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K53" s="1" t="s">
         <v>326</v>
       </c>
-      <c r="L53" s="25" t="s">
-        <v>33</v>
-      </c>
-      <c r="M53" s="25" t="s">
-        <v>33</v>
-      </c>
-      <c r="N53" s="25" t="s">
+      <c r="L53" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="M53" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="N53" s="1" t="s">
         <v>327</v>
       </c>
-      <c r="O53" s="25" t="s">
+      <c r="O53" s="1" t="s">
         <v>328</v>
       </c>
-      <c r="P53" s="25" t="s">
+      <c r="P53" s="1" t="s">
         <v>329</v>
       </c>
-      <c r="Q53" s="25" t="s">
+      <c r="Q53" s="1" t="s">
         <v>330</v>
       </c>
     </row>
     <row r="54" spans="1:17" s="15" customFormat="1" ht="306" x14ac:dyDescent="0.2">
-      <c r="A54" s="25" t="s">
+      <c r="A54" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B54" s="25" t="s">
+      <c r="B54" s="1" t="s">
         <v>309</v>
       </c>
-      <c r="C54" s="25" t="s">
+      <c r="C54" s="1" t="s">
         <v>331</v>
       </c>
-      <c r="D54" s="25">
+      <c r="D54" s="1">
         <v>2024</v>
       </c>
-      <c r="E54" s="25" t="s">
+      <c r="E54" s="1" t="s">
         <v>332</v>
       </c>
-      <c r="F54" s="25" t="s">
+      <c r="F54" s="1" t="s">
         <v>333</v>
       </c>
-      <c r="G54" s="26" t="s">
+      <c r="G54" s="25" t="s">
         <v>334</v>
       </c>
-      <c r="H54" s="25" t="s">
+      <c r="H54" s="1" t="s">
         <v>335</v>
       </c>
-      <c r="I54" s="25" t="s">
-        <v>25</v>
-      </c>
-      <c r="J54" s="25" t="s">
-        <v>33</v>
-      </c>
-      <c r="K54" s="25" t="s">
+      <c r="I54" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J54" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K54" s="1" t="s">
         <v>336</v>
       </c>
-      <c r="L54" s="25" t="s">
-        <v>33</v>
-      </c>
-      <c r="M54" s="25" t="s">
-        <v>33</v>
-      </c>
-      <c r="N54" s="27" t="s">
+      <c r="L54" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="M54" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="N54" s="26" t="s">
         <v>337</v>
       </c>
-      <c r="O54" s="25" t="s">
+      <c r="O54" s="1" t="s">
         <v>328</v>
       </c>
-      <c r="P54" s="25" t="s">
+      <c r="P54" s="1" t="s">
         <v>338</v>
       </c>
-      <c r="Q54" s="25" t="s">
+      <c r="Q54" s="1" t="s">
         <v>339</v>
       </c>
     </row>
@@ -4793,55 +4820,55 @@
       </c>
     </row>
     <row r="56" spans="1:17" ht="85" x14ac:dyDescent="0.2">
-      <c r="A56" s="25" t="s">
+      <c r="A56" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B56" s="25" t="s">
+      <c r="B56" s="1" t="s">
         <v>348</v>
       </c>
-      <c r="C56" s="25" t="s">
+      <c r="C56" s="1" t="s">
         <v>349</v>
       </c>
-      <c r="D56" s="25">
+      <c r="D56" s="1">
         <v>2020</v>
       </c>
-      <c r="E56" s="25" t="s">
+      <c r="E56" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="F56" s="25" t="s">
+      <c r="F56" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="G56" s="26" t="s">
+      <c r="G56" s="25" t="s">
         <v>351</v>
       </c>
-      <c r="H56" s="25" t="s">
+      <c r="H56" s="1" t="s">
         <v>352</v>
       </c>
-      <c r="I56" s="25" t="s">
-        <v>33</v>
-      </c>
-      <c r="J56" s="25" t="s">
-        <v>33</v>
-      </c>
-      <c r="K56" s="25" t="s">
+      <c r="I56" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J56" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K56" s="1" t="s">
         <v>353</v>
       </c>
-      <c r="L56" s="25" t="s">
-        <v>25</v>
-      </c>
-      <c r="M56" s="25" t="s">
-        <v>25</v>
-      </c>
-      <c r="N56" s="25" t="s">
+      <c r="L56" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M56" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N56" s="1" t="s">
         <v>354</v>
       </c>
-      <c r="O56" s="25" t="s">
+      <c r="O56" s="1" t="s">
         <v>355</v>
       </c>
-      <c r="P56" s="25" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q56" s="25" t="s">
+      <c r="P56" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q56" s="1" t="s">
         <v>356</v>
       </c>
     </row>
@@ -4864,7 +4891,7 @@
       <c r="F57" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="G57" s="28" t="s">
+      <c r="G57" s="27" t="s">
         <v>360</v>
       </c>
       <c r="H57" s="18" t="s">
@@ -4898,24 +4925,52 @@
         <v>364</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A58" s="1"/>
-      <c r="B58" s="1"/>
-      <c r="C58" s="1"/>
-      <c r="D58" s="1"/>
-      <c r="E58" s="1"/>
-      <c r="F58" s="1"/>
-      <c r="G58" s="9"/>
-      <c r="H58" s="1"/>
-      <c r="I58" s="1"/>
-      <c r="J58" s="1"/>
-      <c r="K58" s="1"/>
-      <c r="L58" s="1"/>
-      <c r="M58" s="1"/>
-      <c r="N58" s="1"/>
-      <c r="O58" s="1"/>
-      <c r="P58" s="1"/>
-      <c r="Q58" s="1"/>
+    <row r="58" spans="1:17" ht="68" x14ac:dyDescent="0.2">
+      <c r="A58" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="B58" s="10" t="s">
+        <v>357</v>
+      </c>
+      <c r="C58" s="10" t="s">
+        <v>373</v>
+      </c>
+      <c r="D58" s="10">
+        <v>2019</v>
+      </c>
+      <c r="E58" s="29" t="s">
+        <v>375</v>
+      </c>
+      <c r="F58" s="10" t="s">
+        <v>374</v>
+      </c>
+      <c r="G58" s="30" t="s">
+        <v>376</v>
+      </c>
+      <c r="H58" s="10" t="s">
+        <v>377</v>
+      </c>
+      <c r="I58" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="J58" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="K58" s="10"/>
+      <c r="L58" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="M58" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="N58" s="10"/>
+      <c r="O58" s="10" t="s">
+        <v>328</v>
+      </c>
+      <c r="P58" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q58" s="10"/>
     </row>
     <row r="59" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A59" s="1"/>
@@ -4956,7 +5011,7 @@
       <c r="Q60" s="1"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:Q49 A50:G50 J50 L50:Q50 A51:Q53 A54:M54 O54:Q54 F55:G55 I55:Q55 A55:D56 F56:Q56 A57:Q1048576">
+  <conditionalFormatting sqref="A1:Q49 A50:G50 J50 L50:Q50 A51:Q53 A54:M54 O54:Q54 F55:G55 I55:Q55 A55:D56 F56:Q56 A57:Q57 A59:Q1048576 A58:D58 F58 H58:Q58">
     <cfRule type="expression" dxfId="8" priority="5">
       <formula>$A1="Does not quantify P availability and/or does not manipulate P fertilization"</formula>
     </cfRule>
@@ -5055,11 +5110,11 @@
   <sheetPr>
     <tabColor theme="9" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:Q32"/>
+  <dimension ref="A1:Q33"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5135,7 +5190,7 @@
     </row>
     <row r="2" spans="1:17" ht="85" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="str" cm="1">
-        <f t="array" ref="A2:Q32">_xlfn._xlws.FILTER(all_papers!A:Q, all_papers!A:A = "P fertilization experiment that measures photosynthetic traits")</f>
+        <f t="array" ref="A2:Q33">_xlfn._xlws.FILTER(all_papers!A:Q, all_papers!A:A = "P fertilization experiment that measures photosynthetic traits")</f>
         <v>P fertilization experiment that measures photosynthetic traits</v>
       </c>
       <c r="B2" s="2" t="str">
@@ -6788,6 +6843,59 @@
       </c>
       <c r="Q32" s="2" t="str">
         <v>really ideal dataset for this meta analysis!</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" ht="51" x14ac:dyDescent="0.2">
+      <c r="A33" s="2" t="str">
+        <v>P fertilization experiment that measures photosynthetic traits</v>
+      </c>
+      <c r="B33" s="2" t="str">
+        <v>Evan</v>
+      </c>
+      <c r="C33" s="1" t="str">
+        <v>Firn et al.</v>
+      </c>
+      <c r="D33" s="1">
+        <v>2019</v>
+      </c>
+      <c r="E33" s="1" t="str">
+        <v>Leaf nutrients, not specific leaf area, are consistent indicators of elevated nutrient inputs</v>
+      </c>
+      <c r="F33" s="1" t="str">
+        <v>Nature Ecology and Evoluation</v>
+      </c>
+      <c r="G33" s="1" t="str">
+        <v>https://doi.org/10.1038/s41559-018-0790-1</v>
+      </c>
+      <c r="H33" s="1" t="str">
+        <v>LMA (through SLA), Nmass, Pmass. Can use LMA to calculate Narea and Parea</v>
+      </c>
+      <c r="I33" s="1" t="str">
+        <v>y</v>
+      </c>
+      <c r="J33" s="1" t="str">
+        <v>y</v>
+      </c>
+      <c r="K33" s="1">
+        <v>0</v>
+      </c>
+      <c r="L33" s="1" t="str">
+        <v>y</v>
+      </c>
+      <c r="M33" s="1" t="str">
+        <v>y</v>
+      </c>
+      <c r="N33" s="1">
+        <v>0</v>
+      </c>
+      <c r="O33" s="1" t="str">
+        <v>field</v>
+      </c>
+      <c r="P33" s="1" t="str">
+        <v>y</v>
+      </c>
+      <c r="Q33" s="1">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add some scripts for digitizing plots, load Wang 2019 Pfraction papers
</commit_message>
<xml_diff>
--- a/lit_search_np_fert_exps.xlsx
+++ b/lit_search_np_fert_exps.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10112"/>
   <workbookPr updateLinks="always"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eaperkowski/git/p_meta/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7C58801-5A95-0D4C-91CC-C77EB87455DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCE44919-EDFA-3A45-8029-100645321FD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1400" yWindow="500" windowWidth="44880" windowHeight="28300" activeTab="1" xr2:uid="{50492CE8-F5C0-524A-968F-FD9EC2022F6C}"/>
+    <workbookView xWindow="51140" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{50492CE8-F5C0-524A-968F-FD9EC2022F6C}"/>
   </bookViews>
   <sheets>
     <sheet name="all_papers" sheetId="1" r:id="rId1"/>
@@ -40,9 +40,10 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="2">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+    <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
   </metadataTypes>
   <futureMetadata name="XLDAPR" count="1">
     <bk>
@@ -53,16 +54,30 @@
       </extLst>
     </bk>
   </futureMetadata>
+  <futureMetadata name="XLRICHVALUE" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
   <cellMetadata count="1">
     <bk>
       <rc t="1" v="0"/>
     </bk>
   </cellMetadata>
+  <valueMetadata count="1">
+    <bk>
+      <rc t="2" v="0"/>
+    </bk>
+  </valueMetadata>
 </metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="822" uniqueCount="378">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="881" uniqueCount="397">
   <si>
     <t>category (drop down, auto colors row)</t>
   </si>
@@ -1232,6 +1247,63 @@
   </si>
   <si>
     <t>LMA (through SLA), Nmass, Pmass. Can use LMA to calculate Narea and Parea</t>
+  </si>
+  <si>
+    <t>Cleland et al.</t>
+  </si>
+  <si>
+    <t>Belowground biomass response to nutrient enrichment depends on light limitation across globally distributed grasslands</t>
+  </si>
+  <si>
+    <t>Ecosystems</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1007/s10021-019-00350-4</t>
+  </si>
+  <si>
+    <t>root mass fraction, belowground biomass, aboveground biomass (estimated using rmf and bgb)</t>
+  </si>
+  <si>
+    <t>Nutrient Network fertilization scheme</t>
+  </si>
+  <si>
+    <t>summary table cleaned in R to make for easy load into compiled data file</t>
+  </si>
+  <si>
+    <t>Wang et al.</t>
+  </si>
+  <si>
+    <t>Effects of nutrient addition on foliar phosphorus fractions and their resorption in different-aged leaves of Chinese fir in subtropical China</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1007/s11104-019-04221-8</t>
+  </si>
+  <si>
+    <t>leaf phosphorus fractions (Pi, sugar P, nucleic P, residual P), Nmass, Pmass</t>
+  </si>
+  <si>
+    <t>Two nitrogen addition treatments (N1 = 50 kg N/ha/yr, N2 = 100 kg N/ha/yr) and one phosphorus treatment (50 kg P/ha/yr) in full factorial setup (i.e. N1, N2, P, N1P, N2P, Control)</t>
+  </si>
+  <si>
+    <t>n; mean and SE reported in supplemental table</t>
+  </si>
+  <si>
+    <t>summary table copied from supplemental table, then cleaned in R to make for easy load into compiled data file</t>
+  </si>
+  <si>
+    <t>Ye et al.</t>
+  </si>
+  <si>
+    <t>Species divergence in seedling leaf traits and tree growth response to nitrogen and phosphorus additions in an evergreen broadleaved forest of subtropical China</t>
+  </si>
+  <si>
+    <t>Journal of Forestry Research</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1007/s11676-021-01437-2</t>
+  </si>
+  <si>
+    <t>Full factorial NP experiment</t>
   </si>
 </sst>
 </file>
@@ -1445,7 +1517,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1469,9 +1541,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1537,12 +1606,42 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="28">
+  <dxfs count="29">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1786,27 +1885,89 @@
 </styleSheet>
 </file>
 
+<file path=xl/richData/rdRichValueTypes.xml><?xml version="1.0" encoding="utf-8"?>
+<rvTypesInfo xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
+  <global>
+    <keyFlags>
+      <key name="_Self">
+        <flag name="ExcludeFromFile" value="1"/>
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_DisplayString">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Flags">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Format">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_SubLabel">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Attribution">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Icon">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Display">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_CanonicalPropertyNames">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_ClassificationId">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+    </keyFlags>
+  </global>
+</rvTypesInfo>
+</file>
+
+<file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
+<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
+  <rv s="0">
+    <v>16</v>
+    <v>8</v>
+    <v>33</v>
+    <v>1</v>
+  </rv>
+</rvData>
+</file>
+
+<file path=xl/richData/rdrichvaluestructure.xml><?xml version="1.0" encoding="utf-8"?>
+<rvStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
+  <s t="_error">
+    <k n="colOffset" t="i"/>
+    <k n="errorType" t="i"/>
+    <k n="rwOffset" t="i"/>
+    <k n="subType" t="i"/>
+  </s>
+</rvStructures>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8093FBDE-B7CD-8C4A-9997-94ED3A5AF75C}" name="Table1" displayName="Table1" ref="A1:Q60" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26">
-  <autoFilter ref="A1:Q60" xr:uid="{8093FBDE-B7CD-8C4A-9997-94ED3A5AF75C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8093FBDE-B7CD-8C4A-9997-94ED3A5AF75C}" name="Table1" displayName="Table1" ref="A1:Q61" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27">
+  <autoFilter ref="A1:Q61" xr:uid="{8093FBDE-B7CD-8C4A-9997-94ED3A5AF75C}"/>
   <tableColumns count="17">
-    <tableColumn id="1" xr3:uid="{E15574CC-1F76-B945-BDBD-AD4BA8C8C3B7}" name="category (drop down, auto colors row)" dataDxfId="25"/>
-    <tableColumn id="19" xr3:uid="{6AFE88A9-1A96-4113-AD81-F820945F5841}" name="notes_by(your name)" dataDxfId="24"/>
-    <tableColumn id="14" xr3:uid="{CAFD1825-FCB5-4229-8252-87372B4269FB}" name="authors" dataDxfId="23"/>
-    <tableColumn id="2" xr3:uid="{3CEA2BFA-BD8F-594C-BAA2-8C8B6F8C553C}" name="year" dataDxfId="22"/>
-    <tableColumn id="3" xr3:uid="{C9E5E426-1492-8748-A2E5-D10DF0CB21E7}" name="title" dataDxfId="21"/>
-    <tableColumn id="4" xr3:uid="{CE25BE8F-B854-264F-BDDD-2F8207E04481}" name="journal" dataDxfId="20"/>
-    <tableColumn id="5" xr3:uid="{47E94D51-0CD6-234D-BFD6-C597383AF0F8}" name="doi" dataDxfId="19" dataCellStyle="Hyperlink"/>
-    <tableColumn id="6" xr3:uid="{1A230D2C-4AF7-8240-8A8A-813805B9F442}" name="traits_measured" dataDxfId="18"/>
-    <tableColumn id="7" xr3:uid="{EAB07DEB-B8D2-7F4D-87F0-F44EA418AE96}" name="n_fert_yn" dataDxfId="17"/>
-    <tableColumn id="8" xr3:uid="{28747112-425A-EF46-BC2E-352E96918620}" name="p_fert_yn" dataDxfId="16"/>
-    <tableColumn id="9" xr3:uid="{B2C892FE-5FF1-7B4A-BA0A-E82FA960CA3D}" name="np_fert_method" dataDxfId="15"/>
-    <tableColumn id="10" xr3:uid="{DB1AB260-DCF4-3049-8F11-4321A3205248}" name="n_avail_yn" dataDxfId="14"/>
-    <tableColumn id="11" xr3:uid="{C4BE562A-BE9F-AF49-A89E-2A47F832C256}" name="p_avail_yn" dataDxfId="13"/>
-    <tableColumn id="12" xr3:uid="{70CD1115-165E-D34F-84D2-2E2BC95B0A35}" name="np_method" dataDxfId="12"/>
-    <tableColumn id="15" xr3:uid="{45D59765-0EA3-F44D-A74A-98D0D16C0FF1}" name="experiment_type" dataDxfId="11"/>
-    <tableColumn id="16" xr3:uid="{FF08C533-3661-42BC-95A5-7AD222A24ACE}" name="data_available_yn" dataDxfId="10"/>
-    <tableColumn id="13" xr3:uid="{A95F19E6-DD0D-574F-B162-EA325C31A05F}" name="notes" dataDxfId="9"/>
+    <tableColumn id="1" xr3:uid="{E15574CC-1F76-B945-BDBD-AD4BA8C8C3B7}" name="category (drop down, auto colors row)" dataDxfId="26"/>
+    <tableColumn id="19" xr3:uid="{6AFE88A9-1A96-4113-AD81-F820945F5841}" name="notes_by(your name)" dataDxfId="25"/>
+    <tableColumn id="14" xr3:uid="{CAFD1825-FCB5-4229-8252-87372B4269FB}" name="authors" dataDxfId="24"/>
+    <tableColumn id="2" xr3:uid="{3CEA2BFA-BD8F-594C-BAA2-8C8B6F8C553C}" name="year" dataDxfId="23"/>
+    <tableColumn id="3" xr3:uid="{C9E5E426-1492-8748-A2E5-D10DF0CB21E7}" name="title" dataDxfId="22"/>
+    <tableColumn id="4" xr3:uid="{CE25BE8F-B854-264F-BDDD-2F8207E04481}" name="journal" dataDxfId="21"/>
+    <tableColumn id="5" xr3:uid="{47E94D51-0CD6-234D-BFD6-C597383AF0F8}" name="doi" dataDxfId="20" dataCellStyle="Hyperlink"/>
+    <tableColumn id="6" xr3:uid="{1A230D2C-4AF7-8240-8A8A-813805B9F442}" name="traits_measured" dataDxfId="19"/>
+    <tableColumn id="7" xr3:uid="{EAB07DEB-B8D2-7F4D-87F0-F44EA418AE96}" name="n_fert_yn" dataDxfId="18"/>
+    <tableColumn id="8" xr3:uid="{28747112-425A-EF46-BC2E-352E96918620}" name="p_fert_yn" dataDxfId="17"/>
+    <tableColumn id="9" xr3:uid="{B2C892FE-5FF1-7B4A-BA0A-E82FA960CA3D}" name="np_fert_method" dataDxfId="16"/>
+    <tableColumn id="10" xr3:uid="{DB1AB260-DCF4-3049-8F11-4321A3205248}" name="n_avail_yn" dataDxfId="15"/>
+    <tableColumn id="11" xr3:uid="{C4BE562A-BE9F-AF49-A89E-2A47F832C256}" name="p_avail_yn" dataDxfId="14"/>
+    <tableColumn id="12" xr3:uid="{70CD1115-165E-D34F-84D2-2E2BC95B0A35}" name="np_method" dataDxfId="13"/>
+    <tableColumn id="15" xr3:uid="{45D59765-0EA3-F44D-A74A-98D0D16C0FF1}" name="experiment_type" dataDxfId="12"/>
+    <tableColumn id="16" xr3:uid="{FF08C533-3661-42BC-95A5-7AD222A24ACE}" name="data_available_yn" dataDxfId="11"/>
+    <tableColumn id="13" xr3:uid="{A95F19E6-DD0D-574F-B162-EA325C31A05F}" name="notes" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2129,13 +2290,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72E471E8-ACD0-FD4B-A457-BF8C11A8C657}">
-  <dimension ref="A1:S60"/>
+  <dimension ref="A1:S61"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B54" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B58" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C58" sqref="C58:H58"/>
+      <selection pane="bottomRight" activeCell="B63" sqref="B63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2555,55 +2716,55 @@
       <c r="P8" s="1"/>
     </row>
     <row r="9" spans="1:19" ht="136" x14ac:dyDescent="0.2">
-      <c r="A9" s="18" t="s">
+      <c r="A9" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="B9" s="18" t="s">
+      <c r="B9" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="18" t="s">
+      <c r="C9" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="D9" s="18">
+      <c r="D9" s="17">
         <v>2022</v>
       </c>
-      <c r="E9" s="18" t="s">
+      <c r="E9" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="F9" s="18" t="s">
+      <c r="F9" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="G9" s="19" t="s">
+      <c r="G9" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="H9" s="18" t="s">
+      <c r="H9" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="I9" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="J9" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="K9" s="18" t="s">
+      <c r="I9" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="J9" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="K9" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="L9" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="M9" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="N9" s="18" t="s">
+      <c r="L9" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="M9" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="N9" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="O9" s="18" t="s">
+      <c r="O9" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="P9" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q9" s="18"/>
+      <c r="P9" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q9" s="17"/>
     </row>
     <row r="10" spans="1:19" ht="119" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
@@ -3168,7 +3329,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:17" ht="153" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:17" ht="170" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>41</v>
       </c>
@@ -3357,54 +3518,54 @@
         <v>156</v>
       </c>
     </row>
-    <row r="26" spans="1:17" s="28" customFormat="1" ht="119" x14ac:dyDescent="0.2">
-      <c r="A26" s="18" t="s">
+    <row r="26" spans="1:17" s="27" customFormat="1" ht="119" x14ac:dyDescent="0.2">
+      <c r="A26" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="B26" s="18" t="s">
+      <c r="B26" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="C26" s="18" t="s">
+      <c r="C26" s="17" t="s">
         <v>157</v>
       </c>
-      <c r="D26" s="18">
+      <c r="D26" s="17">
         <v>2018</v>
       </c>
-      <c r="E26" s="18" t="s">
+      <c r="E26" s="17" t="s">
         <v>158</v>
       </c>
-      <c r="F26" s="18" t="s">
+      <c r="F26" s="17" t="s">
         <v>143</v>
       </c>
-      <c r="G26" s="19" t="s">
+      <c r="G26" s="18" t="s">
         <v>159</v>
       </c>
-      <c r="H26" s="18" t="s">
+      <c r="H26" s="17" t="s">
         <v>160</v>
       </c>
-      <c r="I26" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="J26" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="K26" s="18" t="s">
+      <c r="I26" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="J26" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="K26" s="17" t="s">
         <v>161</v>
       </c>
-      <c r="L26" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="M26" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="N26" s="18" t="s">
+      <c r="L26" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="M26" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="N26" s="17" t="s">
         <v>162</v>
       </c>
-      <c r="O26" s="18"/>
-      <c r="P26" s="18" t="s">
+      <c r="O26" s="17"/>
+      <c r="P26" s="17" t="s">
         <v>155</v>
       </c>
-      <c r="Q26" s="18"/>
+      <c r="Q26" s="17"/>
     </row>
     <row r="27" spans="1:17" ht="136" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
@@ -3554,53 +3715,53 @@
       <c r="Q29" s="1"/>
     </row>
     <row r="30" spans="1:17" ht="119" x14ac:dyDescent="0.2">
-      <c r="A30" s="18" t="s">
+      <c r="A30" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="B30" s="18" t="s">
+      <c r="B30" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="C30" s="18" t="s">
+      <c r="C30" s="17" t="s">
         <v>184</v>
       </c>
-      <c r="D30" s="18">
+      <c r="D30" s="17">
         <v>2021</v>
       </c>
-      <c r="E30" s="18" t="s">
+      <c r="E30" s="17" t="s">
         <v>185</v>
       </c>
-      <c r="F30" s="18" t="s">
+      <c r="F30" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="G30" s="19" t="s">
+      <c r="G30" s="18" t="s">
         <v>186</v>
       </c>
-      <c r="H30" s="18" t="s">
+      <c r="H30" s="17" t="s">
         <v>187</v>
       </c>
-      <c r="I30" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="J30" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="K30" s="18" t="s">
+      <c r="I30" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="J30" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="K30" s="17" t="s">
         <v>188</v>
       </c>
-      <c r="L30" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="M30" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="N30" s="18" t="s">
+      <c r="L30" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="M30" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="N30" s="17" t="s">
         <v>189</v>
       </c>
-      <c r="O30" s="18"/>
-      <c r="P30" s="18" t="s">
+      <c r="O30" s="17"/>
+      <c r="P30" s="17" t="s">
         <v>190</v>
       </c>
-      <c r="Q30" s="18" t="s">
+      <c r="Q30" s="17" t="s">
         <v>191</v>
       </c>
     </row>
@@ -3940,53 +4101,53 @@
       </c>
     </row>
     <row r="38" spans="1:17" ht="119" x14ac:dyDescent="0.2">
-      <c r="A38" s="18" t="s">
+      <c r="A38" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="B38" s="18" t="s">
+      <c r="B38" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="C38" s="18" t="s">
+      <c r="C38" s="17" t="s">
         <v>238</v>
       </c>
-      <c r="D38" s="18">
+      <c r="D38" s="17">
         <v>2017</v>
       </c>
-      <c r="E38" s="18" t="s">
+      <c r="E38" s="17" t="s">
         <v>368</v>
       </c>
-      <c r="F38" s="18" t="s">
+      <c r="F38" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="G38" s="19" t="s">
+      <c r="G38" s="18" t="s">
         <v>239</v>
       </c>
-      <c r="H38" s="18" t="s">
+      <c r="H38" s="17" t="s">
         <v>240</v>
       </c>
-      <c r="I38" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="J38" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="K38" s="18" t="s">
+      <c r="I38" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="J38" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="K38" s="17" t="s">
         <v>241</v>
       </c>
-      <c r="L38" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="M38" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="N38" s="18" t="s">
+      <c r="L38" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="M38" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="N38" s="17" t="s">
         <v>242</v>
       </c>
-      <c r="O38" s="18"/>
-      <c r="P38" s="18" t="s">
+      <c r="O38" s="17"/>
+      <c r="P38" s="17" t="s">
         <v>243</v>
       </c>
-      <c r="Q38" s="18"/>
+      <c r="Q38" s="17"/>
     </row>
     <row r="39" spans="1:17" ht="102" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
@@ -4029,154 +4190,154 @@
       <c r="P39" s="1"/>
       <c r="Q39" s="1"/>
     </row>
-    <row r="40" spans="1:17" s="28" customFormat="1" ht="136" x14ac:dyDescent="0.2">
-      <c r="A40" s="18" t="s">
+    <row r="40" spans="1:17" s="27" customFormat="1" ht="136" x14ac:dyDescent="0.2">
+      <c r="A40" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="B40" s="18" t="s">
+      <c r="B40" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="C40" s="18" t="s">
+      <c r="C40" s="17" t="s">
         <v>248</v>
       </c>
-      <c r="D40" s="18">
+      <c r="D40" s="17">
         <v>2014</v>
       </c>
-      <c r="E40" s="18" t="s">
+      <c r="E40" s="17" t="s">
         <v>249</v>
       </c>
-      <c r="F40" s="18" t="s">
+      <c r="F40" s="17" t="s">
         <v>250</v>
       </c>
-      <c r="G40" s="19" t="s">
+      <c r="G40" s="18" t="s">
         <v>251</v>
       </c>
-      <c r="H40" s="18" t="s">
+      <c r="H40" s="17" t="s">
         <v>252</v>
       </c>
-      <c r="I40" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="J40" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="K40" s="18" t="s">
+      <c r="I40" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="J40" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="K40" s="17" t="s">
         <v>253</v>
       </c>
-      <c r="L40" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="M40" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="N40" s="18" t="s">
+      <c r="L40" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="M40" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="N40" s="17" t="s">
         <v>254</v>
       </c>
-      <c r="O40" s="18"/>
-      <c r="P40" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q40" s="18"/>
+      <c r="O40" s="17"/>
+      <c r="P40" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q40" s="17"/>
     </row>
     <row r="41" spans="1:17" ht="102" x14ac:dyDescent="0.2">
-      <c r="A41" s="18" t="s">
+      <c r="A41" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="B41" s="18" t="s">
+      <c r="B41" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="C41" s="18" t="s">
+      <c r="C41" s="17" t="s">
         <v>255</v>
       </c>
-      <c r="D41" s="18">
+      <c r="D41" s="17">
         <v>2007</v>
       </c>
-      <c r="E41" s="18" t="s">
+      <c r="E41" s="17" t="s">
         <v>256</v>
       </c>
-      <c r="F41" s="18" t="s">
+      <c r="F41" s="17" t="s">
         <v>257</v>
       </c>
-      <c r="G41" s="19" t="s">
+      <c r="G41" s="18" t="s">
         <v>258</v>
       </c>
-      <c r="H41" s="18" t="s">
+      <c r="H41" s="17" t="s">
         <v>259</v>
       </c>
-      <c r="I41" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="J41" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="K41" s="18" t="s">
+      <c r="I41" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="J41" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="K41" s="17" t="s">
         <v>260</v>
       </c>
-      <c r="L41" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="M41" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="N41" s="18" t="s">
+      <c r="L41" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="M41" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="N41" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="O41" s="18"/>
-      <c r="P41" s="18" t="s">
+      <c r="O41" s="17"/>
+      <c r="P41" s="17" t="s">
         <v>261</v>
       </c>
-      <c r="Q41" s="18" t="s">
+      <c r="Q41" s="17" t="s">
         <v>262</v>
       </c>
     </row>
     <row r="42" spans="1:17" ht="119" x14ac:dyDescent="0.2">
-      <c r="A42" s="18" t="s">
+      <c r="A42" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="B42" s="18" t="s">
+      <c r="B42" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="C42" s="18" t="s">
+      <c r="C42" s="17" t="s">
         <v>263</v>
       </c>
-      <c r="D42" s="18">
+      <c r="D42" s="17">
         <v>2005</v>
       </c>
-      <c r="E42" s="18" t="s">
+      <c r="E42" s="17" t="s">
         <v>264</v>
       </c>
-      <c r="F42" s="18" t="s">
+      <c r="F42" s="17" t="s">
         <v>265</v>
       </c>
-      <c r="G42" s="19" t="s">
+      <c r="G42" s="18" t="s">
         <v>266</v>
       </c>
-      <c r="H42" s="18" t="s">
+      <c r="H42" s="17" t="s">
         <v>267</v>
       </c>
-      <c r="I42" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="J42" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="K42" s="18" t="s">
+      <c r="I42" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="J42" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="K42" s="17" t="s">
         <v>268</v>
       </c>
-      <c r="L42" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="M42" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="N42" s="18" t="s">
+      <c r="L42" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="M42" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="N42" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="O42" s="18"/>
-      <c r="P42" s="18" t="s">
+      <c r="O42" s="17"/>
+      <c r="P42" s="17" t="s">
         <v>261</v>
       </c>
-      <c r="Q42" s="18" t="s">
+      <c r="Q42" s="17" t="s">
         <v>262</v>
       </c>
     </row>
@@ -4229,105 +4390,105 @@
         <v>274</v>
       </c>
     </row>
-    <row r="44" spans="1:17" s="15" customFormat="1" ht="102" x14ac:dyDescent="0.2">
-      <c r="A44" s="18" t="s">
+    <row r="44" spans="1:17" s="14" customFormat="1" ht="102" x14ac:dyDescent="0.2">
+      <c r="A44" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="B44" s="18" t="s">
+      <c r="B44" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="C44" s="18" t="s">
+      <c r="C44" s="17" t="s">
         <v>269</v>
       </c>
-      <c r="D44" s="18">
+      <c r="D44" s="17">
         <v>2002</v>
       </c>
-      <c r="E44" s="18" t="s">
+      <c r="E44" s="17" t="s">
         <v>270</v>
       </c>
-      <c r="F44" s="18" t="s">
+      <c r="F44" s="17" t="s">
         <v>257</v>
       </c>
-      <c r="G44" s="20" t="s">
+      <c r="G44" s="19" t="s">
         <v>271</v>
       </c>
-      <c r="H44" s="18" t="s">
+      <c r="H44" s="17" t="s">
         <v>272</v>
       </c>
-      <c r="I44" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="J44" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="K44" s="18" t="s">
+      <c r="I44" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="J44" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="K44" s="17" t="s">
         <v>275</v>
       </c>
-      <c r="L44" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="M44" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="N44" s="18" t="s">
+      <c r="L44" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="M44" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="N44" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="O44" s="18"/>
-      <c r="P44" s="18" t="s">
+      <c r="O44" s="17"/>
+      <c r="P44" s="17" t="s">
         <v>276</v>
       </c>
-      <c r="Q44" s="18" t="s">
+      <c r="Q44" s="17" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="45" spans="1:17" s="12" customFormat="1" ht="119" x14ac:dyDescent="0.2">
-      <c r="A45" s="16" t="s">
+    <row r="45" spans="1:17" s="11" customFormat="1" ht="119" x14ac:dyDescent="0.2">
+      <c r="A45" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="B45" s="16" t="s">
+      <c r="B45" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="C45" s="16" t="s">
+      <c r="C45" s="15" t="s">
         <v>184</v>
       </c>
-      <c r="D45" s="16">
+      <c r="D45" s="15">
         <v>2019</v>
       </c>
-      <c r="E45" s="16" t="s">
+      <c r="E45" s="15" t="s">
         <v>278</v>
       </c>
-      <c r="F45" s="16" t="s">
+      <c r="F45" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="G45" s="17" t="s">
+      <c r="G45" s="16" t="s">
         <v>279</v>
       </c>
-      <c r="H45" s="16" t="s">
+      <c r="H45" s="15" t="s">
         <v>280</v>
       </c>
-      <c r="I45" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="J45" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="K45" s="16" t="s">
+      <c r="I45" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="J45" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="K45" s="15" t="s">
         <v>281</v>
       </c>
-      <c r="L45" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="M45" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="N45" s="16" t="s">
+      <c r="L45" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="M45" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="N45" s="15" t="s">
         <v>282</v>
       </c>
-      <c r="O45" s="16"/>
-      <c r="P45" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q45" s="16" t="s">
+      <c r="O45" s="15"/>
+      <c r="P45" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q45" s="15" t="s">
         <v>283</v>
       </c>
     </row>
@@ -4381,100 +4542,100 @@
       </c>
     </row>
     <row r="47" spans="1:17" ht="119" x14ac:dyDescent="0.2">
-      <c r="A47" s="13" t="s">
+      <c r="A47" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="B47" s="13" t="s">
+      <c r="B47" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="C47" s="13" t="s">
+      <c r="C47" s="12" t="s">
         <v>291</v>
       </c>
-      <c r="D47" s="13">
+      <c r="D47" s="12">
         <v>1989</v>
       </c>
-      <c r="E47" s="13" t="s">
+      <c r="E47" s="12" t="s">
         <v>292</v>
       </c>
-      <c r="F47" s="13" t="s">
+      <c r="F47" s="12" t="s">
         <v>225</v>
       </c>
-      <c r="G47" s="14" t="s">
+      <c r="G47" s="13" t="s">
         <v>293</v>
       </c>
-      <c r="H47" s="13" t="s">
+      <c r="H47" s="12" t="s">
         <v>294</v>
       </c>
-      <c r="I47" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="J47" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="K47" s="13" t="s">
+      <c r="I47" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="J47" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="K47" s="12" t="s">
         <v>295</v>
       </c>
-      <c r="L47" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="M47" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="N47" s="13" t="s">
+      <c r="L47" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="M47" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="N47" s="12" t="s">
         <v>26</v>
       </c>
       <c r="O47" s="1"/>
-      <c r="P47" s="13" t="s">
+      <c r="P47" s="12" t="s">
         <v>222</v>
       </c>
       <c r="Q47" s="1"/>
     </row>
-    <row r="48" spans="1:17" s="15" customFormat="1" ht="153" x14ac:dyDescent="0.2">
-      <c r="A48" s="13" t="s">
+    <row r="48" spans="1:17" s="14" customFormat="1" ht="153" x14ac:dyDescent="0.2">
+      <c r="A48" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="B48" s="13" t="s">
+      <c r="B48" s="12" t="s">
         <v>296</v>
       </c>
-      <c r="C48" s="13" t="s">
+      <c r="C48" s="12" t="s">
         <v>297</v>
       </c>
-      <c r="D48" s="13">
+      <c r="D48" s="12">
         <v>1995</v>
       </c>
-      <c r="E48" s="13" t="s">
+      <c r="E48" s="12" t="s">
         <v>298</v>
       </c>
-      <c r="F48" s="13" t="s">
+      <c r="F48" s="12" t="s">
         <v>299</v>
       </c>
-      <c r="G48" s="14" t="s">
+      <c r="G48" s="13" t="s">
         <v>300</v>
       </c>
-      <c r="H48" s="13" t="s">
+      <c r="H48" s="12" t="s">
         <v>301</v>
       </c>
-      <c r="I48" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="J48" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="K48" s="13" t="s">
+      <c r="I48" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="J48" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="K48" s="12" t="s">
         <v>302</v>
       </c>
-      <c r="L48" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="M48" s="13"/>
-      <c r="N48" s="13"/>
-      <c r="O48" s="13" t="s">
+      <c r="L48" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="M48" s="12"/>
+      <c r="N48" s="12"/>
+      <c r="O48" s="12" t="s">
         <v>303</v>
       </c>
-      <c r="P48" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q48" s="13" t="s">
+      <c r="P48" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q48" s="12" t="s">
         <v>369</v>
       </c>
     </row>
@@ -4512,102 +4673,102 @@
       <c r="Q49" s="1"/>
     </row>
     <row r="50" spans="1:17" ht="85" x14ac:dyDescent="0.2">
-      <c r="A50" s="18" t="s">
+      <c r="A50" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="B50" s="18" t="s">
+      <c r="B50" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="C50" s="18" t="s">
+      <c r="C50" s="17" t="s">
         <v>269</v>
       </c>
-      <c r="D50" s="18">
+      <c r="D50" s="17">
         <v>2011</v>
       </c>
-      <c r="E50" s="18" t="s">
+      <c r="E50" s="17" t="s">
         <v>307</v>
       </c>
-      <c r="F50" s="18" t="s">
+      <c r="F50" s="17" t="s">
         <v>257</v>
       </c>
-      <c r="G50" s="19" t="s">
+      <c r="G50" s="18" t="s">
         <v>308</v>
       </c>
-      <c r="H50" s="21" t="s">
+      <c r="H50" s="20" t="s">
         <v>370</v>
       </c>
-      <c r="I50" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="J50" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="K50" s="21" t="s">
+      <c r="I50" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="J50" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="K50" s="20" t="s">
         <v>371</v>
       </c>
-      <c r="L50" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="M50" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="N50" s="10" t="s">
+      <c r="L50" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="M50" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="N50" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="O50" s="10" t="s">
+      <c r="O50" s="9" t="s">
         <v>355</v>
       </c>
-      <c r="P50" s="10" t="s">
+      <c r="P50" s="9" t="s">
         <v>372</v>
       </c>
-      <c r="Q50" s="18"/>
-    </row>
-    <row r="51" spans="1:17" s="15" customFormat="1" ht="153" x14ac:dyDescent="0.2">
-      <c r="A51" s="18" t="s">
+      <c r="Q50" s="17"/>
+    </row>
+    <row r="51" spans="1:17" s="14" customFormat="1" ht="153" x14ac:dyDescent="0.2">
+      <c r="A51" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="B51" s="18" t="s">
+      <c r="B51" s="17" t="s">
         <v>309</v>
       </c>
-      <c r="C51" s="18" t="s">
+      <c r="C51" s="17" t="s">
         <v>310</v>
       </c>
-      <c r="D51" s="18">
+      <c r="D51" s="17">
         <v>2022</v>
       </c>
-      <c r="E51" s="18" t="s">
+      <c r="E51" s="17" t="s">
         <v>311</v>
       </c>
-      <c r="F51" s="18" t="s">
+      <c r="F51" s="17" t="s">
         <v>312</v>
       </c>
-      <c r="G51" s="20" t="s">
+      <c r="G51" s="19" t="s">
         <v>313</v>
       </c>
-      <c r="H51" s="18" t="s">
+      <c r="H51" s="17" t="s">
         <v>314</v>
       </c>
-      <c r="I51" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="J51" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="K51" s="18" t="s">
+      <c r="I51" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="J51" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="K51" s="17" t="s">
         <v>315</v>
       </c>
-      <c r="L51" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="M51" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="N51" s="18"/>
-      <c r="O51" s="18"/>
-      <c r="P51" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q51" s="18" t="s">
+      <c r="L51" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="M51" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="N51" s="17"/>
+      <c r="O51" s="17"/>
+      <c r="P51" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q51" s="17" t="s">
         <v>367</v>
       </c>
     </row>
@@ -4630,7 +4791,7 @@
       <c r="F52" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="G52" s="25" t="s">
+      <c r="G52" s="24" t="s">
         <v>318</v>
       </c>
       <c r="H52" s="1" t="s">
@@ -4662,7 +4823,7 @@
       </c>
       <c r="Q52" s="1"/>
     </row>
-    <row r="53" spans="1:17" s="15" customFormat="1" ht="187" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:17" s="14" customFormat="1" ht="187" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>41</v>
       </c>
@@ -4681,7 +4842,7 @@
       <c r="F53" s="1" t="s">
         <v>305</v>
       </c>
-      <c r="G53" s="25" t="s">
+      <c r="G53" s="24" t="s">
         <v>324</v>
       </c>
       <c r="H53" s="1" t="s">
@@ -4715,7 +4876,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="54" spans="1:17" s="15" customFormat="1" ht="306" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:17" s="14" customFormat="1" ht="306" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>41</v>
       </c>
@@ -4734,7 +4895,7 @@
       <c r="F54" s="1" t="s">
         <v>333</v>
       </c>
-      <c r="G54" s="25" t="s">
+      <c r="G54" s="24" t="s">
         <v>334</v>
       </c>
       <c r="H54" s="1" t="s">
@@ -4755,7 +4916,7 @@
       <c r="M54" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="N54" s="26" t="s">
+      <c r="N54" s="25" t="s">
         <v>337</v>
       </c>
       <c r="O54" s="1" t="s">
@@ -4768,54 +4929,54 @@
         <v>339</v>
       </c>
     </row>
-    <row r="55" spans="1:17" s="15" customFormat="1" ht="113.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="22" t="s">
+    <row r="55" spans="1:17" s="14" customFormat="1" ht="113.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="B55" s="22" t="s">
+      <c r="B55" s="21" t="s">
         <v>309</v>
       </c>
-      <c r="C55" s="22" t="s">
+      <c r="C55" s="21" t="s">
         <v>340</v>
       </c>
-      <c r="D55" s="22">
+      <c r="D55" s="21">
         <v>2023</v>
       </c>
-      <c r="E55" s="22" t="s">
+      <c r="E55" s="21" t="s">
         <v>341</v>
       </c>
-      <c r="F55" s="22" t="s">
+      <c r="F55" s="21" t="s">
         <v>342</v>
       </c>
-      <c r="G55" s="23" t="s">
+      <c r="G55" s="22" t="s">
         <v>343</v>
       </c>
-      <c r="H55" s="24" t="s">
+      <c r="H55" s="23" t="s">
         <v>344</v>
       </c>
-      <c r="I55" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="J55" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="K55" s="22"/>
-      <c r="L55" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="M55" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="N55" s="22" t="s">
+      <c r="I55" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="J55" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="K55" s="21"/>
+      <c r="L55" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="M55" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="N55" s="21" t="s">
         <v>345</v>
       </c>
-      <c r="O55" s="22" t="s">
+      <c r="O55" s="21" t="s">
         <v>328</v>
       </c>
-      <c r="P55" s="22" t="s">
+      <c r="P55" s="21" t="s">
         <v>346</v>
       </c>
-      <c r="Q55" s="22" t="s">
+      <c r="Q55" s="21" t="s">
         <v>347</v>
       </c>
     </row>
@@ -4838,7 +4999,7 @@
       <c r="F56" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="G56" s="25" t="s">
+      <c r="G56" s="24" t="s">
         <v>351</v>
       </c>
       <c r="H56" s="1" t="s">
@@ -4873,170 +5034,270 @@
       </c>
     </row>
     <row r="57" spans="1:17" ht="102" x14ac:dyDescent="0.2">
-      <c r="A57" s="18" t="s">
+      <c r="A57" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="B57" s="18" t="s">
+      <c r="B57" s="17" t="s">
         <v>357</v>
       </c>
-      <c r="C57" s="18" t="s">
+      <c r="C57" s="17" t="s">
         <v>358</v>
       </c>
-      <c r="D57" s="18">
+      <c r="D57" s="17">
         <v>2024</v>
       </c>
-      <c r="E57" s="18" t="s">
+      <c r="E57" s="17" t="s">
         <v>359</v>
       </c>
-      <c r="F57" s="18" t="s">
+      <c r="F57" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="G57" s="27" t="s">
+      <c r="G57" s="26" t="s">
         <v>360</v>
       </c>
-      <c r="H57" s="18" t="s">
+      <c r="H57" s="17" t="s">
         <v>361</v>
       </c>
-      <c r="I57" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="J57" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="K57" s="18" t="s">
+      <c r="I57" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="J57" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="K57" s="17" t="s">
         <v>362</v>
       </c>
-      <c r="L57" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="M57" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="N57" s="18" t="s">
+      <c r="L57" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="M57" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="N57" s="17" t="s">
         <v>363</v>
       </c>
-      <c r="O57" s="18" t="s">
+      <c r="O57" s="17" t="s">
         <v>328</v>
       </c>
-      <c r="P57" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q57" s="18" t="s">
+      <c r="P57" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q57" s="17" t="s">
         <v>364</v>
       </c>
     </row>
     <row r="58" spans="1:17" ht="68" x14ac:dyDescent="0.2">
-      <c r="A58" s="10" t="s">
+      <c r="A58" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="B58" s="10" t="s">
+      <c r="B58" s="9" t="s">
         <v>357</v>
       </c>
-      <c r="C58" s="10" t="s">
+      <c r="C58" s="9" t="s">
         <v>373</v>
       </c>
-      <c r="D58" s="10">
+      <c r="D58" s="9">
         <v>2019</v>
       </c>
-      <c r="E58" s="29" t="s">
+      <c r="E58" s="28" t="s">
         <v>375</v>
       </c>
-      <c r="F58" s="10" t="s">
+      <c r="F58" s="9" t="s">
         <v>374</v>
       </c>
-      <c r="G58" s="30" t="s">
+      <c r="G58" s="29" t="s">
         <v>376</v>
       </c>
-      <c r="H58" s="10" t="s">
+      <c r="H58" s="9" t="s">
         <v>377</v>
       </c>
-      <c r="I58" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="J58" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="K58" s="10"/>
-      <c r="L58" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="M58" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="N58" s="10"/>
-      <c r="O58" s="10" t="s">
+      <c r="I58" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="J58" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="K58" s="9"/>
+      <c r="L58" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="M58" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="N58" s="9"/>
+      <c r="O58" s="9" t="s">
         <v>328</v>
       </c>
-      <c r="P58" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q58" s="10"/>
-    </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A59" s="1"/>
-      <c r="B59" s="1"/>
-      <c r="C59" s="1"/>
-      <c r="D59" s="1"/>
-      <c r="E59" s="1"/>
-      <c r="F59" s="1"/>
-      <c r="G59" s="9"/>
-      <c r="H59" s="1"/>
-      <c r="I59" s="1"/>
-      <c r="J59" s="1"/>
-      <c r="K59" s="1"/>
-      <c r="L59" s="1"/>
-      <c r="M59" s="1"/>
-      <c r="N59" s="1"/>
-      <c r="O59" s="1"/>
-      <c r="P59" s="1"/>
-      <c r="Q59" s="1"/>
-    </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A60" s="1"/>
-      <c r="B60" s="1"/>
-      <c r="C60" s="1"/>
-      <c r="D60" s="1"/>
-      <c r="E60" s="1"/>
-      <c r="F60" s="1"/>
-      <c r="G60" s="9"/>
-      <c r="H60" s="1"/>
-      <c r="I60" s="1"/>
-      <c r="J60" s="1"/>
-      <c r="K60" s="1"/>
-      <c r="L60" s="1"/>
-      <c r="M60" s="1"/>
-      <c r="N60" s="1"/>
-      <c r="O60" s="1"/>
-      <c r="P60" s="1"/>
-      <c r="Q60" s="1"/>
+      <c r="P58" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q58" s="9"/>
+    </row>
+    <row r="59" spans="1:17" ht="102" x14ac:dyDescent="0.2">
+      <c r="A59" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B59" s="30" t="s">
+        <v>357</v>
+      </c>
+      <c r="C59" s="30" t="s">
+        <v>378</v>
+      </c>
+      <c r="D59" s="30">
+        <v>2019</v>
+      </c>
+      <c r="E59" s="30" t="s">
+        <v>379</v>
+      </c>
+      <c r="F59" s="30" t="s">
+        <v>380</v>
+      </c>
+      <c r="G59" s="31" t="s">
+        <v>381</v>
+      </c>
+      <c r="H59" s="30" t="s">
+        <v>382</v>
+      </c>
+      <c r="I59" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="J59" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="K59" s="30" t="s">
+        <v>383</v>
+      </c>
+      <c r="L59" s="32"/>
+      <c r="M59" s="32"/>
+      <c r="N59" s="32"/>
+      <c r="O59" s="30" t="s">
+        <v>328</v>
+      </c>
+      <c r="P59" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q59" s="30" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="60" spans="1:17" ht="136" x14ac:dyDescent="0.2">
+      <c r="A60" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B60" s="30" t="s">
+        <v>357</v>
+      </c>
+      <c r="C60" s="30" t="s">
+        <v>385</v>
+      </c>
+      <c r="D60" s="30">
+        <v>2019</v>
+      </c>
+      <c r="E60" s="30" t="s">
+        <v>386</v>
+      </c>
+      <c r="F60" s="30" t="s">
+        <v>179</v>
+      </c>
+      <c r="G60" s="31" t="s">
+        <v>387</v>
+      </c>
+      <c r="H60" s="30" t="s">
+        <v>388</v>
+      </c>
+      <c r="I60" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="J60" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="K60" s="30" t="s">
+        <v>389</v>
+      </c>
+      <c r="L60" s="32"/>
+      <c r="M60" s="32"/>
+      <c r="N60" s="32"/>
+      <c r="O60" s="30" t="s">
+        <v>328</v>
+      </c>
+      <c r="P60" s="30" t="s">
+        <v>390</v>
+      </c>
+      <c r="Q60" s="30" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="61" spans="1:17" ht="119" x14ac:dyDescent="0.2">
+      <c r="A61" s="34" t="s">
+        <v>41</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="C61" s="34" t="s">
+        <v>392</v>
+      </c>
+      <c r="D61" s="34">
+        <v>2021</v>
+      </c>
+      <c r="E61" s="34" t="s">
+        <v>393</v>
+      </c>
+      <c r="F61" s="34" t="s">
+        <v>394</v>
+      </c>
+      <c r="G61" t="s">
+        <v>395</v>
+      </c>
+      <c r="H61" s="34"/>
+      <c r="I61" s="34"/>
+      <c r="J61" s="34"/>
+      <c r="K61" s="34" t="s">
+        <v>396</v>
+      </c>
+      <c r="L61" s="34"/>
+      <c r="M61" s="34"/>
+      <c r="N61" s="34"/>
+      <c r="O61" s="34" t="s">
+        <v>328</v>
+      </c>
+      <c r="P61" s="34" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q61" s="34"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:Q49 A50:G50 J50 L50:Q50 A51:Q53 A54:M54 O54:Q54 F55:G55 I55:Q55 A55:D56 F56:Q56 A57:Q57 A59:Q1048576 A58:D58 F58 H58:Q58">
-    <cfRule type="expression" dxfId="8" priority="5">
+  <conditionalFormatting sqref="A1:Q49 A50:G50 J50 L50:Q50 A51:Q53 A54:M54 O54:Q54 F55:G55 I55:Q55 A55:D56 F56:Q56 A57:Q57 A58:D58 F58 H58:Q58 A62:Q1048576 A59:A60 A61:F61 H61:Q61">
+    <cfRule type="expression" dxfId="9" priority="6">
       <formula>$A1="Does not quantify P availability and/or does not manipulate P fertilization"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="6">
+    <cfRule type="expression" dxfId="8" priority="7">
       <formula>$A1="P fertilization experiment that measures photosynthetic traits"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="7">
+    <cfRule type="expression" dxfId="7" priority="8">
       <formula>$A1="P fertilization experiment but does not measure photosynthetic traits"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="8">
+    <cfRule type="expression" dxfId="6" priority="9">
       <formula>$A1="Quantifies P availability"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E55:E56">
-    <cfRule type="expression" dxfId="4" priority="1">
+    <cfRule type="expression" dxfId="5" priority="2">
       <formula>$A55="Does not quantify P availability and/or does not manipulate P fertilization"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="2">
+    <cfRule type="expression" dxfId="4" priority="3">
       <formula>$A55="P fertilization experiment that measures photosynthetic traits"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="3">
+    <cfRule type="expression" dxfId="3" priority="4">
       <formula>$A55="P fertilization experiment but does not measure photosynthetic traits"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="4">
+    <cfRule type="expression" dxfId="2" priority="5">
       <formula>$A55="Quantifies P availability"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L59:N60">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>$A59="P fertilization experiment that measures photosynthetic traits"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
@@ -5110,11 +5371,11 @@
   <sheetPr>
     <tabColor theme="9" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:Q33"/>
+  <dimension ref="A1:Q35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E40" sqref="E40"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5135,1772 +5396,315 @@
     <col min="18" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="10" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:17" s="9" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A1" s="10" t="s">
         <v>365</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="10" t="s">
         <v>366</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="H1" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="I1" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="11" t="s">
+      <c r="J1" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="11" t="s">
+      <c r="K1" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="11" t="s">
+      <c r="L1" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="11" t="s">
+      <c r="M1" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="11" t="s">
+      <c r="N1" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="11" t="s">
+      <c r="O1" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="11" t="s">
+      <c r="P1" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="11" t="s">
+      <c r="Q1" s="10" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="85" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="str" cm="1">
-        <f t="array" ref="A2:Q33">_xlfn._xlws.FILTER(all_papers!A:Q, all_papers!A:A = "P fertilization experiment that measures photosynthetic traits")</f>
-        <v>P fertilization experiment that measures photosynthetic traits</v>
-      </c>
-      <c r="B2" s="2" t="str">
-        <v>evan</v>
-      </c>
-      <c r="C2" s="2" t="str">
-        <v>Verryckt et al.</v>
-      </c>
-      <c r="D2" s="2">
-        <v>2022</v>
-      </c>
-      <c r="E2" s="1" t="str">
-        <v>Vertical profiles of leaf photosynthesis and leaf traits and soil nutrients in two tropical rainforests in French Guiana before and after a 3-year nitrogen and phosphorus addition experiment</v>
-      </c>
-      <c r="F2" s="2" t="str">
-        <v>Earth System Science Data</v>
-      </c>
-      <c r="G2" s="2" t="str">
-        <v>https://doi.org/10.5194/essd-14-5-2022</v>
-      </c>
-      <c r="H2" s="1" t="str">
-        <v xml:space="preserve">Vcmax, Jmax, Asat, SLA,LAI, Nmass, Pmass </v>
-      </c>
-      <c r="I2" s="2" t="str">
-        <v>y</v>
-      </c>
-      <c r="J2" s="2" t="str">
-        <v>y</v>
-      </c>
-      <c r="K2" s="2" t="str">
-        <v>N, P, NP additions. Hand broadcasted urea and/or triple super phosphate at rate of 125 kg N per ha per yr or 50 kg P per ha per yr</v>
-      </c>
-      <c r="L2" s="2" t="str">
-        <v>y</v>
-      </c>
-      <c r="M2" s="2" t="str">
-        <v>y</v>
-      </c>
-      <c r="N2" s="2" t="str">
-        <v>bulk</v>
-      </c>
-      <c r="O2" s="2" t="str">
-        <v>field exp</v>
-      </c>
-      <c r="P2" s="2" t="str">
-        <v>y</v>
-      </c>
-      <c r="Q2" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" ht="68" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="str">
-        <v>P fertilization experiment that measures photosynthetic traits</v>
-      </c>
-      <c r="B3" s="2" t="str">
-        <v>evan</v>
-      </c>
-      <c r="C3" s="2" t="str">
-        <v>Denton et al.</v>
-      </c>
-      <c r="D3" s="2">
-        <v>2007</v>
-      </c>
-      <c r="E3" s="1" t="str">
-        <v>Banksia species (Proteaceae) from severely phosphorus-impoverished soils exhibit extreme efficiency in the use and remobilization of phosphorus</v>
-      </c>
-      <c r="F3" s="2" t="str">
-        <v>Plant, Cell &amp; Environment</v>
-      </c>
-      <c r="G3" s="2" t="str">
-        <v>https://doi.org/10.1111/j.1365-3040.2007.01733.x</v>
-      </c>
-      <c r="H3" s="1" t="str">
-        <v>Pmass, LMA, dry matter content, leaf lifespan, Parea, Amax_area, Amax_mass</v>
-      </c>
-      <c r="I3" s="2" t="str">
-        <v>n</v>
-      </c>
-      <c r="J3" s="2" t="str">
-        <v>n</v>
-      </c>
-      <c r="K3" s="2" t="str">
-        <v>n/a</v>
-      </c>
-      <c r="L3" s="2" t="str">
-        <v>n</v>
-      </c>
-      <c r="M3" s="2" t="str">
-        <v>y</v>
-      </c>
-      <c r="N3" s="2" t="str">
-        <v>Bulk P (ug/g) and bicarbonate extracable P (ug/g, though under detection limits in all spp)</v>
-      </c>
-      <c r="O3" s="2">
-        <v>0</v>
-      </c>
-      <c r="P3" s="2" t="str">
-        <v>n</v>
-      </c>
-      <c r="Q3" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" ht="68" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="str">
-        <v>P fertilization experiment that measures photosynthetic traits</v>
-      </c>
-      <c r="B4" s="2" t="str">
-        <v>evan</v>
-      </c>
-      <c r="C4" s="2" t="str">
-        <v>Jacob &amp; Lawlor</v>
-      </c>
-      <c r="D4" s="2">
-        <v>1993</v>
-      </c>
-      <c r="E4" s="1" t="str">
-        <v>In vivo photosynthetic electron transport does not limit photosynthetic capacity in phosphate-deficient sunflower and maize leaves</v>
-      </c>
-      <c r="F4" s="2" t="str">
-        <v>Plant, Cell &amp; Environment</v>
-      </c>
-      <c r="G4" s="2" t="str">
-        <v>https://doi.org/10.1111/j.1365-3040.1993.tb00500.x</v>
-      </c>
-      <c r="H4" s="1" t="str">
-        <v>chlorophyll fluorescence, snapshot gas exchange (anet, presumably stomatal conductance as well?)</v>
-      </c>
-      <c r="I4" s="2" t="str">
-        <v>n</v>
-      </c>
-      <c r="J4" s="2" t="str">
-        <v>y</v>
-      </c>
-      <c r="K4" s="2" t="str">
-        <v>P addition experiment with either 0 or 10 mol/m3 Pi</v>
-      </c>
-      <c r="L4" s="2" t="str">
-        <v>n</v>
-      </c>
-      <c r="M4" s="2" t="str">
-        <v>n</v>
-      </c>
-      <c r="N4" s="2">
-        <v>0</v>
-      </c>
-      <c r="O4" s="2">
-        <v>0</v>
-      </c>
-      <c r="P4" s="2" t="str">
-        <v>n</v>
-      </c>
-      <c r="Q4" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" ht="136" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="str">
-        <v>P fertilization experiment that measures photosynthetic traits</v>
-      </c>
-      <c r="B5" s="2" t="str">
-        <v>evan</v>
-      </c>
-      <c r="C5" s="2" t="str">
-        <v>Campbell &amp; Sage (2006)</v>
-      </c>
-      <c r="D5" s="2">
-        <v>2006</v>
-      </c>
-      <c r="E5" s="1" t="str">
-        <v>Interactions between the effects of atmospheric CO2 content and P nutrition on photosynthesis in white lupin (Lupinus albus L.)</v>
-      </c>
-      <c r="F5" s="2" t="str">
-        <v>Plant, Cell &amp; Environment</v>
-      </c>
-      <c r="G5" s="2" t="str">
-        <v>https://doi.org/10.1111/j.1365-3040.2005.01464.x</v>
-      </c>
-      <c r="H5" s="1" t="str">
-        <v>net photosynthesis, stomatal conductance, leaf Ci:Ca, Vcmax (Vc, predicted rate of carboxylation), Jmax, Rubisco activity, Rubisco content, chlorophyll content, chlorophyll fluorescence, SLA, Nmass, Narea, Pmass, leaf C:N</v>
-      </c>
-      <c r="I5" s="2" t="str">
-        <v>n</v>
-      </c>
-      <c r="J5" s="2" t="str">
-        <v>y</v>
-      </c>
-      <c r="K5" s="2" t="str">
-        <v>P addition experiment with either 0.69μm or 250μm P. Plants grown under 200, 400 or 750ppm CO2</v>
-      </c>
-      <c r="L5" s="2" t="str">
-        <v>n</v>
-      </c>
-      <c r="M5" s="2" t="str">
-        <v>n</v>
-      </c>
-      <c r="N5" s="2" t="str">
-        <v>n/a</v>
-      </c>
-      <c r="O5" s="2">
-        <v>0</v>
-      </c>
-      <c r="P5" s="2" t="str">
-        <v>n</v>
-      </c>
-      <c r="Q5" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" ht="68" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="str">
-        <v>P fertilization experiment that measures photosynthetic traits</v>
-      </c>
-      <c r="B6" s="2" t="str">
-        <v>evan</v>
-      </c>
-      <c r="C6" s="2" t="str">
-        <v>Xia et al.</v>
-      </c>
-      <c r="D6" s="2">
-        <v>2024</v>
-      </c>
-      <c r="E6" s="1" t="str">
-        <v>Enhancing alfalfa photosynthetic performance through arbuscular mycorrhizal fungi incoulation across varied phosphorus application levels</v>
-      </c>
-      <c r="F6" s="2" t="str">
-        <v>Frontiers in Plant Science</v>
-      </c>
-      <c r="G6" s="2" t="str">
-        <v>https://doi.org/10.3389/fpls.2023.1256084</v>
-      </c>
-      <c r="H6" s="1" t="str">
-        <v>net photosynthesis, stomatal conductance, chlorophyll content, Ci, LUE, WUE,</v>
-      </c>
-      <c r="I6" s="2" t="str">
-        <v>n</v>
-      </c>
-      <c r="J6" s="2" t="str">
-        <v>y</v>
-      </c>
-      <c r="K6" s="2" t="str">
-        <v>P addition experiment with 4 levels: 0 P2O5, 50 P2O5, 100 P2O5, 150 P2O5 (all mg/kg)</v>
-      </c>
-      <c r="L6" s="2" t="str">
-        <v>y</v>
-      </c>
-      <c r="M6" s="2" t="str">
-        <v>y</v>
-      </c>
-      <c r="N6" s="2" t="str">
-        <v>alkaline nitrogen (mg/kg), available phosphorus (mg/kg), total phosphorus (g/kg)</v>
-      </c>
-      <c r="O6" s="2">
-        <v>0</v>
-      </c>
-      <c r="P6" s="2" t="str">
-        <v>n</v>
-      </c>
-      <c r="Q6" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" ht="68" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="str">
-        <v>P fertilization experiment that measures photosynthetic traits</v>
-      </c>
-      <c r="B7" s="2" t="str">
-        <v>evan</v>
-      </c>
-      <c r="C7" s="2" t="str">
-        <v>Chtouki et al.</v>
-      </c>
-      <c r="D7" s="2">
-        <v>2022</v>
-      </c>
-      <c r="E7" s="1" t="str">
-        <v>Interactive effect of soil moisture content and phosphorus fertilizer form on chickpea growth, photosynthesis, and nutrient uptake</v>
-      </c>
-      <c r="F7" s="2" t="str">
-        <v>Scientific Reports</v>
-      </c>
-      <c r="G7" s="2" t="str">
-        <v>https://doi.org/10.1038/s41598-022-10703-0</v>
-      </c>
-      <c r="H7" s="1" t="str">
-        <v>stomatal density, stomatal conductance, chlorophyll content (SPAD), SLA, Puptake, P use efficiency, root:shoot ratio</v>
-      </c>
-      <c r="I7" s="2" t="str">
-        <v>n</v>
-      </c>
-      <c r="J7" s="2" t="str">
-        <v>y</v>
-      </c>
-      <c r="K7" s="2" t="str">
-        <v>P addition experiment with either 0 mg P2O5 per kg dry soil or 16 mg P2O5 per kg dry soil. Soil moisture also manipulated at 25, 50, and 75% of field capacity</v>
-      </c>
-      <c r="L7" s="2" t="str">
-        <v>y</v>
-      </c>
-      <c r="M7" s="2" t="str">
-        <v>y</v>
-      </c>
-      <c r="N7" s="2" t="str">
-        <v>0.9 g/kg of total nitrogen, 26 mg/kg of Olsen-P background soils (not including fertilizer</v>
-      </c>
-      <c r="O7" s="2">
-        <v>0</v>
-      </c>
-      <c r="P7" s="2" t="str">
-        <v>n; contact author for raw files ~_~</v>
-      </c>
-      <c r="Q7" s="2" t="str">
-        <v>photosynthesis not measured</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" ht="72.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="str">
-        <v>P fertilization experiment that measures photosynthetic traits</v>
-      </c>
-      <c r="B8" s="2" t="str">
-        <v>evan</v>
-      </c>
-      <c r="C8" s="2" t="str">
-        <v>Zavišić et al.</v>
-      </c>
-      <c r="D8" s="2">
-        <v>2018</v>
-      </c>
-      <c r="E8" s="1" t="str">
-        <v>Forest soil phosphorus resources and fertilization affect ectomycorrhizal community composition, beech P updake efficiency, and photosynthesis</v>
-      </c>
-      <c r="F8" s="2" t="str">
-        <v>Frontiers in Plant Science</v>
-      </c>
-      <c r="G8" s="2" t="str">
-        <v xml:space="preserve">https://doi.org/10.3389/fpls.2018.00463 </v>
-      </c>
-      <c r="H8" s="1" t="str">
-        <v>net photosynthesis, stomatal conductance, iWUE, Ci, Puptake, Puptake rate, organ P content, P uptake efficiency</v>
-      </c>
-      <c r="I8" s="2" t="str">
-        <v>n</v>
-      </c>
-      <c r="J8" s="2" t="str">
-        <v>y</v>
-      </c>
-      <c r="K8" s="2" t="str">
-        <v>P addition experiment. Beech trees excavated in P-poor and P-rich forests. P added as triple superphosphate at single dose of 795mg P2O5, or 0 mg P2O5 (control)</v>
-      </c>
-      <c r="L8" s="2" t="str">
-        <v>n</v>
-      </c>
-      <c r="M8" s="2" t="str">
-        <v>y</v>
-      </c>
-      <c r="N8" s="2" t="str">
-        <v>Plabile calculated using malachite green reaction (mg/g)</v>
-      </c>
-      <c r="O8" s="2">
-        <v>0</v>
-      </c>
-      <c r="P8" s="2" t="str">
-        <v>n; contact author for raw files ~_~</v>
-      </c>
-      <c r="Q8" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" ht="68" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="str">
-        <v>P fertilization experiment that measures photosynthetic traits</v>
-      </c>
-      <c r="B9" s="2" t="str">
-        <v>evan</v>
-      </c>
-      <c r="C9" s="2" t="str">
-        <v>Chen et al.</v>
-      </c>
-      <c r="D9" s="2">
-        <v>2024</v>
-      </c>
-      <c r="E9" s="1" t="str">
-        <v>Enhancing photosynthetic phosphorus-use efficiency through coordination of leaf phosphorus fractions, allocation, and anatomy during soybean domestication</v>
-      </c>
-      <c r="F9" s="2" t="str">
-        <v>Journal of Experimental Botany</v>
-      </c>
-      <c r="G9" s="2" t="str">
-        <v>https://doi.org/10.1093/jxb/erae427</v>
-      </c>
-      <c r="H9" s="1" t="str">
-        <v>net photosynthesis, SPAD, LMA, Amass, PPUE, leaf thickness, inorganic leaf P fraction, organic leaf P fraction</v>
-      </c>
-      <c r="I9" s="2" t="str">
-        <v>y</v>
-      </c>
-      <c r="J9" s="2" t="str">
-        <v>y</v>
-      </c>
-      <c r="K9" s="2" t="str">
-        <v>P addition experiment with either no P addition or 40 ug P/g dry soil supplied as KH2PO4. N supplied at 188 ugN/g and K supplied as 27.9 ug K/g. N and K supplied similarly between P treatments</v>
-      </c>
-      <c r="L9" s="2" t="str">
-        <v>n</v>
-      </c>
-      <c r="M9" s="2" t="str">
-        <v>y</v>
-      </c>
-      <c r="N9" s="2" t="str">
-        <v>Olsen P: 2.2 ug P/g plant-available soil P as background soil P</v>
-      </c>
-      <c r="O9" s="2">
-        <v>0</v>
-      </c>
-      <c r="P9" s="2" t="str">
-        <v>n; contact author for raw files ~_~</v>
-      </c>
-      <c r="Q9" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" ht="68" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="str">
-        <v>P fertilization experiment that measures photosynthetic traits</v>
-      </c>
-      <c r="B10" s="2" t="str">
-        <v>evan</v>
-      </c>
-      <c r="C10" s="2" t="str">
-        <v>Syvertsen &amp; Graham</v>
-      </c>
-      <c r="D10" s="2">
-        <v>1999</v>
-      </c>
-      <c r="E10" s="1" t="str">
-        <v>Phosphorus supply and aurbuscular mycorrhizas increase growth and net gas exchange responses of two Citrus spp. grown at elevated [CO2]</v>
-      </c>
-      <c r="F10" s="2" t="str">
-        <v>Plant and Soil</v>
-      </c>
-      <c r="G10" s="2" t="str">
-        <v>https://doi.org/10.1023/A:1004553315041</v>
-      </c>
-      <c r="H10" s="1" t="str">
-        <v>net photosynthesis, total plant dry weight, root weight, shoot weight, root weight ratio, leaf starch, Parea, Narea, leaf C:N</v>
-      </c>
-      <c r="I10" s="2" t="str">
-        <v>n</v>
-      </c>
-      <c r="J10" s="2" t="str">
-        <v>y</v>
-      </c>
-      <c r="K10" s="2" t="str">
-        <v>P addition experiment with either no P addition or 2 mM P as a modified Hoagland's solution. P added in full factorial design with 2 CO2 levels and 2 AMF treatments</v>
-      </c>
-      <c r="L10" s="2" t="str">
-        <v>n</v>
-      </c>
-      <c r="M10" s="2" t="str">
-        <v>y</v>
-      </c>
-      <c r="N10" s="2" t="str">
-        <v>Background soil P concentration: 4 mg/kg available P</v>
-      </c>
-      <c r="O10" s="2">
-        <v>0</v>
-      </c>
-      <c r="P10" s="2" t="str">
-        <v>n</v>
-      </c>
-      <c r="Q10" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" ht="51" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="str">
-        <v>P fertilization experiment that measures photosynthetic traits</v>
-      </c>
-      <c r="B11" s="2" t="str">
-        <v>evan</v>
-      </c>
-      <c r="C11" s="2" t="str">
-        <v>Mo et al.</v>
-      </c>
-      <c r="D11" s="2">
-        <v>2021</v>
-      </c>
-      <c r="E11" s="1" t="str">
-        <v>Response of foliar mineral nutrients to long-term nitrogen and phosphorus addition in a tropical forest</v>
-      </c>
-      <c r="F11" s="2" t="str">
-        <v>Functional Ecology</v>
-      </c>
-      <c r="G11" s="2" t="str">
-        <v>https://doi.org/10.1111/1365-2435.13896</v>
-      </c>
-      <c r="H11" s="1" t="str">
-        <v>Nmass, Pmass, transpiration, water use efficiency</v>
-      </c>
-      <c r="I11" s="2" t="str">
-        <v>y</v>
-      </c>
-      <c r="J11" s="2" t="str">
-        <v>y</v>
-      </c>
-      <c r="K11" s="2" t="str">
-        <v>N, P, NP additions. N added annually at 100 kg N/ha/yr as Nh4No3 and P was added at 100 kg P/ha/yr as Na2HPO4</v>
-      </c>
-      <c r="L11" s="2" t="str">
-        <v>y</v>
-      </c>
-      <c r="M11" s="2" t="str">
-        <v>y</v>
-      </c>
-      <c r="N11" s="2" t="str">
-        <v>atmospheric N deposition is 40 kg N/ha at study site. total N (g/kg), total P (g/kg), plant-available P (mg/kg)</v>
-      </c>
-      <c r="O11" s="2">
-        <v>0</v>
-      </c>
-      <c r="P11" s="2" t="str">
-        <v>y, but doi is not active/found</v>
-      </c>
-      <c r="Q11" s="2" t="str">
-        <v>Measured leaf transpiration and WUE using an LI-6400- presumably net photosynthesis, stomatal conductance and other snapshot measures are also quantified?</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" ht="51" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="str">
-        <v>P fertilization experiment that measures photosynthetic traits</v>
-      </c>
-      <c r="B12" s="2" t="str">
-        <v>evan</v>
-      </c>
-      <c r="C12" s="2" t="str">
-        <v>Jiang et al.</v>
-      </c>
-      <c r="D12" s="2">
-        <v>2020</v>
-      </c>
-      <c r="E12" s="1" t="str">
-        <v>Low phosphorus supply constrains plant responses to elevated CO2: a meta-analysis</v>
-      </c>
-      <c r="F12" s="2" t="str">
-        <v>Global Change Biology</v>
-      </c>
-      <c r="G12" s="2" t="str">
-        <v>https://doi.org/10.1111/gcb.15277</v>
-      </c>
-      <c r="H12" s="1" t="str">
-        <v>Anet, stomatal conductance, iWUE, LMA, Nuptake, Puptake, PNUE, PPUE</v>
-      </c>
-      <c r="I12" s="2" t="str">
-        <v>n</v>
-      </c>
-      <c r="J12" s="2" t="str">
-        <v>y</v>
-      </c>
-      <c r="K12" s="2" t="str">
-        <v>varies across experiments</v>
-      </c>
-      <c r="L12" s="2">
-        <v>0</v>
-      </c>
-      <c r="M12" s="2">
-        <v>0</v>
-      </c>
-      <c r="N12" s="2">
-        <v>0</v>
-      </c>
-      <c r="O12" s="2" t="str">
-        <v>meta-analysis</v>
-      </c>
-      <c r="P12" s="2" t="str">
-        <v>y</v>
-      </c>
-      <c r="Q12" s="2" t="str">
-        <v>Meta-analysis of 45 studies</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" ht="119" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="str">
-        <v>P fertilization experiment that measures photosynthetic traits</v>
-      </c>
-      <c r="B13" s="2" t="str">
-        <v>evan</v>
-      </c>
-      <c r="C13" s="2" t="str">
-        <v>Singh et al.</v>
-      </c>
-      <c r="D13" s="2">
-        <v>2014</v>
-      </c>
-      <c r="E13" s="1" t="str">
-        <v>Growth, nutrient dynamics, and efficiency responses to carbon dioxide and phosphorus nutrition in soybean</v>
-      </c>
-      <c r="F13" s="2" t="str">
-        <v>Journal of Plant Interactions</v>
-      </c>
-      <c r="G13" s="2" t="str">
-        <v>https://doi.org/10.1080/17429145.2014.959570</v>
-      </c>
-      <c r="H13" s="1" t="str">
-        <v>total leaf area, total biomass, allocation partitioning, net photosynthesis, stomatal conductance, Ci, chlorophyll content (Chlarea), total N and P content of organs, PUE, NUE, PUPE, NUPE, Pmass, Nmass</v>
-      </c>
-      <c r="I13" s="2" t="str">
-        <v>n</v>
-      </c>
-      <c r="J13" s="2" t="str">
-        <v>y</v>
-      </c>
-      <c r="K13" s="2" t="str">
-        <v>P addition experiment with three P levels: 0.5 mM Pi, 0.1 mM Pi, or 0.01 mM Pi as a modified Hoagland's solution. Plants also grown under two CO2 levels</v>
-      </c>
-      <c r="L13" s="2" t="str">
-        <v>n</v>
-      </c>
-      <c r="M13" s="2" t="str">
-        <v>n</v>
-      </c>
-      <c r="N13" s="2" t="str">
-        <v>n/a</v>
-      </c>
-      <c r="O13" s="2">
-        <v>0</v>
-      </c>
-      <c r="P13" s="2" t="str">
-        <v>y, but only treatment means</v>
-      </c>
-      <c r="Q13" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" ht="51" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="str">
-        <v>P fertilization experiment that measures photosynthetic traits</v>
-      </c>
-      <c r="B14" s="2" t="str">
-        <v>evan</v>
-      </c>
-      <c r="C14" s="2" t="str">
-        <v>Conroy et al.</v>
-      </c>
-      <c r="D14" s="2">
-        <v>1990</v>
-      </c>
-      <c r="E14" s="1" t="str">
-        <v>Increases in phosphorus requirements for CO2-enriched pine species</v>
-      </c>
-      <c r="F14" s="2" t="str">
-        <v>Plant Physiology</v>
-      </c>
-      <c r="G14" s="2" t="str">
-        <v>https://doi.org/10.1104/pp.92.4.977</v>
-      </c>
-      <c r="H14" s="1" t="str">
-        <v>shoot dry weight, stem:foliage ratio, net photosynthesis, chlorophyll fluorescence,</v>
-      </c>
-      <c r="I14" s="2" t="str">
-        <v>n</v>
-      </c>
-      <c r="J14" s="2" t="str">
-        <v>y</v>
-      </c>
-      <c r="K14" s="2" t="str">
-        <v>P addition experiment with 7 levels: 0, 46, 92, 182, 274, 456, 1368 mg/kg as CaHPO4. Supplemental soluble P was added at 5 mg/kg as NH4H2PO4 for all treatments at week 2 and added on a regular basis to the P4, P5, and P6 treatments. Plants alsow grown under two CO2 levels</v>
-      </c>
-      <c r="L14" s="2" t="str">
-        <v>y</v>
-      </c>
-      <c r="M14" s="2" t="str">
-        <v>y</v>
-      </c>
-      <c r="N14" s="2" t="str">
-        <v>see citation in paper for background soil N/P values</v>
-      </c>
-      <c r="O14" s="2">
-        <v>0</v>
-      </c>
-      <c r="P14" s="2" t="str">
-        <v>n</v>
-      </c>
-      <c r="Q14" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" ht="68" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="str">
-        <v>P fertilization experiment that measures photosynthetic traits</v>
-      </c>
-      <c r="B15" s="2" t="str">
-        <v>evan</v>
-      </c>
-      <c r="C15" s="2" t="str">
-        <v>Crous et al.</v>
-      </c>
-      <c r="D15" s="2">
-        <v>2017</v>
-      </c>
-      <c r="E15" s="1" t="str">
-        <v>Nitrogen and phosphorus availabilities interact to modulate leaf trait scaling relationships across six plant functional types in a controlled-environment study</v>
-      </c>
-      <c r="F15" s="2" t="str">
-        <v>New Phytologist</v>
-      </c>
-      <c r="G15" s="2" t="str">
-        <v>https://doi.org/10.1111/nph.14591</v>
-      </c>
-      <c r="H15" s="1" t="str">
-        <v>net photosynthesis, Nmass, Pmass, Narea, Parea, Rdark, Rlight, LMA,</v>
-      </c>
-      <c r="I15" s="2" t="str">
-        <v>y</v>
-      </c>
-      <c r="J15" s="2" t="str">
-        <v>y</v>
-      </c>
-      <c r="K15" s="2" t="str">
-        <v>N, P, NP additions.Two N levels (0.4 mM, 5 mM), two P levels (2μM, 1 mM), full factorial design. Nutrients added as a modified Hoagland's solution</v>
-      </c>
-      <c r="L15" s="2" t="str">
-        <v>n</v>
-      </c>
-      <c r="M15" s="2" t="str">
-        <v>n</v>
-      </c>
-      <c r="N15" s="2" t="str">
-        <v>Background soil N and P not realistic as plants were potted in sterilized sand</v>
-      </c>
-      <c r="O15" s="2">
-        <v>0</v>
-      </c>
-      <c r="P15" s="2" t="str">
-        <v>y, treatment means listed in supplement</v>
-      </c>
-      <c r="Q15" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" ht="68" x14ac:dyDescent="0.2">
-      <c r="A16" s="2" t="str">
-        <v>P fertilization experiment that measures photosynthetic traits</v>
-      </c>
-      <c r="B16" s="2" t="str">
-        <v>evan</v>
-      </c>
-      <c r="C16" s="2" t="str">
-        <v>Bloomfield et al.</v>
-      </c>
-      <c r="D16" s="2">
-        <v>2014</v>
-      </c>
-      <c r="E16" s="1" t="str">
-        <v>Photosynthesis-nitrogen relationships in tropical forest tree species as affected by soil phosphorus availability: a controlled environment study</v>
-      </c>
-      <c r="F16" s="2" t="str">
-        <v>Functional Plant Biology</v>
-      </c>
-      <c r="G16" s="2" t="str">
-        <v>https://doi.org/10.1071/FP13278</v>
-      </c>
-      <c r="H16" s="1" t="str">
-        <v>Anet, Amax, Vcmax, Jmax, LMA, Nmass, Pmass, PNUE, PPUE, Narea, Parea,</v>
-      </c>
-      <c r="I16" s="2" t="str">
-        <v>n</v>
-      </c>
-      <c r="J16" s="2" t="str">
-        <v>y</v>
-      </c>
-      <c r="K16" s="2" t="str">
-        <v>P addition experiment with 2 levels: 0P and a 1/3 strength Hewitt's olution (0.44 mM NaH2PO4 as P addition substrate). 0P solution also as modified Hewitt's solution, but without NaH2PO4)</v>
-      </c>
-      <c r="L16" s="2" t="str">
-        <v>y</v>
-      </c>
-      <c r="M16" s="2" t="str">
-        <v>y</v>
-      </c>
-      <c r="N16" s="2" t="str">
-        <v>Purchased seedlings were growing in high nutrient potting mix (17.6N : 2.9P : 6.9K % + trace elements). Potting mix retained for exp</v>
-      </c>
-      <c r="O16" s="2">
-        <v>0</v>
-      </c>
-      <c r="P16" s="2" t="str">
-        <v>n</v>
-      </c>
-      <c r="Q16" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" ht="68" x14ac:dyDescent="0.2">
-      <c r="A17" s="2" t="str">
-        <v>P fertilization experiment that measures photosynthetic traits</v>
-      </c>
-      <c r="B17" s="2" t="str">
-        <v>evan</v>
-      </c>
-      <c r="C17" s="2" t="str">
-        <v>Bown et al.</v>
-      </c>
-      <c r="D17" s="2">
-        <v>2007</v>
-      </c>
-      <c r="E17" s="1" t="str">
-        <v>Partitioning concurrent influences of nitrogen and phosphorus supply on photosynthetic model parameters of Pinus radiata</v>
-      </c>
-      <c r="F17" s="2" t="str">
-        <v>Tree Physiology</v>
-      </c>
-      <c r="G17" s="2" t="str">
-        <v>https://doi.org/10.1093/treephys/27.3.335</v>
-      </c>
-      <c r="H17" s="1" t="str">
-        <v>Anet, stomatal conductance, Vcmax, Jmax, TPU, Narea, Parea, leaf N:P, SLA, stomatal limitation to photosynthesis</v>
-      </c>
-      <c r="I17" s="2" t="str">
-        <v>y</v>
-      </c>
-      <c r="J17" s="2" t="str">
-        <v>y</v>
-      </c>
-      <c r="K17" s="2" t="str">
-        <v>N, P, NP additions. N added as 1.43 mM N or 7.14 mM N; P added as 0.084 mM N or 0.42 mM N. Plants received 0.5 dm3 of nutrient solution per week</v>
-      </c>
-      <c r="L17" s="2" t="str">
-        <v>n</v>
-      </c>
-      <c r="M17" s="2" t="str">
-        <v>n</v>
-      </c>
-      <c r="N17" s="2" t="str">
-        <v>n/a</v>
-      </c>
-      <c r="O17" s="2">
-        <v>0</v>
-      </c>
-      <c r="P17" s="2" t="str">
-        <v>y, treatment means listed in tables</v>
-      </c>
-      <c r="Q17" s="2" t="str">
-        <v>used in Walker et al. (2014)</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17" ht="51" x14ac:dyDescent="0.2">
-      <c r="A18" s="2" t="str">
-        <v>P fertilization experiment that measures photosynthetic traits</v>
-      </c>
-      <c r="B18" s="2" t="str">
-        <v>evan</v>
-      </c>
-      <c r="C18" s="2" t="str">
-        <v>Carswell et al.</v>
-      </c>
-      <c r="D18" s="2">
-        <v>2005</v>
-      </c>
-      <c r="E18" s="1" t="str">
-        <v>Plasticity in photosynthetic responses to nutrient supply of seedlings from a mixed conifer-angiosperm forest</v>
-      </c>
-      <c r="F18" s="2" t="str">
-        <v>Austral Ecology</v>
-      </c>
-      <c r="G18" s="2" t="str">
-        <v>https://doi.org/10.1111/j.1442-9993.2005.01486.x</v>
-      </c>
-      <c r="H18" s="1" t="str">
-        <v>Nmass, Narea, Pmass, Parea, Amax, Vcmax, Jmax, PNUE, PPUE,</v>
-      </c>
-      <c r="I18" s="2" t="str">
-        <v>y</v>
-      </c>
-      <c r="J18" s="2" t="str">
-        <v>y</v>
-      </c>
-      <c r="K18" s="2" t="str">
-        <v>N, P, NP additions. N added as 0.5 mM or 5 mM NH4NO3, P added as 0.133 mM or 1.33 mM Na2HPO4*2H2O. All other nutrients kept constant across treatments</v>
-      </c>
-      <c r="L18" s="2" t="str">
-        <v>n</v>
-      </c>
-      <c r="M18" s="2" t="str">
-        <v>n</v>
-      </c>
-      <c r="N18" s="2" t="str">
-        <v>n/a</v>
-      </c>
-      <c r="O18" s="2">
-        <v>0</v>
-      </c>
-      <c r="P18" s="2" t="str">
-        <v>y, treatment means listed in tables</v>
-      </c>
-      <c r="Q18" s="2" t="str">
-        <v>used in Walker et al. (2014)</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17" ht="34" x14ac:dyDescent="0.2">
-      <c r="A19" s="2" t="str">
-        <v>P fertilization experiment that measures photosynthetic traits</v>
-      </c>
-      <c r="B19" s="2" t="str">
-        <v>evan</v>
-      </c>
-      <c r="C19" s="2" t="str">
-        <v>Warren &amp; Adams</v>
-      </c>
-      <c r="D19" s="2">
-        <v>2002</v>
-      </c>
-      <c r="E19" s="1" t="str">
-        <v>Phosphorus affects growth and paritioning of nitrogen to Rubisco in Pinus pinaster</v>
-      </c>
-      <c r="F19" s="2" t="str">
-        <v>Tree Physiology</v>
-      </c>
-      <c r="G19" s="2" t="str">
-        <v>https://doi.org/10.1093/treephys/22.1.11</v>
-      </c>
-      <c r="H19" s="1" t="str">
-        <v>Amax, Nmass, Pmass, Pi, Rubisco content, chlorophyll content</v>
-      </c>
-      <c r="I19" s="2" t="str">
-        <v>y</v>
-      </c>
-      <c r="J19" s="2" t="str">
-        <v>y</v>
-      </c>
-      <c r="K19" s="2" t="str">
-        <v>N, P, NP additions both in greenhouse. N added as 0.125 mM or 2.0 mM as ammonium or nitrate (?), P added as 0.02 mM, 0.08 mM, or 0.34 mM H2PO4</v>
-      </c>
-      <c r="L19" s="2" t="str">
-        <v>n</v>
-      </c>
-      <c r="M19" s="2" t="str">
-        <v>n</v>
-      </c>
-      <c r="N19" s="2" t="str">
-        <v>n/a</v>
-      </c>
-      <c r="O19" s="2">
-        <v>0</v>
-      </c>
-      <c r="P19" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q19" s="2" t="str">
-        <v>greenhouse experiment part of paper</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17" ht="34" x14ac:dyDescent="0.2">
-      <c r="A20" s="2" t="str">
-        <v>P fertilization experiment that measures photosynthetic traits</v>
-      </c>
-      <c r="B20" s="2" t="str">
-        <v>evan</v>
-      </c>
-      <c r="C20" s="2" t="str">
-        <v>Warren &amp; Adams</v>
-      </c>
-      <c r="D20" s="2">
-        <v>2002</v>
-      </c>
-      <c r="E20" s="1" t="str">
-        <v>Phosphorus affects growth and paritioning of nitrogen to Rubisco in Pinus pinaster</v>
-      </c>
-      <c r="F20" s="2" t="str">
-        <v>Tree Physiology</v>
-      </c>
-      <c r="G20" s="2" t="str">
-        <v>https://doi.org/10.1093/treephys/22.1.11</v>
-      </c>
-      <c r="H20" s="1" t="str">
-        <v>Amax, Nmass, Pmass, Pi, Rubisco content, chlorophyll content</v>
-      </c>
-      <c r="I20" s="2" t="str">
-        <v>n</v>
-      </c>
-      <c r="J20" s="2" t="str">
-        <v>y</v>
-      </c>
-      <c r="K20" s="2" t="str">
-        <v>P added at five rates as double super fosphate (0, 35, 70, 105, 140, 175 kg/ha) with similar doses of N, K, and other macronutrients across plots also added</v>
-      </c>
-      <c r="L20" s="2" t="str">
-        <v>n</v>
-      </c>
-      <c r="M20" s="2" t="str">
-        <v>n</v>
-      </c>
-      <c r="N20" s="2" t="str">
-        <v>n/a</v>
-      </c>
-      <c r="O20" s="2">
-        <v>0</v>
-      </c>
-      <c r="P20" s="2" t="str">
-        <v>treatment means in table, might be available by reaching out to authors</v>
-      </c>
-      <c r="Q20" s="2" t="str">
-        <v>field experiment part of paper</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17" ht="85" x14ac:dyDescent="0.2">
-      <c r="A21" s="2" t="str">
-        <v>P fertilization experiment that measures photosynthetic traits</v>
-      </c>
-      <c r="B21" s="2" t="str">
-        <v>evan</v>
-      </c>
-      <c r="C21" s="2" t="str">
-        <v>Mo et al.</v>
-      </c>
-      <c r="D21" s="2">
+      <c r="A2" s="2" t="e" cm="1" vm="1">
+        <f t="array" aca="1" ref="A2" ca="1">_xlfn._xlws.FILTER(all_papers!A:Q, all_papers!A:A = "P fertilization experiment that measures photosynthetic traits")</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" ht="68" x14ac:dyDescent="0.2"/>
+    <row r="4" spans="1:17" ht="68" x14ac:dyDescent="0.2"/>
+    <row r="5" spans="1:17" ht="136" x14ac:dyDescent="0.2"/>
+    <row r="6" spans="1:17" ht="68" x14ac:dyDescent="0.2"/>
+    <row r="7" spans="1:17" ht="68" x14ac:dyDescent="0.2"/>
+    <row r="8" spans="1:17" ht="72.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="9" spans="1:17" ht="68" x14ac:dyDescent="0.2"/>
+    <row r="10" spans="1:17" ht="68" x14ac:dyDescent="0.2"/>
+    <row r="11" spans="1:17" ht="51" x14ac:dyDescent="0.2"/>
+    <row r="12" spans="1:17" ht="51" x14ac:dyDescent="0.2"/>
+    <row r="13" spans="1:17" ht="119" x14ac:dyDescent="0.2"/>
+    <row r="14" spans="1:17" ht="51" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="1:17" ht="68" x14ac:dyDescent="0.2"/>
+    <row r="16" spans="1:17" ht="68" x14ac:dyDescent="0.2"/>
+    <row r="17" spans="1:17" ht="68" x14ac:dyDescent="0.2"/>
+    <row r="18" spans="1:17" ht="51" x14ac:dyDescent="0.2"/>
+    <row r="19" spans="1:17" ht="34" x14ac:dyDescent="0.2"/>
+    <row r="20" spans="1:17" ht="34" x14ac:dyDescent="0.2"/>
+    <row r="21" spans="1:17" ht="85" x14ac:dyDescent="0.2"/>
+    <row r="22" spans="1:17" ht="102" x14ac:dyDescent="0.2">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
+      <c r="L22" s="1"/>
+      <c r="M22" s="1"/>
+      <c r="N22" s="1"/>
+      <c r="O22" s="1"/>
+      <c r="P22" s="1"/>
+      <c r="Q22" s="1"/>
+    </row>
+    <row r="23" spans="1:17" ht="119" x14ac:dyDescent="0.2">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
+      <c r="L23" s="1"/>
+      <c r="M23" s="1"/>
+      <c r="N23" s="1"/>
+      <c r="O23" s="1"/>
+      <c r="P23" s="1"/>
+      <c r="Q23" s="1"/>
+    </row>
+    <row r="24" spans="1:17" ht="85" x14ac:dyDescent="0.2">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+      <c r="K24" s="1"/>
+      <c r="L24" s="1"/>
+      <c r="M24" s="1"/>
+      <c r="N24" s="1"/>
+      <c r="O24" s="1"/>
+      <c r="P24" s="1"/>
+      <c r="Q24" s="1"/>
+    </row>
+    <row r="25" spans="1:17" ht="119" x14ac:dyDescent="0.2">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
+      <c r="K25" s="1"/>
+      <c r="L25" s="1"/>
+      <c r="M25" s="1"/>
+      <c r="N25" s="1"/>
+      <c r="O25" s="1"/>
+      <c r="P25" s="1"/>
+      <c r="Q25" s="1"/>
+    </row>
+    <row r="26" spans="1:17" ht="153" x14ac:dyDescent="0.2">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
+      <c r="K26" s="1"/>
+      <c r="L26" s="1"/>
+      <c r="M26" s="1"/>
+      <c r="N26" s="1"/>
+      <c r="O26" s="1"/>
+      <c r="P26" s="1"/>
+      <c r="Q26" s="1"/>
+    </row>
+    <row r="27" spans="1:17" ht="85" x14ac:dyDescent="0.2">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="I27" s="1"/>
+      <c r="J27" s="1"/>
+      <c r="K27" s="1"/>
+      <c r="L27" s="1"/>
+      <c r="M27" s="1"/>
+      <c r="N27" s="1"/>
+      <c r="O27" s="1"/>
+      <c r="P27" s="1"/>
+      <c r="Q27" s="1"/>
+    </row>
+    <row r="28" spans="1:17" ht="136" x14ac:dyDescent="0.2">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="I28" s="1"/>
+      <c r="J28" s="1"/>
+      <c r="K28" s="1"/>
+      <c r="L28" s="1"/>
+      <c r="M28" s="1"/>
+      <c r="N28" s="1"/>
+      <c r="O28" s="1"/>
+      <c r="P28" s="1"/>
+      <c r="Q28" s="1"/>
+    </row>
+    <row r="29" spans="1:17" ht="85" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:17" ht="68" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:17" ht="51" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:17" ht="51" x14ac:dyDescent="0.2"/>
+    <row r="33" spans="1:17" ht="51" x14ac:dyDescent="0.2">
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
+      <c r="I33" s="1"/>
+      <c r="J33" s="1"/>
+      <c r="K33" s="1"/>
+      <c r="L33" s="1"/>
+      <c r="M33" s="1"/>
+      <c r="N33" s="1"/>
+      <c r="O33" s="1"/>
+      <c r="P33" s="1"/>
+      <c r="Q33" s="1"/>
+    </row>
+    <row r="34" spans="1:17" s="33" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A34" s="30"/>
+      <c r="B34" s="30" t="s">
+        <v>357</v>
+      </c>
+      <c r="C34" s="30" t="s">
+        <v>378</v>
+      </c>
+      <c r="D34" s="30">
         <v>2019</v>
       </c>
-      <c r="E21" s="1" t="str">
-        <v>Foliar phosphorus fractions reveal how tropical plants maintain photosynthetic rates despite low soil phosphorus availability</v>
-      </c>
-      <c r="F21" s="2" t="str">
-        <v>Functional Ecology</v>
-      </c>
-      <c r="G21" s="2" t="str">
-        <v>https://doi.org/10.1111/1365-2435.13252</v>
-      </c>
-      <c r="H21" s="1" t="str">
-        <v>net photosynthesis, PPUE, PNUE, LMA, Nmass, Pmass, leaf P fractional pools (structural, metabolic, nucleic acid, residual P)</v>
-      </c>
-      <c r="I21" s="2" t="str">
-        <v>y</v>
-      </c>
-      <c r="J21" s="2" t="str">
-        <v>y</v>
-      </c>
-      <c r="K21" s="2" t="str">
-        <v>N, P, NP additions. N: 100 kg N/ha/yr as NH4NO3, P: 100 kg P/ha/yr as Na2HPO4</v>
-      </c>
-      <c r="L21" s="2" t="str">
-        <v>y</v>
-      </c>
-      <c r="M21" s="2" t="str">
-        <v>y</v>
-      </c>
-      <c r="N21" s="2" t="str">
-        <v>Nitrate-N (mg/kg), ammonium-N (mg/kg), total N (g/kg), total P (g/kg), available P (mg/kg)</v>
-      </c>
-      <c r="O21" s="2">
-        <v>0</v>
-      </c>
-      <c r="P21" s="2" t="str">
-        <v>y</v>
-      </c>
-      <c r="Q21" s="2" t="str">
-        <v>presumably also stomatal conductance data if gas exchange data were collected. Can also calculate Narea and Parea given that LMA was also measured</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" ht="102" x14ac:dyDescent="0.2">
-      <c r="A22" s="1" t="str">
-        <v>P fertilization experiment that measures photosynthetic traits</v>
-      </c>
-      <c r="B22" s="1" t="str">
-        <v>evan</v>
-      </c>
-      <c r="C22" s="1" t="str">
-        <v>Lauer et al.</v>
-      </c>
-      <c r="D22" s="1">
-        <v>1989</v>
-      </c>
-      <c r="E22" s="1" t="str">
-        <v>Whole leaf carbon exchange characteristics of phosphate deficient soybeans (Glycine max L.</v>
-      </c>
-      <c r="F22" s="1" t="str">
-        <v>Plant Physiology</v>
-      </c>
-      <c r="G22" s="1" t="str">
-        <v>https://doi.org/10.1104/pp.91.3.848</v>
-      </c>
-      <c r="H22" s="1" t="str">
-        <v>Anet, stomatal conductance, stomatal limitation, Vcmax (termed carboxylation efficiency), Ci, Rubisco content, specific Rubisco activity, chlorophylll content, SLA</v>
-      </c>
-      <c r="I22" s="1" t="str">
-        <v>n</v>
-      </c>
-      <c r="J22" s="1" t="str">
-        <v>y</v>
-      </c>
-      <c r="K22" s="1" t="str">
-        <v>Two P levels: 0.05 mM Pi or 0.50 mM Pi as H2HPO4 (from Lauer et al. 1989b)</v>
-      </c>
-      <c r="L22" s="1" t="str">
-        <v>n</v>
-      </c>
-      <c r="M22" s="1" t="str">
-        <v>n</v>
-      </c>
-      <c r="N22" s="1" t="str">
-        <v>n/a</v>
-      </c>
-      <c r="O22" s="1">
-        <v>0</v>
-      </c>
-      <c r="P22" s="1" t="str">
-        <v>y, but only treatment means</v>
-      </c>
-      <c r="Q22" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17" ht="119" x14ac:dyDescent="0.2">
-      <c r="A23" s="1" t="str">
-        <v>P fertilization experiment that measures photosynthetic traits</v>
-      </c>
-      <c r="B23" s="1" t="str">
-        <v>monika</v>
-      </c>
-      <c r="C23" s="1" t="str">
-        <v>Barrett &amp; Gifford</v>
-      </c>
-      <c r="D23" s="1">
-        <v>1995</v>
-      </c>
-      <c r="E23" s="1" t="str">
-        <v>Acclimation of photosynthesis and growth by cotton to elevated CO2: interactions with severe phosphate deficiency and restricted rooting volume</v>
-      </c>
-      <c r="F23" s="1" t="str">
-        <v>Australian Journal of Plant Physiology</v>
-      </c>
-      <c r="G23" s="1" t="str">
-        <v>https://doi.org/10.1071/PP9950955</v>
-      </c>
-      <c r="H23" s="1" t="str">
-        <v>Vcmax, LMA, RGR, NARS (net assimilation rate), LARS (leaf area ratios), C and P concentrations (total?), P uptake efficiency, P uptake per unit root mass, P utilisation efficiency, total soluble carbohydrates and starch</v>
-      </c>
-      <c r="I23" s="1" t="str">
-        <v>n</v>
-      </c>
-      <c r="J23" s="1" t="str">
-        <v>y</v>
-      </c>
-      <c r="K23" s="1" t="str">
-        <v>three P levels: 2.1, 6.1, 18.2 (mg P plant-1)</v>
-      </c>
-      <c r="L23" s="1" t="str">
-        <v>n</v>
-      </c>
-      <c r="M23" s="1">
-        <v>0</v>
-      </c>
-      <c r="N23" s="1">
-        <v>0</v>
-      </c>
-      <c r="O23" s="1" t="str">
-        <v>growth chambers</v>
-      </c>
-      <c r="P23" s="1" t="str">
-        <v>n</v>
-      </c>
-      <c r="Q23" s="1" t="str">
-        <v>Three CO2 concentrations (376, 652 and 935 μmol mol-1), and varying pot volumes. 
-old data set unlikely to be available (paper and website mention nothing about data availablity)</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17" ht="85" x14ac:dyDescent="0.2">
-      <c r="A24" s="1" t="str">
-        <v>P fertilization experiment that measures photosynthetic traits</v>
-      </c>
-      <c r="B24" s="1" t="str">
-        <v>evan</v>
-      </c>
-      <c r="C24" s="1" t="str">
-        <v>Singh et al.</v>
-      </c>
-      <c r="D24" s="1">
+      <c r="E34" s="30" t="s">
+        <v>379</v>
+      </c>
+      <c r="F34" s="30" t="s">
+        <v>380</v>
+      </c>
+      <c r="G34" s="31" t="s">
+        <v>381</v>
+      </c>
+      <c r="H34" s="30" t="s">
+        <v>382</v>
+      </c>
+      <c r="I34" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="J34" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="K34" s="30" t="s">
+        <v>383</v>
+      </c>
+      <c r="L34" s="32"/>
+      <c r="M34" s="32"/>
+      <c r="N34" s="32"/>
+      <c r="O34" s="30" t="s">
+        <v>328</v>
+      </c>
+      <c r="P34" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q34" s="30" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" s="33" customFormat="1" ht="136" x14ac:dyDescent="0.2">
+      <c r="A35" s="30"/>
+      <c r="B35" s="30" t="s">
+        <v>357</v>
+      </c>
+      <c r="C35" s="30" t="s">
+        <v>385</v>
+      </c>
+      <c r="D35" s="30">
         <v>2019</v>
       </c>
-      <c r="E24" s="1" t="str">
-        <v>Interactive effects of temperature and phosphorus nutrition on soybean: leaf photosynthesis, chlorophyll fluorescence, and nutrient efficiency</v>
-      </c>
-      <c r="F24" s="1" t="str">
-        <v>Photosynthetica</v>
-      </c>
-      <c r="G24" s="1" t="str">
-        <v>10.32615/ps.2019.036</v>
-      </c>
-      <c r="H24" s="1">
-        <v>0</v>
-      </c>
-      <c r="I24" s="1">
-        <v>0</v>
-      </c>
-      <c r="J24" s="1">
-        <v>0</v>
-      </c>
-      <c r="K24" s="1">
-        <v>0</v>
-      </c>
-      <c r="L24" s="1">
-        <v>0</v>
-      </c>
-      <c r="M24" s="1">
-        <v>0</v>
-      </c>
-      <c r="N24" s="1">
-        <v>0</v>
-      </c>
-      <c r="O24" s="1">
-        <v>0</v>
-      </c>
-      <c r="P24" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q24" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17" ht="119" x14ac:dyDescent="0.2">
-      <c r="A25" s="1" t="str">
-        <v>P fertilization experiment that measures photosynthetic traits</v>
-      </c>
-      <c r="B25" s="1" t="str">
-        <v>evan</v>
-      </c>
-      <c r="C25" s="1" t="str">
-        <v>Warren &amp; Adams</v>
-      </c>
-      <c r="D25" s="1">
-        <v>2011</v>
-      </c>
-      <c r="E25" s="1" t="str">
-        <v>How does P affect photosynthesis and metabolite profiles of Eucalyptus globulus?</v>
-      </c>
-      <c r="F25" s="1" t="str">
-        <v>Tree Physiology</v>
-      </c>
-      <c r="G25" s="1" t="str">
-        <v>https://doi.org/10.1093/treephys/tpr064</v>
-      </c>
-      <c r="H25" s="1" t="str">
-        <v>Narea, Parea, leaf N:P, Amax, gsw, Vcmax, J, TPU</v>
-      </c>
-      <c r="I25" s="1" t="str">
-        <v>n</v>
-      </c>
-      <c r="J25" s="1" t="str">
-        <v>y</v>
-      </c>
-      <c r="K25" s="1" t="str">
-        <v xml:space="preserve">P added at four concentrations as equimolar K2HPO4 and KH2PO4: 0, 0.005, 0.02, 0.1 mM P) </v>
-      </c>
-      <c r="L25" s="1" t="str">
-        <v>n</v>
-      </c>
-      <c r="M25" s="1" t="str">
-        <v>n</v>
-      </c>
-      <c r="N25" s="1" t="str">
-        <v>n/a</v>
-      </c>
-      <c r="O25" s="1" t="str">
-        <v>greenhouse</v>
-      </c>
-      <c r="P25" s="1" t="str">
-        <v>n; treatment mean and standard errors in text</v>
-      </c>
-      <c r="Q25" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:17" ht="153" x14ac:dyDescent="0.2">
-      <c r="A26" s="1" t="str">
-        <v>P fertilization experiment that measures photosynthetic traits</v>
-      </c>
-      <c r="B26" s="1" t="str">
-        <v>Huiying</v>
-      </c>
-      <c r="C26" s="1" t="str">
-        <v>Yu et al.</v>
-      </c>
-      <c r="D26" s="1">
-        <v>2022</v>
-      </c>
-      <c r="E26" s="1" t="str">
-        <v>Foliar phosphorus allocation and photosynthesis reveal plants' adaptative strategies to phosphorus limitation in tropical forests at different successional stages</v>
-      </c>
-      <c r="F26" s="1" t="str">
-        <v>Science of Total Environment</v>
-      </c>
-      <c r="G26" s="1" t="str">
-        <v>https://doi.org/10.1016/j.scitotenv.2022.157456</v>
-      </c>
-      <c r="H26" s="1" t="str">
-        <v>Amax, gsw, chlorophyll content, LA, LT, LDMC, SLA, PNUE, PPUE, leaf C, N &amp; P, leaf P allocated to four parts</v>
-      </c>
-      <c r="I26" s="1" t="str">
-        <v>y</v>
-      </c>
-      <c r="J26" s="1" t="str">
-        <v>y</v>
-      </c>
-      <c r="K26" s="1" t="str">
-        <v>N addition (N50, 50 kg N ha−1 yr−1), P addition (P50, 50 kg P ha−1 yr−1), and NP addition (N50P50, 50 kg N ha−1 yr−1 + 50 kg P ha−1 yr−1). N and P were added in the forms of NH4NO3 and Ca(H2PO4)2 dissolved in 30 L of water</v>
-      </c>
-      <c r="L26" s="1" t="str">
-        <v>y</v>
-      </c>
-      <c r="M26" s="1" t="str">
-        <v>y</v>
-      </c>
-      <c r="N26" s="1">
-        <v>0</v>
-      </c>
-      <c r="O26" s="1">
-        <v>0</v>
-      </c>
-      <c r="P26" s="1" t="str">
-        <v>y</v>
-      </c>
-      <c r="Q26" s="1" t="str">
-        <v>Data will be made available on request; leaf nutrient data are extractable from Table 2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:17" ht="85" x14ac:dyDescent="0.2">
-      <c r="A27" s="1" t="str">
-        <v>P fertilization experiment that measures photosynthetic traits</v>
-      </c>
-      <c r="B27" s="1" t="str">
-        <v>monika</v>
-      </c>
-      <c r="C27" s="1" t="str">
-        <v>Cheng et al.</v>
-      </c>
-      <c r="D27" s="1">
-        <v>2014</v>
-      </c>
-      <c r="E27" s="1" t="str">
-        <v>Interactions between light intensity and phosphorus nutrition affect the phosphate-mining capacity of white lupin (Lupinus albus L.)</v>
-      </c>
-      <c r="F27" s="1" t="str">
-        <v>Journal of Experimental Botany</v>
-      </c>
-      <c r="G27" s="1" t="str">
-        <v>https://doi.org/10.1093/jxb/eru135</v>
-      </c>
-      <c r="H27" s="1" t="str">
-        <v>Cluster roots, root length &amp; surface area, Net photosynthetic rate (Pn), P concentraiton of roots and shoots, root exudates, RNA</v>
-      </c>
-      <c r="I27" s="1" t="str">
-        <v>n</v>
-      </c>
-      <c r="J27" s="1" t="str">
-        <v>y</v>
-      </c>
-      <c r="K27" s="1" t="str">
-        <v>P supplied at 1  µM (P deficiency) or 50  µM (P sufficienct). P supplied at KH2PO4</v>
-      </c>
-      <c r="L27" s="1" t="str">
-        <v>y</v>
-      </c>
-      <c r="M27" s="1" t="str">
-        <v>y</v>
-      </c>
-      <c r="N27" s="1" t="str">
-        <v>N: 2000 µM Ca(NO3), 0.01 µM (NH4)6Mo7O24 . 
-P: 50 µM and 1 µM as KH2PO4</v>
-      </c>
-      <c r="O27" s="1" t="str">
-        <v>growth chambers</v>
-      </c>
-      <c r="P27" s="1" t="str">
-        <v>n</v>
-      </c>
-      <c r="Q27" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:17" ht="136" x14ac:dyDescent="0.2">
-      <c r="A28" s="1" t="str">
-        <v>P fertilization experiment that measures photosynthetic traits</v>
-      </c>
-      <c r="B28" s="1" t="str">
-        <v>monika</v>
-      </c>
-      <c r="C28" s="1" t="str">
-        <v>Zhao et al.</v>
-      </c>
-      <c r="D28" s="1">
-        <v>2022</v>
-      </c>
-      <c r="E28" s="1" t="str">
-        <v>Phosphate fertilizers increase CO2 assimilation and yield of soybean in a shaded environment</v>
-      </c>
-      <c r="F28" s="1" t="str">
-        <v>Photosynthetica</v>
-      </c>
-      <c r="G28" s="1" t="str">
-        <v>https://ps.ueb.cas.cz/pdfs/phs/2022/02/01.pdf</v>
-      </c>
-      <c r="H28" s="1" t="str">
-        <v>Net photosynthetic rate  - light intensity curves, chlorophyll fluorescence</v>
-      </c>
-      <c r="I28" s="1" t="str">
-        <v>n</v>
-      </c>
-      <c r="J28" s="1" t="str">
-        <v>y</v>
-      </c>
-      <c r="K28" s="1" t="str">
-        <v>two P concentrations: 
-P1, 0 kg(P2O5) ha-1; 
-P2, 180 kg(P2O5) ha-1</v>
-      </c>
-      <c r="L28" s="1" t="str">
-        <v>y</v>
-      </c>
-      <c r="M28" s="1" t="str">
-        <v>y</v>
-      </c>
-      <c r="N28" s="1" t="str">
-        <v>within the 0–20 cm soil depth were: 12.53 g(soil organic
-carbon) kg−1, 1.15 g(soil total nitrogen) kg−1, 11.27
-mg(available phosphorus) kg−1, 0.68 g(total phosphorus)
-kg–1, 80.9 mg(available potassium) kg–1, and pH of 6.8</v>
-      </c>
-      <c r="O28" s="1" t="str">
-        <v>field</v>
-      </c>
-      <c r="P28" s="1" t="str">
-        <v>unsure
-Might have to reach out to authors for data</v>
-      </c>
-      <c r="Q28" s="1" t="str">
-        <v xml:space="preserve">two light treatments, ambient sunlight, and 40% shade.
-</v>
-      </c>
-    </row>
-    <row r="29" spans="1:17" ht="85" x14ac:dyDescent="0.2">
-      <c r="A29" s="2" t="str">
-        <v>P fertilization experiment that measures photosynthetic traits</v>
-      </c>
-      <c r="B29" s="2" t="str">
-        <v>Huiying</v>
-      </c>
-      <c r="C29" s="2" t="str">
-        <v xml:space="preserve">Xiaodong Wang </v>
-      </c>
-      <c r="D29" s="2">
-        <v>2024</v>
-      </c>
-      <c r="E29" s="1" t="str">
-        <v>The effect of phosphorus addition on the rhizosphere process and root and leaf traits for dominant tree species of Schima superba and Castanopsis fargesii in an evergreen broad-leaved forest</v>
-      </c>
-      <c r="F29" s="2" t="str">
-        <v>PhD thesis</v>
-      </c>
-      <c r="G29" s="2" t="str">
-        <v>https://tlink.lib.tsinghua.edu.cn/https/443/net/cnki/kns/yitlink/kcms2/article/abstract?v=UjEBX92ALNEtsjI9aefwRwj3YlLSAn5S1mkrShM31qMg1m9eqwXAOt7cj_iUZx_i4zJvZMveBPwSdwZThRTNbN-OM_WtlD3iOxh54hvZMuiAhMSnnlr2H12FVws-ptRip7CsrKCIUCpQ-Yh0hHsWj1qltYOtjS0xfYmDH2eWfH8BqqmAUV_yT4kOe2swxvCe&amp;uniplatform=NZKPT&amp;language=CHS</v>
-      </c>
-      <c r="H29" s="1" t="str">
-        <v>chlorophyll content; PNUE; Vcmax; Jmax; gs; A; iWUE</v>
-      </c>
-      <c r="I29" s="2" t="str">
-        <v>n</v>
-      </c>
-      <c r="J29" s="2" t="str">
-        <v>y</v>
-      </c>
-      <c r="K29" s="2" t="str">
-        <v>50 kg P ha-1 a-1</v>
-      </c>
-      <c r="L29" s="2" t="str">
-        <v>y</v>
-      </c>
-      <c r="M29" s="2" t="str">
-        <v>y</v>
-      </c>
-      <c r="N29" s="2" t="str">
-        <v>NaH2PO4 was applied in March and Sept</v>
-      </c>
-      <c r="O29" s="2" t="str">
-        <v>field</v>
-      </c>
-      <c r="P29" s="2" t="str">
-        <v>unsure
-having trouble finding paper, help</v>
-      </c>
-      <c r="Q29" s="2" t="str">
-        <v>can be extracted from figure, mean and se. 
-Having trouble finding paper, help! - Monika</v>
-      </c>
-    </row>
-    <row r="30" spans="1:17" ht="68" x14ac:dyDescent="0.2">
-      <c r="A30" s="2" t="str">
-        <v>P fertilization experiment that measures photosynthetic traits</v>
-      </c>
-      <c r="B30" s="2" t="str">
-        <v>Huiying</v>
-      </c>
-      <c r="C30" s="2" t="str">
-        <v>Ma et al.</v>
-      </c>
-      <c r="D30" s="2">
-        <v>2023</v>
-      </c>
-      <c r="E30" s="1" t="str">
-        <v>Effects of Nitrogen and Phosphorus Addition on Photosynthetic Characteristics and Antioxidant System of Suaeda salsa in the Yellow River Delta</v>
-      </c>
-      <c r="F30" s="2" t="str">
-        <v>Journal of Yunnan Agricultural University</v>
-      </c>
-      <c r="G30" s="2" t="str">
-        <v>10.12101/j.issn.1004-390X(n).202209020</v>
-      </c>
-      <c r="H30" s="1" t="str">
-        <v>chlorophyll content; Anet; gs; ci; WUE</v>
-      </c>
-      <c r="I30" s="2" t="str">
-        <v>y</v>
-      </c>
-      <c r="J30" s="2" t="str">
-        <v>y</v>
-      </c>
-      <c r="K30" s="2">
-        <v>0</v>
-      </c>
-      <c r="L30" s="2" t="str">
-        <v>y</v>
-      </c>
-      <c r="M30" s="2" t="str">
-        <v>y</v>
-      </c>
-      <c r="N30" s="2" t="str">
-        <v>N0, N5, N15, N45 are  0, 5, 15 and 45 g/m2; P0 and P1 are 0 and 1g/m2; N5P0、N15P0, N45P0, N0P1, N5P1, N15P1, N45P1, N0P0</v>
-      </c>
-      <c r="O30" s="2" t="str">
-        <v>field</v>
-      </c>
-      <c r="P30" s="2" t="str">
-        <v>part available
-having trouble finding paper, help</v>
-      </c>
-      <c r="Q30" s="2" t="str">
-        <v xml:space="preserve">can be extracted from figure, </v>
-      </c>
-    </row>
-    <row r="31" spans="1:17" ht="51" x14ac:dyDescent="0.2">
-      <c r="A31" s="2" t="str">
-        <v>P fertilization experiment that measures photosynthetic traits</v>
-      </c>
-      <c r="B31" s="2" t="str">
-        <v>Jan</v>
-      </c>
-      <c r="C31" s="2" t="str">
-        <v>S. Wang et al</v>
-      </c>
-      <c r="D31" s="2">
-        <v>2020</v>
-      </c>
-      <c r="E31" s="1" t="str">
-        <v>Source and sink activity of Holcus lanatus in response to absolute and relative supply of nitrogen and phosphorus</v>
-      </c>
-      <c r="F31" s="2" t="str">
-        <v>Functional Plant Biology</v>
-      </c>
-      <c r="G31" s="2" t="str">
-        <v>DOI: 10.1071/FP20118</v>
-      </c>
-      <c r="H31" s="1" t="str">
-        <v xml:space="preserve">Amax, SLA, </v>
-      </c>
-      <c r="I31" s="2" t="str">
-        <v>y</v>
-      </c>
-      <c r="J31" s="2" t="str">
-        <v>y</v>
-      </c>
-      <c r="K31" s="2" t="str">
-        <v xml:space="preserve">three N:P ratio's, two absolute levels. </v>
-      </c>
-      <c r="L31" s="2" t="str">
-        <v>n</v>
-      </c>
-      <c r="M31" s="2" t="str">
-        <v>n</v>
-      </c>
-      <c r="N31" s="2" t="str">
-        <v>N: low:30, 52, 90, 90, 156, 270 (mg)
-P: 6, 3.5, 2, 18, 10.5, 6 (mg)</v>
-      </c>
-      <c r="O31" s="2" t="str">
-        <v>greenhouse</v>
-      </c>
-      <c r="P31" s="2" t="str">
-        <v>n</v>
-      </c>
-      <c r="Q31" s="2" t="str">
-        <v>Maybe ask Hugo</v>
-      </c>
-    </row>
-    <row r="32" spans="1:17" ht="51" x14ac:dyDescent="0.2">
-      <c r="A32" s="2" t="str">
-        <v>P fertilization experiment that measures photosynthetic traits</v>
-      </c>
-      <c r="B32" s="2" t="str">
-        <v>Evan</v>
-      </c>
-      <c r="C32" s="2" t="str">
-        <v>Fan et al.</v>
-      </c>
-      <c r="D32" s="2">
-        <v>2024</v>
-      </c>
-      <c r="E32" s="1" t="str">
-        <v>Variation in leaf phosphorus fractions reflects plant adaptations and distribution in low-phosphorus tropical forests</v>
-      </c>
-      <c r="F32" s="2" t="str">
-        <v>Functional Ecology</v>
-      </c>
-      <c r="G32" s="2" t="str">
-        <v>https://doi.org/10.1111/1365-2435.14721</v>
-      </c>
-      <c r="H32" s="1" t="str">
-        <v>LMA, Nmass, Pmass, RGR, Amax, Vcmax, Jmax, PPUE, PNUE, leaf phosphorus fractions</v>
-      </c>
-      <c r="I32" s="2" t="str">
-        <v>n</v>
-      </c>
-      <c r="J32" s="2" t="str">
-        <v>y</v>
-      </c>
-      <c r="K32" s="2" t="str">
-        <v>40 mg/kg P as NaH2PO4*H2O and a control (no P addition)</v>
-      </c>
-      <c r="L32" s="2" t="str">
-        <v>y</v>
-      </c>
-      <c r="M32" s="2" t="str">
-        <v>y</v>
-      </c>
-      <c r="N32" s="2" t="str">
-        <v>g/kg</v>
-      </c>
-      <c r="O32" s="2" t="str">
-        <v>field</v>
-      </c>
-      <c r="P32" s="2" t="str">
-        <v>y</v>
-      </c>
-      <c r="Q32" s="2" t="str">
-        <v>really ideal dataset for this meta analysis!</v>
-      </c>
-    </row>
-    <row r="33" spans="1:17" ht="51" x14ac:dyDescent="0.2">
-      <c r="A33" s="2" t="str">
-        <v>P fertilization experiment that measures photosynthetic traits</v>
-      </c>
-      <c r="B33" s="2" t="str">
-        <v>Evan</v>
-      </c>
-      <c r="C33" s="1" t="str">
-        <v>Firn et al.</v>
-      </c>
-      <c r="D33" s="1">
-        <v>2019</v>
-      </c>
-      <c r="E33" s="1" t="str">
-        <v>Leaf nutrients, not specific leaf area, are consistent indicators of elevated nutrient inputs</v>
-      </c>
-      <c r="F33" s="1" t="str">
-        <v>Nature Ecology and Evoluation</v>
-      </c>
-      <c r="G33" s="1" t="str">
-        <v>https://doi.org/10.1038/s41559-018-0790-1</v>
-      </c>
-      <c r="H33" s="1" t="str">
-        <v>LMA (through SLA), Nmass, Pmass. Can use LMA to calculate Narea and Parea</v>
-      </c>
-      <c r="I33" s="1" t="str">
-        <v>y</v>
-      </c>
-      <c r="J33" s="1" t="str">
-        <v>y</v>
-      </c>
-      <c r="K33" s="1">
-        <v>0</v>
-      </c>
-      <c r="L33" s="1" t="str">
-        <v>y</v>
-      </c>
-      <c r="M33" s="1" t="str">
-        <v>y</v>
-      </c>
-      <c r="N33" s="1">
-        <v>0</v>
-      </c>
-      <c r="O33" s="1" t="str">
-        <v>field</v>
-      </c>
-      <c r="P33" s="1" t="str">
-        <v>y</v>
-      </c>
-      <c r="Q33" s="1">
-        <v>0</v>
+      <c r="E35" s="30" t="s">
+        <v>386</v>
+      </c>
+      <c r="F35" s="30" t="s">
+        <v>179</v>
+      </c>
+      <c r="G35" s="31" t="s">
+        <v>387</v>
+      </c>
+      <c r="H35" s="30" t="s">
+        <v>388</v>
+      </c>
+      <c r="I35" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="J35" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="K35" s="30" t="s">
+        <v>389</v>
+      </c>
+      <c r="L35" s="32"/>
+      <c r="M35" s="32"/>
+      <c r="N35" s="32"/>
+      <c r="O35" s="30" t="s">
+        <v>328</v>
+      </c>
+      <c r="P35" s="30" t="s">
+        <v>390</v>
+      </c>
+      <c r="Q35" s="30" t="s">
+        <v>391</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:Q1048576">
-    <cfRule type="expression" dxfId="0" priority="1">
+  <conditionalFormatting sqref="A1:Q33 A36:Q1048576 L34:N35">
+    <cfRule type="expression" dxfId="1" priority="1">
       <formula>$A1="P fertilization experiment that measures photosynthetic traits"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
add plots to digitize, start code for digitization
</commit_message>
<xml_diff>
--- a/lit_search_np_fert_exps.xlsx
+++ b/lit_search_np_fert_exps.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10112"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
   <workbookPr updateLinks="always"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eaperkowski/git/p_meta/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCE44919-EDFA-3A45-8029-100645321FD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{940DB49B-D5E0-264B-B87F-B928F3DA7ACB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51140" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{50492CE8-F5C0-524A-968F-FD9EC2022F6C}"/>
+    <workbookView minimized="1" xWindow="1520" yWindow="500" windowWidth="49680" windowHeight="28300" xr2:uid="{50492CE8-F5C0-524A-968F-FD9EC2022F6C}"/>
   </bookViews>
   <sheets>
     <sheet name="all_papers" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">p_fert_papers!$A$1:$Q$1</definedName>
   </definedNames>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1517,7 +1517,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1606,20 +1606,11 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2293,10 +2284,10 @@
   <dimension ref="A1:S61"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B58" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B56" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B63" sqref="B63"/>
+      <selection pane="bottomRight" activeCell="G61" sqref="G61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3329,7 +3320,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:17" ht="170" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:17" ht="153" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>41</v>
       </c>
@@ -5167,9 +5158,6 @@
       <c r="K59" s="30" t="s">
         <v>383</v>
       </c>
-      <c r="L59" s="32"/>
-      <c r="M59" s="32"/>
-      <c r="N59" s="32"/>
       <c r="O59" s="30" t="s">
         <v>328</v>
       </c>
@@ -5214,9 +5202,6 @@
       <c r="K60" s="30" t="s">
         <v>389</v>
       </c>
-      <c r="L60" s="32"/>
-      <c r="M60" s="32"/>
-      <c r="N60" s="32"/>
       <c r="O60" s="30" t="s">
         <v>328</v>
       </c>
@@ -5228,46 +5213,46 @@
       </c>
     </row>
     <row r="61" spans="1:17" ht="119" x14ac:dyDescent="0.2">
-      <c r="A61" s="34" t="s">
+      <c r="A61" s="1" t="s">
         <v>41</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>357</v>
       </c>
-      <c r="C61" s="34" t="s">
+      <c r="C61" s="1" t="s">
         <v>392</v>
       </c>
-      <c r="D61" s="34">
+      <c r="D61" s="1">
         <v>2021</v>
       </c>
-      <c r="E61" s="34" t="s">
+      <c r="E61" s="1" t="s">
         <v>393</v>
       </c>
-      <c r="F61" s="34" t="s">
+      <c r="F61" s="1" t="s">
         <v>394</v>
       </c>
       <c r="G61" t="s">
         <v>395</v>
       </c>
-      <c r="H61" s="34"/>
-      <c r="I61" s="34"/>
-      <c r="J61" s="34"/>
-      <c r="K61" s="34" t="s">
+      <c r="H61" s="1"/>
+      <c r="I61" s="1"/>
+      <c r="J61" s="1"/>
+      <c r="K61" s="1" t="s">
         <v>396</v>
       </c>
-      <c r="L61" s="34"/>
-      <c r="M61" s="34"/>
-      <c r="N61" s="34"/>
-      <c r="O61" s="34" t="s">
+      <c r="L61" s="1"/>
+      <c r="M61" s="1"/>
+      <c r="N61" s="1"/>
+      <c r="O61" s="1" t="s">
         <v>328</v>
       </c>
-      <c r="P61" s="34" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q61" s="34"/>
+      <c r="P61" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q61" s="1"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:Q49 A50:G50 J50 L50:Q50 A51:Q53 A54:M54 O54:Q54 F55:G55 I55:Q55 A55:D56 F56:Q56 A57:Q57 A58:D58 F58 H58:Q58 A62:Q1048576 A59:A60 A61:F61 H61:Q61">
+  <conditionalFormatting sqref="A1:Q49 A50:G50 J50 L50:Q50 A51:Q53 A54:M54 O54:Q54 F55:G55 I55:Q55 A55:D56 F56:Q56 A57:Q57 A58:D58 F58 H58:Q58 A59:A60 A61:F61 H61:Q61 A62:Q1048576">
     <cfRule type="expression" dxfId="9" priority="6">
       <formula>$A1="Does not quantify P availability and/or does not manipulate P fertilization"</formula>
     </cfRule>
@@ -5296,7 +5281,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L59:N60">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="1" priority="1">
       <formula>$A59="P fertilization experiment that measures photosynthetic traits"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5491,7 +5476,7 @@
       <c r="P22" s="1"/>
       <c r="Q22" s="1"/>
     </row>
-    <row r="23" spans="1:17" ht="119" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -5508,7 +5493,7 @@
       <c r="P23" s="1"/>
       <c r="Q23" s="1"/>
     </row>
-    <row r="24" spans="1:17" ht="85" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -5525,7 +5510,7 @@
       <c r="P24" s="1"/>
       <c r="Q24" s="1"/>
     </row>
-    <row r="25" spans="1:17" ht="119" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -5542,7 +5527,7 @@
       <c r="P25" s="1"/>
       <c r="Q25" s="1"/>
     </row>
-    <row r="26" spans="1:17" ht="153" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -5559,7 +5544,7 @@
       <c r="P26" s="1"/>
       <c r="Q26" s="1"/>
     </row>
-    <row r="27" spans="1:17" ht="85" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -5576,7 +5561,7 @@
       <c r="P27" s="1"/>
       <c r="Q27" s="1"/>
     </row>
-    <row r="28" spans="1:17" ht="136" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -5593,11 +5578,7 @@
       <c r="P28" s="1"/>
       <c r="Q28" s="1"/>
     </row>
-    <row r="29" spans="1:17" ht="85" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="1:17" ht="68" x14ac:dyDescent="0.2"/>
-    <row r="31" spans="1:17" ht="51" x14ac:dyDescent="0.2"/>
-    <row r="32" spans="1:17" ht="51" x14ac:dyDescent="0.2"/>
-    <row r="33" spans="1:17" ht="51" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.2">
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
       <c r="F33" s="1"/>
@@ -5612,7 +5593,7 @@
       <c r="P33" s="1"/>
       <c r="Q33" s="1"/>
     </row>
-    <row r="34" spans="1:17" s="33" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:17" ht="51" x14ac:dyDescent="0.2">
       <c r="A34" s="30"/>
       <c r="B34" s="30" t="s">
         <v>357</v>
@@ -5644,9 +5625,6 @@
       <c r="K34" s="30" t="s">
         <v>383</v>
       </c>
-      <c r="L34" s="32"/>
-      <c r="M34" s="32"/>
-      <c r="N34" s="32"/>
       <c r="O34" s="30" t="s">
         <v>328</v>
       </c>
@@ -5657,7 +5635,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="35" spans="1:17" s="33" customFormat="1" ht="136" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:17" ht="136" x14ac:dyDescent="0.2">
       <c r="A35" s="30"/>
       <c r="B35" s="30" t="s">
         <v>357</v>
@@ -5689,9 +5667,6 @@
       <c r="K35" s="30" t="s">
         <v>389</v>
       </c>
-      <c r="L35" s="32"/>
-      <c r="M35" s="32"/>
-      <c r="N35" s="32"/>
       <c r="O35" s="30" t="s">
         <v>328</v>
       </c>
@@ -5703,8 +5678,8 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:Q33 A36:Q1048576 L34:N35">
-    <cfRule type="expression" dxfId="1" priority="1">
+  <conditionalFormatting sqref="A1:Q33 L34:N35 A36:Q1048576">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>$A1="P fertilization experiment that measures photosynthetic traits"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
start writing methods section, backcalculate total biomass from cleland 2019, add digitized data into script, convert meta-analysis to .R instead of .Rmd for easy work
</commit_message>
<xml_diff>
--- a/lit_search_np_fert_exps.xlsx
+++ b/lit_search_np_fert_exps.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eaperkowski/git/p_meta/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{940DB49B-D5E0-264B-B87F-B928F3DA7ACB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85B66616-665D-9448-867D-24A2E6C4A62F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="1520" yWindow="500" windowWidth="49680" windowHeight="28300" xr2:uid="{50492CE8-F5C0-524A-968F-FD9EC2022F6C}"/>
+    <workbookView xWindow="9420" yWindow="16060" windowWidth="49540" windowHeight="28300" xr2:uid="{50492CE8-F5C0-524A-968F-FD9EC2022F6C}"/>
   </bookViews>
   <sheets>
     <sheet name="all_papers" sheetId="1" r:id="rId1"/>
@@ -2287,7 +2287,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B56" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G61" sqref="G61"/>
+      <selection pane="bottomRight" activeCell="D61" sqref="D61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5212,7 +5212,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="61" spans="1:17" ht="119" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:17" ht="102" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>41</v>
       </c>
@@ -5223,7 +5223,7 @@
         <v>392</v>
       </c>
       <c r="D61" s="1">
-        <v>2021</v>
+        <v>2023</v>
       </c>
       <c r="E61" s="1" t="s">
         <v>393</v>

</xml_diff>

<commit_message>
file reorganization. start quality control of mesi by manually compiling dataset
</commit_message>
<xml_diff>
--- a/lit_search_np_fert_exps.xlsx
+++ b/lit_search_np_fert_exps.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr updateLinks="always"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eaperkowski/git/p_meta/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85B66616-665D-9448-867D-24A2E6C4A62F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F554999-8629-7A4B-AADE-CADF78CDF06E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9420" yWindow="16060" windowWidth="49540" windowHeight="28300" xr2:uid="{50492CE8-F5C0-524A-968F-FD9EC2022F6C}"/>
+    <workbookView xWindow="1680" yWindow="500" windowWidth="49520" windowHeight="28300" xr2:uid="{50492CE8-F5C0-524A-968F-FD9EC2022F6C}"/>
   </bookViews>
   <sheets>
     <sheet name="all_papers" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">p_fert_papers!$A$1:$Q$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1517,7 +1518,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1576,23 +1577,14 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1600,17 +1592,41 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2284,10 +2300,10 @@
   <dimension ref="A1:S61"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B56" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B54" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D61" sqref="D61"/>
+      <selection pane="bottomRight" activeCell="K50" sqref="K50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3509,7 +3525,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="26" spans="1:17" s="27" customFormat="1" ht="119" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:17" s="24" customFormat="1" ht="119" x14ac:dyDescent="0.2">
       <c r="A26" s="17" t="s">
         <v>41</v>
       </c>
@@ -4181,7 +4197,7 @@
       <c r="P39" s="1"/>
       <c r="Q39" s="1"/>
     </row>
-    <row r="40" spans="1:17" s="27" customFormat="1" ht="136" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:17" s="24" customFormat="1" ht="136" x14ac:dyDescent="0.2">
       <c r="A40" s="17" t="s">
         <v>41</v>
       </c>
@@ -4685,16 +4701,16 @@
       <c r="G50" s="18" t="s">
         <v>308</v>
       </c>
-      <c r="H50" s="20" t="s">
+      <c r="H50" s="36" t="s">
         <v>370</v>
       </c>
-      <c r="I50" s="20" t="s">
+      <c r="I50" s="36" t="s">
         <v>25</v>
       </c>
       <c r="J50" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="K50" s="20" t="s">
+      <c r="K50" s="36" t="s">
         <v>371</v>
       </c>
       <c r="L50" s="9" t="s">
@@ -4782,7 +4798,7 @@
       <c r="F52" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="G52" s="24" t="s">
+      <c r="G52" s="22" t="s">
         <v>318</v>
       </c>
       <c r="H52" s="1" t="s">
@@ -4833,7 +4849,7 @@
       <c r="F53" s="1" t="s">
         <v>305</v>
       </c>
-      <c r="G53" s="24" t="s">
+      <c r="G53" s="22" t="s">
         <v>324</v>
       </c>
       <c r="H53" s="1" t="s">
@@ -4886,7 +4902,7 @@
       <c r="F54" s="1" t="s">
         <v>333</v>
       </c>
-      <c r="G54" s="24" t="s">
+      <c r="G54" s="22" t="s">
         <v>334</v>
       </c>
       <c r="H54" s="1" t="s">
@@ -4907,7 +4923,7 @@
       <c r="M54" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="N54" s="25" t="s">
+      <c r="N54" s="35" t="s">
         <v>337</v>
       </c>
       <c r="O54" s="1" t="s">
@@ -4921,53 +4937,53 @@
       </c>
     </row>
     <row r="55" spans="1:17" s="14" customFormat="1" ht="113.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="21" t="s">
+      <c r="A55" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="B55" s="21" t="s">
+      <c r="B55" s="20" t="s">
         <v>309</v>
       </c>
-      <c r="C55" s="21" t="s">
+      <c r="C55" s="20" t="s">
         <v>340</v>
       </c>
-      <c r="D55" s="21">
+      <c r="D55" s="20">
         <v>2023</v>
       </c>
-      <c r="E55" s="21" t="s">
+      <c r="E55" s="20" t="s">
         <v>341</v>
       </c>
-      <c r="F55" s="21" t="s">
+      <c r="F55" s="20" t="s">
         <v>342</v>
       </c>
-      <c r="G55" s="22" t="s">
+      <c r="G55" s="21" t="s">
         <v>343</v>
       </c>
-      <c r="H55" s="23" t="s">
+      <c r="H55" s="34" t="s">
         <v>344</v>
       </c>
-      <c r="I55" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="J55" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="K55" s="21"/>
-      <c r="L55" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="M55" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="N55" s="21" t="s">
+      <c r="I55" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="J55" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="K55" s="20"/>
+      <c r="L55" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="M55" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="N55" s="20" t="s">
         <v>345</v>
       </c>
-      <c r="O55" s="21" t="s">
+      <c r="O55" s="20" t="s">
         <v>328</v>
       </c>
-      <c r="P55" s="21" t="s">
+      <c r="P55" s="20" t="s">
         <v>346</v>
       </c>
-      <c r="Q55" s="21" t="s">
+      <c r="Q55" s="20" t="s">
         <v>347</v>
       </c>
     </row>
@@ -4990,7 +5006,7 @@
       <c r="F56" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="G56" s="24" t="s">
+      <c r="G56" s="22" t="s">
         <v>351</v>
       </c>
       <c r="H56" s="1" t="s">
@@ -5043,7 +5059,7 @@
       <c r="F57" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="G57" s="26" t="s">
+      <c r="G57" s="23" t="s">
         <v>360</v>
       </c>
       <c r="H57" s="17" t="s">
@@ -5081,48 +5097,48 @@
       <c r="A58" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="B58" s="9" t="s">
+      <c r="B58" s="27" t="s">
         <v>357</v>
       </c>
-      <c r="C58" s="9" t="s">
+      <c r="C58" s="27" t="s">
         <v>373</v>
       </c>
-      <c r="D58" s="9">
+      <c r="D58" s="27">
         <v>2019</v>
       </c>
       <c r="E58" s="28" t="s">
         <v>375</v>
       </c>
-      <c r="F58" s="9" t="s">
+      <c r="F58" s="27" t="s">
         <v>374</v>
       </c>
       <c r="G58" s="29" t="s">
         <v>376</v>
       </c>
-      <c r="H58" s="9" t="s">
+      <c r="H58" s="27" t="s">
         <v>377</v>
       </c>
-      <c r="I58" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="J58" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="K58" s="9"/>
-      <c r="L58" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="M58" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="N58" s="9"/>
-      <c r="O58" s="9" t="s">
+      <c r="I58" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="J58" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="K58" s="27"/>
+      <c r="L58" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="M58" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="N58" s="27"/>
+      <c r="O58" s="27" t="s">
         <v>328</v>
       </c>
-      <c r="P58" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q58" s="9"/>
+      <c r="P58" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q58" s="27"/>
     </row>
     <row r="59" spans="1:17" ht="102" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
@@ -5143,7 +5159,7 @@
       <c r="F59" s="30" t="s">
         <v>380</v>
       </c>
-      <c r="G59" s="31" t="s">
+      <c r="G59" s="30" t="s">
         <v>381</v>
       </c>
       <c r="H59" s="30" t="s">
@@ -5158,6 +5174,9 @@
       <c r="K59" s="30" t="s">
         <v>383</v>
       </c>
+      <c r="L59" s="31"/>
+      <c r="M59" s="31"/>
+      <c r="N59" s="31"/>
       <c r="O59" s="30" t="s">
         <v>328</v>
       </c>
@@ -5187,7 +5206,7 @@
       <c r="F60" s="30" t="s">
         <v>179</v>
       </c>
-      <c r="G60" s="31" t="s">
+      <c r="G60" s="30" t="s">
         <v>387</v>
       </c>
       <c r="H60" s="30" t="s">
@@ -5202,6 +5221,9 @@
       <c r="K60" s="30" t="s">
         <v>389</v>
       </c>
+      <c r="L60" s="31"/>
+      <c r="M60" s="31"/>
+      <c r="N60" s="31"/>
       <c r="O60" s="30" t="s">
         <v>328</v>
       </c>
@@ -5216,40 +5238,40 @@
       <c r="A61" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B61" s="1" t="s">
+      <c r="B61" s="32" t="s">
         <v>357</v>
       </c>
-      <c r="C61" s="1" t="s">
+      <c r="C61" s="32" t="s">
         <v>392</v>
       </c>
-      <c r="D61" s="1">
+      <c r="D61" s="32">
         <v>2023</v>
       </c>
-      <c r="E61" s="1" t="s">
+      <c r="E61" s="32" t="s">
         <v>393</v>
       </c>
-      <c r="F61" s="1" t="s">
+      <c r="F61" s="32" t="s">
         <v>394</v>
       </c>
-      <c r="G61" t="s">
+      <c r="G61" s="33" t="s">
         <v>395</v>
       </c>
-      <c r="H61" s="1"/>
-      <c r="I61" s="1"/>
-      <c r="J61" s="1"/>
-      <c r="K61" s="1" t="s">
+      <c r="H61" s="32"/>
+      <c r="I61" s="32"/>
+      <c r="J61" s="32"/>
+      <c r="K61" s="32" t="s">
         <v>396</v>
       </c>
-      <c r="L61" s="1"/>
-      <c r="M61" s="1"/>
-      <c r="N61" s="1"/>
-      <c r="O61" s="1" t="s">
+      <c r="L61" s="32"/>
+      <c r="M61" s="32"/>
+      <c r="N61" s="32"/>
+      <c r="O61" s="32" t="s">
         <v>328</v>
       </c>
-      <c r="P61" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q61" s="1"/>
+      <c r="P61" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q61" s="32"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:Q49 A50:G50 J50 L50:Q50 A51:Q53 A54:M54 O54:Q54 F55:G55 I55:Q55 A55:D56 F56:Q56 A57:Q57 A58:D58 F58 H58:Q58 A59:A60 A61:F61 H61:Q61 A62:Q1048576">
@@ -5434,32 +5456,14 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="85" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="e" cm="1" vm="1">
         <f t="array" aca="1" ref="A2" ca="1">_xlfn._xlws.FILTER(all_papers!A:Q, all_papers!A:A = "P fertilization experiment that measures photosynthetic traits")</f>
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="68" x14ac:dyDescent="0.2"/>
-    <row r="4" spans="1:17" ht="68" x14ac:dyDescent="0.2"/>
-    <row r="5" spans="1:17" ht="136" x14ac:dyDescent="0.2"/>
-    <row r="6" spans="1:17" ht="68" x14ac:dyDescent="0.2"/>
-    <row r="7" spans="1:17" ht="68" x14ac:dyDescent="0.2"/>
     <row r="8" spans="1:17" ht="72.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="9" spans="1:17" ht="68" x14ac:dyDescent="0.2"/>
-    <row r="10" spans="1:17" ht="68" x14ac:dyDescent="0.2"/>
-    <row r="11" spans="1:17" ht="51" x14ac:dyDescent="0.2"/>
-    <row r="12" spans="1:17" ht="51" x14ac:dyDescent="0.2"/>
-    <row r="13" spans="1:17" ht="119" x14ac:dyDescent="0.2"/>
-    <row r="14" spans="1:17" ht="51" x14ac:dyDescent="0.2"/>
-    <row r="15" spans="1:17" ht="68" x14ac:dyDescent="0.2"/>
-    <row r="16" spans="1:17" ht="68" x14ac:dyDescent="0.2"/>
-    <row r="17" spans="1:17" ht="68" x14ac:dyDescent="0.2"/>
-    <row r="18" spans="1:17" ht="51" x14ac:dyDescent="0.2"/>
-    <row r="19" spans="1:17" ht="34" x14ac:dyDescent="0.2"/>
-    <row r="20" spans="1:17" ht="34" x14ac:dyDescent="0.2"/>
-    <row r="21" spans="1:17" ht="85" x14ac:dyDescent="0.2"/>
-    <row r="22" spans="1:17" ht="102" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -5594,86 +5598,86 @@
       <c r="Q33" s="1"/>
     </row>
     <row r="34" spans="1:17" ht="51" x14ac:dyDescent="0.2">
-      <c r="A34" s="30"/>
-      <c r="B34" s="30" t="s">
+      <c r="A34" s="25"/>
+      <c r="B34" s="25" t="s">
         <v>357</v>
       </c>
-      <c r="C34" s="30" t="s">
+      <c r="C34" s="25" t="s">
         <v>378</v>
       </c>
-      <c r="D34" s="30">
+      <c r="D34" s="25">
         <v>2019</v>
       </c>
-      <c r="E34" s="30" t="s">
+      <c r="E34" s="25" t="s">
         <v>379</v>
       </c>
-      <c r="F34" s="30" t="s">
+      <c r="F34" s="25" t="s">
         <v>380</v>
       </c>
-      <c r="G34" s="31" t="s">
+      <c r="G34" s="26" t="s">
         <v>381</v>
       </c>
-      <c r="H34" s="30" t="s">
+      <c r="H34" s="25" t="s">
         <v>382</v>
       </c>
-      <c r="I34" s="30" t="s">
-        <v>33</v>
-      </c>
-      <c r="J34" s="30" t="s">
-        <v>33</v>
-      </c>
-      <c r="K34" s="30" t="s">
+      <c r="I34" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="J34" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="K34" s="25" t="s">
         <v>383</v>
       </c>
-      <c r="O34" s="30" t="s">
+      <c r="O34" s="25" t="s">
         <v>328</v>
       </c>
-      <c r="P34" s="30" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q34" s="30" t="s">
+      <c r="P34" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q34" s="25" t="s">
         <v>384</v>
       </c>
     </row>
     <row r="35" spans="1:17" ht="136" x14ac:dyDescent="0.2">
-      <c r="A35" s="30"/>
-      <c r="B35" s="30" t="s">
+      <c r="A35" s="25"/>
+      <c r="B35" s="25" t="s">
         <v>357</v>
       </c>
-      <c r="C35" s="30" t="s">
+      <c r="C35" s="25" t="s">
         <v>385</v>
       </c>
-      <c r="D35" s="30">
+      <c r="D35" s="25">
         <v>2019</v>
       </c>
-      <c r="E35" s="30" t="s">
+      <c r="E35" s="25" t="s">
         <v>386</v>
       </c>
-      <c r="F35" s="30" t="s">
+      <c r="F35" s="25" t="s">
         <v>179</v>
       </c>
-      <c r="G35" s="31" t="s">
+      <c r="G35" s="26" t="s">
         <v>387</v>
       </c>
-      <c r="H35" s="30" t="s">
+      <c r="H35" s="25" t="s">
         <v>388</v>
       </c>
-      <c r="I35" s="30" t="s">
-        <v>33</v>
-      </c>
-      <c r="J35" s="30" t="s">
-        <v>33</v>
-      </c>
-      <c r="K35" s="30" t="s">
+      <c r="I35" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="J35" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="K35" s="25" t="s">
         <v>389</v>
       </c>
-      <c r="O35" s="30" t="s">
+      <c r="O35" s="25" t="s">
         <v>328</v>
       </c>
-      <c r="P35" s="30" t="s">
+      <c r="P35" s="25" t="s">
         <v>390</v>
       </c>
-      <c r="Q35" s="30" t="s">
+      <c r="Q35" s="25" t="s">
         <v>391</v>
       </c>
     </row>

</xml_diff>